<commit_message>
post order using 1 stack
</commit_message>
<xml_diff>
--- a/Applications/QuestionListWithApproaches.xlsx
+++ b/Applications/QuestionListWithApproaches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksharkashyap/Documents/VisualStudio/Applications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70AC16B-B002-AC4A-9347-BDEA3380CCA1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388D9737-1633-8741-8085-5F7B6498F3DD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="460" windowWidth="32600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5994,7 +5994,7 @@
 if(state == 3) addtoPostorderList(top) &amp; pop(top)</t>
   </si>
   <si>
-    <t>[using 1 stack (V.IMP)] refer gfg</t>
+    <t>[using 1 stack (V.IMP)]  [Push directly root node two times while traversing to the left. While poping if you find stack top() is same as root then go for root-&gt;right else print root.]</t>
   </si>
 </sst>
 </file>
@@ -6282,7 +6282,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
@@ -6455,9 +6455,6 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6750,8 +6747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" zoomScale="163" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B295" sqref="B295"/>
+    <sheetView tabSelected="1" topLeftCell="A284" zoomScale="163" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C292" sqref="C292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -11830,7 +11827,7 @@
       <c r="B292" s="64" t="s">
         <v>1097</v>
       </c>
-      <c r="C292" s="67" t="s">
+      <c r="C292" s="68" t="s">
         <v>1105</v>
       </c>
       <c r="D292" s="50"/>
@@ -11842,13 +11839,13 @@
       <c r="H292" s="50"/>
     </row>
     <row r="293" spans="1:8" s="59" customFormat="1" ht="74" customHeight="1">
-      <c r="A293" s="68" t="s">
+      <c r="A293" s="67" t="s">
         <v>1101</v>
       </c>
       <c r="B293" s="18" t="s">
         <v>1103</v>
       </c>
-      <c r="C293" s="69" t="s">
+      <c r="C293" s="68" t="s">
         <v>1104</v>
       </c>
       <c r="D293" s="50"/>

</xml_diff>

<commit_message>
make strings of x and y equals
</commit_message>
<xml_diff>
--- a/Applications/QuestionListWithApproaches.xlsx
+++ b/Applications/QuestionListWithApproaches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksharkashyap/Documents/VisualStudio/Applications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E99D76B-17E0-5642-8DC0-F7224342410B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0724F3E0-3EDE-EF47-B101-1F985AD0CDA0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="460" windowWidth="32600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="1152">
   <si>
     <t>Convert Binary Number in a Linked List to Integer</t>
   </si>
@@ -2226,12 +2226,6 @@
     <t>https://leetcode.com/problems/relative-sort-array/</t>
   </si>
   <si>
-    <t>minimum swaps to make strings equal</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/minimum-swaps-to-make-strings-equal/</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/maximum-69-number/</t>
   </si>
   <si>
@@ -4558,27 +4552,6 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve"> [Given a non-negative integer num, return the number of steps to reduce it to zero. If the current number is even, you have to divide it by 2, otherwise, you have to subtract 1 from it.]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>lucky number in a matrix</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> [m * n matrix of distinct numbers, return all lucky numbers in the matrix in any order.
-A lucky number is an element of the matrix such that it is the minimum element in its row and maximum in its column.]</t>
     </r>
   </si>
   <si>
@@ -6327,12 +6300,153 @@
   <si>
     <t>basically in this question we try to discard column(while calculating its values) for the next iteration</t>
   </si>
+  <si>
+    <t>graph is bipartite if it is 2 colorable</t>
+  </si>
+  <si>
+    <t>BFS (optimal approach)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>lucky number in a matrix</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> [m * n matrix of distinct numbers, return all lucky numbers in the matrix in any order. A lucky number is an element of the matrix such that it is the minimum element in its row and maximum in its column.]</t>
+    </r>
+  </si>
+  <si>
+    <t>[see my solution on leetcode]</t>
+  </si>
+  <si>
+    <t>[O(1) solution] leetcode.com/problems/lucky-numbers-in-a-matrix/discuss/539914/min-max-and-max-min-omn-time-o1-space</t>
+  </si>
+  <si>
+    <t>Brute force time complexity O(m*n(m+n))</t>
+  </si>
+  <si>
+    <t>create two arrays that hold MIN(rows) [0-&gt; min of 0th row, 1-&gt; min of 1th row….) of size M and MAX(colmns) of size N, 
+now loop through the matrix and add those elements to answer which 
+satisfy MIN_ROW[r] == MAX_COL[c] [time O(m*n), space O(max(m,n))]</t>
+  </si>
+  <si>
+    <t>create 256(because of ascii) array of objects to store pair(char,frequency), sort the array on the frequency by using comparator, then create a new string out of it [O(n) time and O(1) space because sorting 256 objects doesn’t depend on length of the string so time wont be nlogn]</t>
+  </si>
+  <si>
+    <t>countMap the frequency of arr1 
+traverse arr2 to get count(arr2[i])
+fill the value in answerArr while count&gt;0 
+extra loop to place the values at the last which are not in arr2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">map the elements of arr2 to its indices (to get who should come first in O(1)), now traverse the arr1 and map the elements which are not present in the map  with arr2.length+(0,1...) then apply any sorting algorithm or comparator class [ O(nlogn) time and O(n) space for hashtable] </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>instead of sorting you can use treemap</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>minimum swaps to make strings equal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> [You are given two strings of equal length consisting of letters </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>"x" and "y" only</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Make these two strings equal to each other. You can </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>swap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> any two characters that belong to different strings]</t>
+    </r>
+  </si>
+  <si>
+    <t>notice the examples 1,2 and 3 are base cases , you have to find these 3 base cases in order to reach to the solution in an interview</t>
+  </si>
+  <si>
+    <t>(1) xx &amp;&amp; yy -&gt; 1 swaps (2) xy &amp;&amp; yx -&gt; 2 swaps  (3) xx &amp;&amp; xy -&gt; -1
+note that if at i'th position both letters are same then donot process it because they are at correct position</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-swaps-to-make-strings-equal/discuss/741006/JAVA-O(N)-solution-beats-100-greedy-algorithm</t>
+  </si>
+  <si>
+    <t>1) if both are equal dont process it
+2) calculate the frequency of (x1 (x in s1) ,x2 (x in s2) )
+If frequency(x1+x2) is ODD return -1 as we cant make them equal
+else return (x1/2 + x2%2) + (x1/2 + x2%2)</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/find-common-elements-three-sorted-arrays/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37">
+  <fonts count="38">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6568,6 +6682,13 @@
       <u/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="3"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -7104,8 +7225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E226" zoomScale="158" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G231" sqref="G231"/>
+    <sheetView tabSelected="1" topLeftCell="A256" zoomScale="160" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A259" sqref="A259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7190,13 +7311,13 @@
     </row>
     <row r="4" spans="1:8" ht="38" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -7243,7 +7364,7 @@
         <v>60</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
@@ -7272,7 +7393,7 @@
     </row>
     <row r="8" spans="1:8" ht="23" customHeight="1">
       <c r="A8" s="23" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>40</v>
@@ -7286,13 +7407,13 @@
     </row>
     <row r="9" spans="1:8" ht="58" customHeight="1">
       <c r="A9" s="47" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -7342,7 +7463,7 @@
         <v>41</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
@@ -7355,7 +7476,7 @@
         <v>42</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -7375,10 +7496,10 @@
         <v>45</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>48</v>
@@ -7424,10 +7545,10 @@
     </row>
     <row r="17" spans="1:8" ht="29" customHeight="1">
       <c r="A17" s="14" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>
@@ -7456,13 +7577,13 @@
     </row>
     <row r="19" spans="1:8" ht="46" customHeight="1">
       <c r="A19" s="13" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="B19" s="61" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>1069</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>1072</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -7472,13 +7593,13 @@
     </row>
     <row r="20" spans="1:8" ht="43" customHeight="1">
       <c r="A20" s="14" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -7488,13 +7609,13 @@
     </row>
     <row r="21" spans="1:8" ht="63" customHeight="1">
       <c r="A21" s="14" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="B21" s="61" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="C21" s="62" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -7504,7 +7625,7 @@
     </row>
     <row r="22" spans="1:8" ht="24" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="5"/>
@@ -7516,7 +7637,7 @@
     </row>
     <row r="23" spans="1:8" ht="32" customHeight="1">
       <c r="A23" s="14" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="5"/>
@@ -7528,7 +7649,7 @@
     </row>
     <row r="24" spans="1:8" ht="33" customHeight="1">
       <c r="A24" s="14" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="5"/>
@@ -7540,7 +7661,7 @@
     </row>
     <row r="25" spans="1:8" ht="33" customHeight="1">
       <c r="A25" s="14" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="5"/>
@@ -7552,7 +7673,7 @@
     </row>
     <row r="26" spans="1:8" ht="33" customHeight="1">
       <c r="A26" s="14" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="5"/>
@@ -7564,7 +7685,7 @@
     </row>
     <row r="27" spans="1:8" ht="29" customHeight="1">
       <c r="A27" s="14" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
@@ -7621,7 +7742,7 @@
         <v>61</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>62</v>
@@ -7718,10 +7839,10 @@
     </row>
     <row r="37" spans="1:8" ht="58" customHeight="1">
       <c r="A37" s="13" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C37" s="19" t="s">
         <v>81</v>
@@ -7768,7 +7889,7 @@
     </row>
     <row r="40" spans="1:8" s="4" customFormat="1" ht="55" customHeight="1">
       <c r="A40" s="13" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>88</v>
@@ -7786,7 +7907,7 @@
     </row>
     <row r="41" spans="1:8" ht="25" customHeight="1">
       <c r="A41" s="13" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="B41" s="18" t="s">
         <v>91</v>
@@ -7871,10 +7992,10 @@
         <v>107</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F45" s="19"/>
       <c r="G45" s="20" t="s">
@@ -7918,7 +8039,7 @@
     </row>
     <row r="48" spans="1:8" ht="56">
       <c r="A48" s="13" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B48" s="18" t="s">
         <v>114</v>
@@ -7936,13 +8057,13 @@
     </row>
     <row r="49" spans="1:8" ht="86" customHeight="1">
       <c r="A49" s="13" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B49" s="18" t="s">
         <v>116</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="19"/>
@@ -7974,7 +8095,7 @@
     </row>
     <row r="51" spans="1:8" ht="50" customHeight="1">
       <c r="A51" s="23" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B51" s="18" t="s">
         <v>123</v>
@@ -7992,7 +8113,7 @@
     </row>
     <row r="52" spans="1:8" ht="46" customHeight="1">
       <c r="A52" s="13" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B52" s="18" t="s">
         <v>127</v>
@@ -8014,7 +8135,7 @@
     </row>
     <row r="53" spans="1:8" ht="42">
       <c r="A53" s="13" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>132</v>
@@ -8052,7 +8173,7 @@
     </row>
     <row r="55" spans="1:8" ht="60" customHeight="1">
       <c r="A55" s="13" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>138</v>
@@ -8084,7 +8205,7 @@
     </row>
     <row r="57" spans="1:8" ht="29" customHeight="1">
       <c r="A57" s="13" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>144</v>
@@ -8104,7 +8225,7 @@
     </row>
     <row r="58" spans="1:8" s="3" customFormat="1" ht="39" customHeight="1">
       <c r="A58" s="13" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B58" s="18" t="s">
         <v>19</v>
@@ -8124,13 +8245,13 @@
     </row>
     <row r="59" spans="1:8" ht="71" customHeight="1">
       <c r="A59" s="13" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D59" s="19"/>
       <c r="E59" s="19"/>
@@ -8142,10 +8263,10 @@
     </row>
     <row r="60" spans="1:8" ht="38" customHeight="1">
       <c r="A60" s="13" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="C60" s="19" t="s">
         <v>152</v>
@@ -8178,7 +8299,7 @@
     </row>
     <row r="62" spans="1:8" s="3" customFormat="1" ht="69" customHeight="1">
       <c r="A62" s="13" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B62" s="18" t="s">
         <v>158</v>
@@ -8198,7 +8319,7 @@
     </row>
     <row r="63" spans="1:8" ht="53" customHeight="1">
       <c r="A63" s="13" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B63" s="28" t="s">
         <v>161</v>
@@ -8256,7 +8377,7 @@
     </row>
     <row r="66" spans="1:8" ht="75" customHeight="1">
       <c r="A66" s="13" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="B66" s="18" t="s">
         <v>173</v>
@@ -8292,7 +8413,7 @@
     </row>
     <row r="68" spans="1:8" ht="41" customHeight="1">
       <c r="A68" s="13" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B68" s="18" t="s">
         <v>180</v>
@@ -8370,7 +8491,7 @@
     </row>
     <row r="72" spans="1:8" ht="48" customHeight="1">
       <c r="A72" s="13" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="B72" s="18" t="s">
         <v>197</v>
@@ -8414,7 +8535,7 @@
     </row>
     <row r="74" spans="1:8" ht="38" customHeight="1">
       <c r="A74" s="13" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="B74" s="18" t="s">
         <v>208</v>
@@ -8432,7 +8553,7 @@
     </row>
     <row r="75" spans="1:8" ht="46" customHeight="1">
       <c r="A75" s="13" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="B75" s="18" t="s">
         <v>212</v>
@@ -8450,7 +8571,7 @@
     </row>
     <row r="76" spans="1:8" ht="28" customHeight="1">
       <c r="A76" s="13" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B76" s="18" t="s">
         <v>214</v>
@@ -8492,7 +8613,7 @@
     </row>
     <row r="78" spans="1:8" s="3" customFormat="1" ht="62" customHeight="1">
       <c r="A78" s="13" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="B78" s="18" t="s">
         <v>229</v>
@@ -8520,7 +8641,7 @@
         <v>230</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D79" s="19" t="s">
         <v>231</v>
@@ -8576,10 +8697,10 @@
         <v>241</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="D82" s="19" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="E82" s="19" t="s">
         <v>243</v>
@@ -8598,7 +8719,7 @@
         <v>247</v>
       </c>
       <c r="C83" s="19" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="D83" s="19" t="s">
         <v>245</v>
@@ -8671,7 +8792,7 @@
         <v>260</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="C87" s="19" t="s">
         <v>261</v>
@@ -8706,7 +8827,7 @@
     </row>
     <row r="89" spans="1:8" ht="36" customHeight="1">
       <c r="A89" s="13" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="B89" s="18" t="s">
         <v>267</v>
@@ -8838,7 +8959,7 @@
     </row>
     <row r="96" spans="1:8" s="3" customFormat="1" ht="70">
       <c r="A96" s="13" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B96" s="18" t="s">
         <v>296</v>
@@ -8880,7 +9001,7 @@
         <v>305</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="D98" s="19" t="s">
         <v>306</v>
@@ -8903,7 +9024,7 @@
         <v>310</v>
       </c>
       <c r="D99" s="28" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="E99" s="19" t="s">
         <v>311</v>
@@ -8916,7 +9037,7 @@
     </row>
     <row r="100" spans="1:8" ht="57" customHeight="1">
       <c r="A100" s="13" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B100" s="18" t="s">
         <v>313</v>
@@ -8934,7 +9055,7 @@
     </row>
     <row r="101" spans="1:8" ht="60" customHeight="1">
       <c r="A101" s="13" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B101" s="18" t="s">
         <v>316</v>
@@ -8992,7 +9113,7 @@
     </row>
     <row r="104" spans="1:8" ht="53" customHeight="1">
       <c r="A104" s="13" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B104" s="18" t="s">
         <v>328</v>
@@ -9012,7 +9133,7 @@
     </row>
     <row r="105" spans="1:8" ht="38" customHeight="1">
       <c r="A105" s="13" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B105" s="18" t="s">
         <v>332</v>
@@ -9032,7 +9153,7 @@
     </row>
     <row r="106" spans="1:8" ht="70">
       <c r="A106" s="13" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B106" s="18" t="s">
         <v>338</v>
@@ -9104,7 +9225,7 @@
     </row>
     <row r="110" spans="1:8" ht="28">
       <c r="A110" s="13" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B110" s="18" t="s">
         <v>350</v>
@@ -9158,7 +9279,7 @@
     </row>
     <row r="113" spans="1:13" ht="70">
       <c r="A113" s="13" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B113" s="18" t="s">
         <v>362</v>
@@ -9176,7 +9297,7 @@
     </row>
     <row r="114" spans="1:13" ht="39" customHeight="1">
       <c r="A114" s="13" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B114" s="18" t="s">
         <v>364</v>
@@ -9192,7 +9313,7 @@
     </row>
     <row r="115" spans="1:13" ht="65" customHeight="1">
       <c r="A115" s="13" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B115" s="18" t="s">
         <v>366</v>
@@ -9208,10 +9329,10 @@
     </row>
     <row r="116" spans="1:13" ht="37" customHeight="1">
       <c r="A116" s="13" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B116" s="18" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="C116" s="19" t="s">
         <v>368</v>
@@ -9228,7 +9349,7 @@
     </row>
     <row r="117" spans="1:13" ht="30" customHeight="1">
       <c r="A117" s="13" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B117" s="18" t="s">
         <v>372</v>
@@ -9244,7 +9365,7 @@
     </row>
     <row r="118" spans="1:13" ht="54" customHeight="1">
       <c r="A118" s="13" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B118" s="18" t="s">
         <v>373</v>
@@ -9260,7 +9381,7 @@
     </row>
     <row r="119" spans="1:13" ht="51" customHeight="1">
       <c r="A119" s="13" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="B119" s="18" t="s">
         <v>376</v>
@@ -9276,7 +9397,7 @@
     </row>
     <row r="120" spans="1:13" s="3" customFormat="1" ht="66" customHeight="1">
       <c r="A120" s="13" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B120" s="18" t="s">
         <v>377</v>
@@ -9296,7 +9417,7 @@
     </row>
     <row r="121" spans="1:13" s="3" customFormat="1" ht="80" customHeight="1">
       <c r="A121" s="13" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B121" s="18" t="s">
         <v>381</v>
@@ -9370,7 +9491,7 @@
     </row>
     <row r="125" spans="1:13" ht="84">
       <c r="A125" s="13" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B125" s="18" t="s">
         <v>396</v>
@@ -9390,13 +9511,13 @@
     </row>
     <row r="126" spans="1:13" ht="69" customHeight="1">
       <c r="A126" s="13" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B126" s="18" t="s">
         <v>19</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="D126" s="28"/>
       <c r="E126" s="19"/>
@@ -9430,13 +9551,13 @@
     </row>
     <row r="128" spans="1:13" ht="83" customHeight="1">
       <c r="A128" s="13" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="B128" s="18" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="D128" s="19" t="s">
         <v>407</v>
@@ -9455,7 +9576,7 @@
     </row>
     <row r="129" spans="1:19" ht="98">
       <c r="A129" s="50" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="B129" s="18" t="s">
         <v>408</v>
@@ -9480,7 +9601,7 @@
     </row>
     <row r="130" spans="1:19" s="3" customFormat="1" ht="62" customHeight="1">
       <c r="A130" s="13" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B130" s="18" t="s">
         <v>413</v>
@@ -9498,7 +9619,7 @@
     </row>
     <row r="131" spans="1:19" s="3" customFormat="1" ht="84">
       <c r="A131" s="13" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B131" s="18" t="s">
         <v>417</v>
@@ -9514,7 +9635,7 @@
     </row>
     <row r="132" spans="1:19" ht="49" customHeight="1">
       <c r="A132" s="13" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B132" s="18" t="s">
         <v>418</v>
@@ -9579,7 +9700,7 @@
     </row>
     <row r="135" spans="1:19" ht="51" customHeight="1">
       <c r="A135" s="13" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="B135" s="18" t="s">
         <v>434</v>
@@ -9597,7 +9718,7 @@
     </row>
     <row r="136" spans="1:19" ht="70">
       <c r="A136" s="13" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B136" s="18" t="s">
         <v>438</v>
@@ -9615,7 +9736,7 @@
     </row>
     <row r="137" spans="1:19" ht="59" customHeight="1">
       <c r="A137" s="13" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="B137" s="18" t="s">
         <v>442</v>
@@ -9624,7 +9745,7 @@
         <v>441</v>
       </c>
       <c r="D137" s="31" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="E137" s="19"/>
       <c r="F137" s="19"/>
@@ -9635,7 +9756,7 @@
     </row>
     <row r="138" spans="1:19" ht="47" customHeight="1">
       <c r="A138" s="13" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B138" s="18" t="s">
         <v>444</v>
@@ -9667,7 +9788,7 @@
     </row>
     <row r="140" spans="1:19" ht="66" customHeight="1">
       <c r="A140" s="13" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B140" s="18" t="s">
         <v>450</v>
@@ -9703,10 +9824,10 @@
     </row>
     <row r="142" spans="1:19" ht="40" customHeight="1">
       <c r="A142" s="13" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="B142" s="18" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="C142" s="19"/>
       <c r="D142" s="19"/>
@@ -9719,10 +9840,10 @@
     </row>
     <row r="143" spans="1:19" ht="55" customHeight="1">
       <c r="A143" s="13" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="B143" s="18" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="C143" s="19" t="s">
         <v>456</v>
@@ -9730,7 +9851,7 @@
       <c r="D143" s="19"/>
       <c r="E143" s="19"/>
       <c r="F143" s="19" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="G143" s="19" t="s">
         <v>455</v>
@@ -9742,7 +9863,7 @@
         <v>457</v>
       </c>
       <c r="B144" s="18" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="C144" s="28" t="s">
         <v>459</v>
@@ -9817,7 +9938,7 @@
     </row>
     <row r="148" spans="1:8" ht="64" customHeight="1">
       <c r="A148" s="13" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B148" s="18" t="s">
         <v>475</v>
@@ -9853,7 +9974,7 @@
     </row>
     <row r="150" spans="1:8" ht="71" customHeight="1">
       <c r="A150" s="13" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B150" s="18" t="s">
         <v>482</v>
@@ -9907,7 +10028,7 @@
     </row>
     <row r="153" spans="1:8" ht="43" customHeight="1">
       <c r="A153" s="13" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="B153" s="18" t="s">
         <v>492</v>
@@ -9925,7 +10046,7 @@
     </row>
     <row r="154" spans="1:8" ht="79" customHeight="1">
       <c r="A154" s="13" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B154" s="18" t="s">
         <v>495</v>
@@ -9957,13 +10078,13 @@
     </row>
     <row r="156" spans="1:8" ht="45" customHeight="1">
       <c r="A156" s="13" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B156" s="28" t="s">
         <v>500</v>
       </c>
       <c r="C156" s="19" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="D156" s="19"/>
       <c r="E156" s="19"/>
@@ -10009,10 +10130,10 @@
     </row>
     <row r="159" spans="1:8" ht="54" customHeight="1">
       <c r="A159" s="13" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="B159" s="18" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C159" s="19"/>
       <c r="D159" s="19"/>
@@ -10043,7 +10164,7 @@
     </row>
     <row r="161" spans="1:8" ht="43" customHeight="1">
       <c r="A161" s="13" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="B161" s="18" t="s">
         <v>514</v>
@@ -10069,7 +10190,7 @@
     </row>
     <row r="162" spans="1:8" ht="60" customHeight="1">
       <c r="A162" s="13" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B162" s="18" t="s">
         <v>519</v>
@@ -10119,7 +10240,7 @@
     </row>
     <row r="165" spans="1:8" ht="51" customHeight="1">
       <c r="A165" s="13" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="B165" s="18" t="s">
         <v>526</v>
@@ -10137,7 +10258,7 @@
     </row>
     <row r="166" spans="1:8" ht="84" customHeight="1">
       <c r="A166" s="13" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B166" s="18" t="s">
         <v>529</v>
@@ -10155,7 +10276,7 @@
     </row>
     <row r="167" spans="1:8" ht="53" customHeight="1">
       <c r="A167" s="13" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="B167" s="18" t="s">
         <v>533</v>
@@ -10173,7 +10294,7 @@
     </row>
     <row r="168" spans="1:8" s="3" customFormat="1" ht="126" customHeight="1">
       <c r="A168" s="13" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="B168" s="18" t="s">
         <v>535</v>
@@ -10231,7 +10352,7 @@
     </row>
     <row r="171" spans="1:8" ht="51" customHeight="1">
       <c r="A171" s="13" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="B171" s="18" t="s">
         <v>550</v>
@@ -10253,7 +10374,7 @@
     </row>
     <row r="172" spans="1:8" ht="98">
       <c r="A172" s="13" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="B172" s="18" t="s">
         <v>553</v>
@@ -10273,7 +10394,7 @@
     </row>
     <row r="173" spans="1:8" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="A173" s="13" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B173" s="18" t="s">
         <v>610</v>
@@ -10298,7 +10419,7 @@
         <v>562</v>
       </c>
       <c r="B174" s="18" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="C174" s="19"/>
       <c r="D174" s="34"/>
@@ -10311,7 +10432,7 @@
     </row>
     <row r="175" spans="1:8" ht="51" customHeight="1">
       <c r="A175" s="13" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="B175" s="18" t="s">
         <v>563</v>
@@ -10343,7 +10464,7 @@
     </row>
     <row r="177" spans="1:8" ht="56">
       <c r="A177" s="13" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="B177" s="18" t="s">
         <v>569</v>
@@ -10355,7 +10476,7 @@
         <v>571</v>
       </c>
       <c r="E177" s="19" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="F177" s="19"/>
       <c r="G177" s="19" t="s">
@@ -10365,7 +10486,7 @@
     </row>
     <row r="178" spans="1:8" ht="35" customHeight="1">
       <c r="A178" s="33" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="B178" s="18" t="s">
         <v>572</v>
@@ -10392,7 +10513,7 @@
         <v>578</v>
       </c>
       <c r="D179" s="19" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="E179" s="19"/>
       <c r="F179" s="19"/>
@@ -10406,13 +10527,13 @@
         <v>579</v>
       </c>
       <c r="B180" s="18" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="C180" s="19" t="s">
         <v>152</v>
       </c>
       <c r="D180" s="19" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="E180" s="19"/>
       <c r="F180" s="19"/>
@@ -10423,7 +10544,7 @@
     </row>
     <row r="181" spans="1:8" ht="70">
       <c r="A181" s="13" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="B181" s="18" t="s">
         <v>508</v>
@@ -10438,18 +10559,18 @@
         <v>584</v>
       </c>
       <c r="F181" s="19" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="G181" s="52" t="s">
         <v>583</v>
       </c>
       <c r="H181" s="19" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="36" customHeight="1">
       <c r="A182" s="13" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="B182" s="18" t="s">
         <v>586</v>
@@ -10469,7 +10590,7 @@
     </row>
     <row r="183" spans="1:8" ht="33" customHeight="1">
       <c r="A183" s="13" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="B183" s="18" t="s">
         <v>124</v>
@@ -10507,7 +10628,7 @@
     </row>
     <row r="185" spans="1:8" ht="28">
       <c r="A185" s="13" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="B185" s="18" t="s">
         <v>59</v>
@@ -10527,7 +10648,7 @@
     </row>
     <row r="186" spans="1:8" ht="28">
       <c r="A186" s="13" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B186" s="18" t="s">
         <v>600</v>
@@ -10543,7 +10664,7 @@
     </row>
     <row r="187" spans="1:8" ht="70">
       <c r="A187" s="13" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="B187" s="18" t="s">
         <v>601</v>
@@ -10563,7 +10684,7 @@
     </row>
     <row r="188" spans="1:8" ht="56">
       <c r="A188" s="13" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="B188" s="18" t="s">
         <v>606</v>
@@ -10579,7 +10700,7 @@
     </row>
     <row r="189" spans="1:8" s="10" customFormat="1" ht="140">
       <c r="A189" s="13" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B189" s="18" t="s">
         <v>508</v>
@@ -10703,7 +10824,7 @@
     </row>
     <row r="196" spans="1:8" ht="144" customHeight="1">
       <c r="A196" s="13" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B196" s="35" t="s">
         <v>639</v>
@@ -10721,7 +10842,7 @@
     </row>
     <row r="197" spans="1:8" ht="70" customHeight="1">
       <c r="A197" s="13" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B197" s="18" t="s">
         <v>642</v>
@@ -10737,7 +10858,7 @@
     </row>
     <row r="198" spans="1:8" ht="65" customHeight="1">
       <c r="A198" s="13" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="B198" s="18" t="s">
         <v>645</v>
@@ -10755,16 +10876,16 @@
     </row>
     <row r="199" spans="1:8" ht="90" customHeight="1">
       <c r="A199" s="13" t="s">
+        <v>862</v>
+      </c>
+      <c r="B199" s="18" t="s">
+        <v>775</v>
+      </c>
+      <c r="C199" s="19" t="s">
+        <v>863</v>
+      </c>
+      <c r="D199" s="19" t="s">
         <v>864</v>
-      </c>
-      <c r="B199" s="18" t="s">
-        <v>777</v>
-      </c>
-      <c r="C199" s="19" t="s">
-        <v>865</v>
-      </c>
-      <c r="D199" s="19" t="s">
-        <v>866</v>
       </c>
       <c r="E199" s="36"/>
       <c r="F199" s="36"/>
@@ -10778,7 +10899,7 @@
         <v>649</v>
       </c>
       <c r="B200" s="18" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="C200" s="19" t="s">
         <v>653</v>
@@ -10793,7 +10914,7 @@
     </row>
     <row r="201" spans="1:8" ht="54" customHeight="1">
       <c r="A201" s="13" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="B201" s="18" t="s">
         <v>654</v>
@@ -10847,7 +10968,7 @@
     </row>
     <row r="204" spans="1:8" s="4" customFormat="1" ht="104" customHeight="1">
       <c r="A204" s="13" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B204" s="38" t="s">
         <v>671</v>
@@ -10856,10 +10977,10 @@
         <v>672</v>
       </c>
       <c r="D204" s="19" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="E204" s="19" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="F204" s="19"/>
       <c r="G204" s="20" t="s">
@@ -10887,7 +11008,7 @@
     </row>
     <row r="206" spans="1:8" s="4" customFormat="1" ht="55" customHeight="1">
       <c r="A206" s="13" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B206" s="18" t="s">
         <v>673</v>
@@ -10903,7 +11024,7 @@
     </row>
     <row r="207" spans="1:8" s="12" customFormat="1" ht="47" customHeight="1">
       <c r="A207" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="B207" s="18" t="s">
         <v>677</v>
@@ -10921,7 +11042,7 @@
     </row>
     <row r="208" spans="1:8" ht="63" customHeight="1">
       <c r="A208" s="13" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B208" s="18" t="s">
         <v>686</v>
@@ -10941,7 +11062,7 @@
     </row>
     <row r="209" spans="1:8" s="4" customFormat="1" ht="79" customHeight="1">
       <c r="A209" s="13" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="B209" s="18" t="s">
         <v>686</v>
@@ -10950,7 +11071,7 @@
         <v>687</v>
       </c>
       <c r="D209" s="19" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="E209" s="36"/>
       <c r="F209" s="36"/>
@@ -10961,13 +11082,13 @@
     </row>
     <row r="210" spans="1:8" ht="61" customHeight="1">
       <c r="A210" s="13" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="B210" s="18" t="s">
         <v>152</v>
       </c>
       <c r="C210" s="19" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="D210" s="19" t="s">
         <v>219</v>
@@ -10981,32 +11102,32 @@
     </row>
     <row r="211" spans="1:8" ht="61" customHeight="1">
       <c r="A211" s="13" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="B211" s="18" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="C211" s="19"/>
       <c r="D211" s="19"/>
       <c r="E211" s="19"/>
       <c r="F211" s="19"/>
       <c r="G211" s="20" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="H211" s="19"/>
     </row>
     <row r="212" spans="1:8" ht="78" customHeight="1">
       <c r="A212" s="13" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="B212" s="35" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="C212" s="19" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="D212" s="19" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="F212" s="36"/>
       <c r="G212" s="40" t="s">
@@ -11016,42 +11137,42 @@
     </row>
     <row r="213" spans="1:8" ht="76" customHeight="1">
       <c r="A213" s="13" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="B213" s="18" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="C213" s="36"/>
       <c r="D213" s="36"/>
       <c r="E213" s="36"/>
       <c r="F213" s="36"/>
       <c r="G213" s="40" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="H213" s="36"/>
     </row>
     <row r="214" spans="1:8" ht="83" customHeight="1">
       <c r="A214" s="13" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B214" s="18" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C214" s="39" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D214" s="19" t="s">
         <v>1094</v>
-      </c>
-      <c r="B214" s="18" t="s">
-        <v>1098</v>
-      </c>
-      <c r="C214" s="39" t="s">
-        <v>1099</v>
-      </c>
-      <c r="D214" s="19" t="s">
-        <v>1097</v>
       </c>
       <c r="F214" s="36"/>
       <c r="G214" s="40" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="H214" s="36"/>
     </row>
     <row r="215" spans="1:8" ht="79" customHeight="1">
       <c r="A215" s="13" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B215" s="35" t="s">
         <v>695</v>
@@ -11071,7 +11192,7 @@
     </row>
     <row r="216" spans="1:8" ht="43" customHeight="1">
       <c r="A216" s="14" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="B216" s="18" t="s">
         <v>698</v>
@@ -11087,10 +11208,10 @@
     </row>
     <row r="217" spans="1:8" ht="63" customHeight="1">
       <c r="A217" s="33" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="B217" s="18" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="C217" s="36"/>
       <c r="D217" s="36"/>
@@ -11103,34 +11224,34 @@
     </row>
     <row r="218" spans="1:8" s="4" customFormat="1" ht="104" customHeight="1">
       <c r="A218" s="32" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="B218" s="18" t="s">
         <v>690</v>
       </c>
       <c r="C218" s="67" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="D218" s="19" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E218" s="38" t="s">
         <v>1102</v>
       </c>
-      <c r="E218" s="38" t="s">
-        <v>1105</v>
-      </c>
       <c r="F218" s="62" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="G218" s="19" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="H218" s="19"/>
     </row>
     <row r="219" spans="1:8" ht="71" customHeight="1">
       <c r="A219" s="13" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B219" s="18" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="C219" s="19" t="s">
         <v>702</v>
@@ -11147,22 +11268,22 @@
     </row>
     <row r="220" spans="1:8" ht="96" customHeight="1">
       <c r="A220" s="13" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B220" s="35" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C220" s="19" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D220" s="19" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E220" s="39" t="s">
         <v>1108</v>
       </c>
-      <c r="B220" s="35" t="s">
-        <v>1109</v>
-      </c>
-      <c r="C220" s="19" t="s">
+      <c r="F220" s="19" t="s">
         <v>1110</v>
-      </c>
-      <c r="D220" s="19" t="s">
-        <v>1112</v>
-      </c>
-      <c r="E220" s="39" t="s">
-        <v>1111</v>
-      </c>
-      <c r="F220" s="19" t="s">
-        <v>1113</v>
       </c>
       <c r="G220" s="68" t="s">
         <v>706</v>
@@ -11171,16 +11292,16 @@
     </row>
     <row r="221" spans="1:8" ht="76" customHeight="1">
       <c r="A221" s="13" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B221" s="18" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="C221" s="19" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="D221" s="19" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="E221" s="19"/>
       <c r="F221" s="36"/>
@@ -11191,16 +11312,16 @@
     </row>
     <row r="222" spans="1:8" ht="79" customHeight="1">
       <c r="A222" s="13" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="B222" s="18" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C222" s="19" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D222" s="69" t="s">
         <v>1117</v>
-      </c>
-      <c r="C222" s="19" t="s">
-        <v>1119</v>
-      </c>
-      <c r="D222" s="69" t="s">
-        <v>1120</v>
       </c>
       <c r="E222" s="39"/>
       <c r="F222" s="36"/>
@@ -11211,10 +11332,10 @@
     </row>
     <row r="223" spans="1:8" ht="56" customHeight="1">
       <c r="A223" s="33" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="B223" s="18" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="C223" s="36"/>
       <c r="D223" s="36"/>
@@ -11227,10 +11348,10 @@
     </row>
     <row r="224" spans="1:8" ht="44" customHeight="1">
       <c r="A224" s="13" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B224" s="18" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="C224" s="36"/>
       <c r="D224" s="36"/>
@@ -11243,13 +11364,13 @@
     </row>
     <row r="225" spans="1:8" ht="70" customHeight="1">
       <c r="A225" s="13" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="B225" s="18" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="C225" s="19" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="D225" s="36"/>
       <c r="E225" s="36"/>
@@ -11261,157 +11382,177 @@
     </row>
     <row r="226" spans="1:8" ht="69" customHeight="1">
       <c r="A226" s="13" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="B226" s="18" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C226" s="36"/>
       <c r="D226" s="36"/>
       <c r="E226" s="36"/>
       <c r="F226" s="36"/>
       <c r="G226" s="37" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="H226" s="36"/>
     </row>
     <row r="227" spans="1:8" ht="79" customHeight="1">
       <c r="A227" s="13" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="B227" s="18" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="C227" s="36"/>
       <c r="D227" s="36"/>
       <c r="E227" s="36"/>
       <c r="F227" s="36"/>
       <c r="G227" s="68" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="H227" s="36"/>
     </row>
     <row r="228" spans="1:8" ht="46" customHeight="1">
       <c r="A228" s="14" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B228" s="18" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="C228" s="36"/>
       <c r="D228" s="36"/>
       <c r="E228" s="36"/>
       <c r="F228" s="36"/>
       <c r="G228" s="68" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="H228" s="36"/>
     </row>
     <row r="229" spans="1:8" ht="66" customHeight="1">
       <c r="A229" s="13" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="B229" s="18" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="C229" s="67" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="D229" s="19" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="E229" s="36"/>
       <c r="F229" s="19" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="G229" s="52" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="H229" s="19"/>
     </row>
     <row r="230" spans="1:8" ht="75" customHeight="1">
       <c r="A230" s="13" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B230" s="18" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C230" s="67" t="s">
         <v>1131</v>
       </c>
-      <c r="B230" s="18" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C230" s="67" t="s">
-        <v>1134</v>
-      </c>
       <c r="D230" s="19" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="E230" s="19" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F230" s="19" t="s">
         <v>1135</v>
       </c>
-      <c r="F230" s="19" t="s">
+      <c r="G230" s="68" t="s">
+        <v>732</v>
+      </c>
+      <c r="H230" s="19"/>
+    </row>
+    <row r="231" spans="1:8" ht="68" customHeight="1">
+      <c r="A231" s="13" t="s">
         <v>1138</v>
       </c>
-      <c r="G230" s="68" t="s">
-        <v>734</v>
-      </c>
-      <c r="H230" s="19"/>
-    </row>
-    <row r="231" spans="1:8" ht="74" customHeight="1">
-      <c r="A231" s="13" t="s">
-        <v>895</v>
-      </c>
-      <c r="B231" s="41"/>
-      <c r="C231" s="36"/>
-      <c r="D231" s="36"/>
-      <c r="E231" s="36"/>
+      <c r="B231" s="18" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C231" s="19" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D231" s="19" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E231" s="19" t="s">
+        <v>1140</v>
+      </c>
       <c r="F231" s="36"/>
       <c r="G231" s="55" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="H231" s="36"/>
     </row>
-    <row r="232" spans="1:8" ht="63" customHeight="1">
+    <row r="232" spans="1:8" ht="71" customHeight="1">
       <c r="A232" s="13" t="s">
-        <v>874</v>
-      </c>
-      <c r="B232" s="41"/>
+        <v>881</v>
+      </c>
+      <c r="B232" s="18" t="s">
+        <v>1143</v>
+      </c>
       <c r="C232" s="36"/>
       <c r="D232" s="36"/>
       <c r="E232" s="36"/>
       <c r="F232" s="36"/>
-      <c r="G232" s="20" t="s">
-        <v>691</v>
+      <c r="G232" s="55" t="s">
+        <v>705</v>
       </c>
       <c r="H232" s="36"/>
     </row>
-    <row r="233" spans="1:8" ht="70" customHeight="1">
+    <row r="233" spans="1:8" ht="84" customHeight="1">
       <c r="A233" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="B233" s="41"/>
-      <c r="C233" s="36"/>
+        <v>890</v>
+      </c>
+      <c r="B233" s="18" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C233" s="19" t="s">
+        <v>1144</v>
+      </c>
       <c r="D233" s="36"/>
       <c r="E233" s="36"/>
       <c r="F233" s="36"/>
-      <c r="G233" s="37" t="s">
-        <v>700</v>
+      <c r="G233" s="55" t="s">
+        <v>726</v>
       </c>
       <c r="H233" s="36"/>
     </row>
-    <row r="234" spans="1:8" ht="71" customHeight="1">
+    <row r="234" spans="1:8" ht="74" customHeight="1">
       <c r="A234" s="13" t="s">
-        <v>883</v>
-      </c>
-      <c r="B234" s="41"/>
-      <c r="C234" s="36"/>
-      <c r="D234" s="36"/>
+        <v>1146</v>
+      </c>
+      <c r="B234" s="18" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C234" s="19" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D234" s="19" t="s">
+        <v>1150</v>
+      </c>
       <c r="E234" s="36"/>
       <c r="F234" s="36"/>
-      <c r="G234" s="37" t="s">
-        <v>705</v>
+      <c r="G234" s="52" t="s">
+        <v>1149</v>
       </c>
       <c r="H234" s="36"/>
     </row>
     <row r="235" spans="1:8" ht="70" customHeight="1">
       <c r="A235" s="13" t="s">
-        <v>884</v>
+        <v>877</v>
       </c>
       <c r="B235" s="41"/>
       <c r="C235" s="36"/>
@@ -11419,41 +11560,41 @@
       <c r="E235" s="36"/>
       <c r="F235" s="36"/>
       <c r="G235" s="37" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="H235" s="36"/>
     </row>
-    <row r="236" spans="1:8" ht="60" customHeight="1">
+    <row r="236" spans="1:8" ht="63" customHeight="1">
       <c r="A236" s="13" t="s">
-        <v>885</v>
+        <v>872</v>
       </c>
       <c r="B236" s="41"/>
       <c r="C236" s="36"/>
       <c r="D236" s="36"/>
       <c r="E236" s="36"/>
       <c r="F236" s="36"/>
-      <c r="G236" s="37" t="s">
-        <v>708</v>
+      <c r="G236" s="20" t="s">
+        <v>691</v>
       </c>
       <c r="H236" s="36"/>
     </row>
-    <row r="237" spans="1:8" ht="68" customHeight="1">
+    <row r="237" spans="1:8" ht="70" customHeight="1">
       <c r="A237" s="13" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="B237" s="41"/>
       <c r="C237" s="36"/>
       <c r="D237" s="36"/>
       <c r="E237" s="36"/>
       <c r="F237" s="36"/>
-      <c r="G237" s="19" t="s">
-        <v>715</v>
+      <c r="G237" s="37" t="s">
+        <v>707</v>
       </c>
       <c r="H237" s="36"/>
     </row>
-    <row r="238" spans="1:8" ht="66" customHeight="1">
+    <row r="238" spans="1:8" ht="60" customHeight="1">
       <c r="A238" s="13" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="B238" s="41"/>
       <c r="C238" s="36"/>
@@ -11461,327 +11602,331 @@
       <c r="E238" s="36"/>
       <c r="F238" s="36"/>
       <c r="G238" s="37" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="H238" s="36"/>
     </row>
-    <row r="239" spans="1:8" ht="69" customHeight="1">
+    <row r="239" spans="1:8" ht="66" customHeight="1">
       <c r="A239" s="13" t="s">
-        <v>888</v>
-      </c>
-      <c r="B239" s="18" t="s">
-        <v>717</v>
-      </c>
+        <v>885</v>
+      </c>
+      <c r="B239" s="41"/>
       <c r="C239" s="36"/>
       <c r="D239" s="36"/>
       <c r="E239" s="36"/>
       <c r="F239" s="36"/>
       <c r="G239" s="37" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="H239" s="36"/>
     </row>
-    <row r="240" spans="1:8" ht="65" customHeight="1">
+    <row r="240" spans="1:8" ht="68" customHeight="1">
       <c r="A240" s="13" t="s">
-        <v>891</v>
-      </c>
-      <c r="B240" s="35" t="s">
-        <v>724</v>
-      </c>
-      <c r="C240" s="37" t="s">
-        <v>725</v>
+        <v>884</v>
+      </c>
+      <c r="B240" s="18" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C240" s="19" t="s">
+        <v>1137</v>
       </c>
       <c r="D240" s="36"/>
       <c r="E240" s="36"/>
       <c r="F240" s="36"/>
-      <c r="G240" s="37" t="s">
-        <v>723</v>
+      <c r="G240" s="19" t="s">
+        <v>715</v>
       </c>
       <c r="H240" s="36"/>
     </row>
-    <row r="241" spans="1:8" ht="84" customHeight="1">
+    <row r="241" spans="1:8" ht="69" customHeight="1">
       <c r="A241" s="13" t="s">
-        <v>892</v>
-      </c>
-      <c r="B241" s="41"/>
+        <v>886</v>
+      </c>
+      <c r="B241" s="18" t="s">
+        <v>717</v>
+      </c>
       <c r="C241" s="36"/>
       <c r="D241" s="36"/>
       <c r="E241" s="36"/>
       <c r="F241" s="36"/>
       <c r="G241" s="37" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
       <c r="H241" s="36"/>
     </row>
-    <row r="242" spans="1:8" ht="43" customHeight="1">
-      <c r="A242" s="14" t="s">
-        <v>727</v>
-      </c>
-      <c r="B242" s="41"/>
-      <c r="C242" s="36"/>
+    <row r="242" spans="1:8" ht="65" customHeight="1">
+      <c r="A242" s="13" t="s">
+        <v>889</v>
+      </c>
+      <c r="B242" s="35" t="s">
+        <v>724</v>
+      </c>
+      <c r="C242" s="37" t="s">
+        <v>725</v>
+      </c>
       <c r="D242" s="36"/>
       <c r="E242" s="36"/>
       <c r="F242" s="36"/>
       <c r="G242" s="37" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="H242" s="36"/>
     </row>
     <row r="243" spans="1:8" ht="55" customHeight="1">
       <c r="A243" s="13" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="B243" s="18" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C243" s="19" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D243" s="43" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E243" s="44"/>
       <c r="F243" s="44"/>
       <c r="G243" s="37" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="H243" s="44"/>
     </row>
     <row r="244" spans="1:8" ht="71" customHeight="1">
       <c r="A244" s="13" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="B244" s="18" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="C244" s="36"/>
       <c r="D244" s="44"/>
       <c r="E244" s="44"/>
       <c r="F244" s="43" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="G244" s="19" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="H244" s="44"/>
     </row>
     <row r="245" spans="1:8" ht="43" customHeight="1">
       <c r="A245" s="13" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="B245" s="35" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C245" s="19" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D245" s="45" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E245" s="44"/>
       <c r="F245" s="44"/>
       <c r="G245" s="37" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="H245" s="44"/>
     </row>
     <row r="246" spans="1:8" ht="97" customHeight="1">
       <c r="A246" s="13" t="s">
+        <v>751</v>
+      </c>
+      <c r="B246" s="35" t="s">
+        <v>752</v>
+      </c>
+      <c r="C246" s="19" t="s">
         <v>753</v>
       </c>
-      <c r="B246" s="35" t="s">
-        <v>754</v>
-      </c>
-      <c r="C246" s="19" t="s">
+      <c r="D246" s="45" t="s">
         <v>755</v>
-      </c>
-      <c r="D246" s="45" t="s">
-        <v>757</v>
       </c>
       <c r="E246" s="44"/>
       <c r="F246" s="44"/>
       <c r="G246" s="37" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="H246" s="44"/>
     </row>
     <row r="247" spans="1:8" ht="63" customHeight="1">
       <c r="A247" s="13" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="B247" s="18" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C247" s="19" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="D247" s="44"/>
       <c r="E247" s="44"/>
       <c r="F247" s="44"/>
       <c r="G247" s="37" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="H247" s="44"/>
     </row>
     <row r="248" spans="1:8" ht="57" customHeight="1">
       <c r="A248" s="13" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="B248" s="18" t="s">
+        <v>758</v>
+      </c>
+      <c r="C248" s="37" t="s">
         <v>760</v>
-      </c>
-      <c r="C248" s="37" t="s">
-        <v>762</v>
       </c>
       <c r="D248" s="44"/>
       <c r="E248" s="44"/>
       <c r="F248" s="44"/>
       <c r="G248" s="37" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="H248" s="44"/>
     </row>
     <row r="249" spans="1:8" ht="69" customHeight="1">
       <c r="A249" s="13" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="B249" s="18" t="s">
+        <v>762</v>
+      </c>
+      <c r="C249" s="19" t="s">
+        <v>763</v>
+      </c>
+      <c r="D249" s="19" t="s">
+        <v>765</v>
+      </c>
+      <c r="E249" s="19" t="s">
         <v>764</v>
       </c>
-      <c r="C249" s="19" t="s">
-        <v>765</v>
-      </c>
-      <c r="D249" s="19" t="s">
-        <v>767</v>
-      </c>
-      <c r="E249" s="19" t="s">
+      <c r="F249" s="19" t="s">
         <v>766</v>
       </c>
-      <c r="F249" s="19" t="s">
-        <v>768</v>
-      </c>
       <c r="G249" s="19" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="H249" s="44"/>
     </row>
     <row r="250" spans="1:8" ht="101" customHeight="1">
       <c r="A250" s="13" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="B250" s="35" t="s">
+        <v>768</v>
+      </c>
+      <c r="C250" s="19" t="s">
+        <v>769</v>
+      </c>
+      <c r="D250" s="19" t="s">
         <v>770</v>
-      </c>
-      <c r="C250" s="19" t="s">
-        <v>771</v>
-      </c>
-      <c r="D250" s="19" t="s">
-        <v>772</v>
       </c>
       <c r="E250" s="44"/>
       <c r="F250" s="44"/>
       <c r="G250" s="37" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="H250" s="44"/>
     </row>
     <row r="251" spans="1:8" s="4" customFormat="1" ht="72" customHeight="1">
       <c r="A251" s="13" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="B251" s="18" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C251" s="19" t="s">
+        <v>772</v>
+      </c>
+      <c r="D251" s="43" t="s">
         <v>774</v>
-      </c>
-      <c r="D251" s="43" t="s">
-        <v>776</v>
       </c>
       <c r="E251" s="43"/>
       <c r="F251" s="43" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="G251" s="20" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="H251" s="43"/>
     </row>
     <row r="252" spans="1:8" s="4" customFormat="1" ht="54" customHeight="1">
       <c r="A252" s="13" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="B252" s="18" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C252" s="19" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D252" s="43"/>
       <c r="E252" s="43"/>
       <c r="F252" s="43"/>
       <c r="G252" s="20" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="H252" s="43"/>
     </row>
     <row r="253" spans="1:8" ht="75" customHeight="1">
       <c r="A253" s="13" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="B253" s="18" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C253" s="36"/>
       <c r="D253" s="44"/>
       <c r="E253" s="44"/>
       <c r="F253" s="44"/>
       <c r="G253" s="37" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="H253" s="44"/>
     </row>
     <row r="254" spans="1:8" s="4" customFormat="1" ht="66" customHeight="1">
       <c r="A254" s="13" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B254" s="18" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C254" s="19"/>
       <c r="D254" s="43"/>
       <c r="E254" s="43"/>
       <c r="F254" s="43"/>
       <c r="G254" s="19" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="H254" s="43"/>
     </row>
     <row r="255" spans="1:8" s="3" customFormat="1" ht="42" customHeight="1">
       <c r="A255" s="14" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B255" s="18" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C255" s="37"/>
       <c r="D255" s="45"/>
       <c r="E255" s="45"/>
       <c r="F255" s="45"/>
       <c r="G255" s="37" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="H255" s="45"/>
     </row>
     <row r="256" spans="1:8" ht="48" customHeight="1">
       <c r="A256" s="13" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B256" s="18" t="s">
         <v>651</v>
       </c>
       <c r="C256" s="19" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D256" s="36"/>
       <c r="E256" s="36"/>
@@ -11793,57 +11938,59 @@
     </row>
     <row r="257" spans="1:8" s="4" customFormat="1" ht="89" customHeight="1">
       <c r="A257" s="13" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B257" s="18" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="C257" s="19" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="D257" s="43" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="E257" s="43"/>
       <c r="F257" s="43"/>
       <c r="G257" s="19" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="H257" s="43"/>
     </row>
     <row r="258" spans="1:8" s="3" customFormat="1" ht="64" customHeight="1">
       <c r="A258" s="13" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="B258" s="11" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="C258" s="6" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D258" s="49"/>
       <c r="E258" s="49"/>
       <c r="F258" s="49"/>
       <c r="G258" s="6" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="H258" s="49"/>
     </row>
     <row r="259" spans="1:8" ht="43" customHeight="1">
       <c r="A259" s="13" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="B259" s="8"/>
       <c r="C259" s="5"/>
       <c r="D259" s="1"/>
       <c r="E259" s="1"/>
       <c r="F259" s="1"/>
-      <c r="G259" s="5"/>
+      <c r="G259" s="49" t="s">
+        <v>1151</v>
+      </c>
       <c r="H259" s="1"/>
     </row>
     <row r="260" spans="1:8" ht="36" customHeight="1">
       <c r="A260" s="13" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="B260" s="8"/>
       <c r="C260" s="5"/>
@@ -11855,7 +12002,7 @@
     </row>
     <row r="261" spans="1:8" ht="46" customHeight="1">
       <c r="A261" s="13" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="B261" s="8"/>
       <c r="C261" s="5"/>
@@ -11867,7 +12014,7 @@
     </row>
     <row r="262" spans="1:8" ht="30" customHeight="1">
       <c r="A262" s="13" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="B262" s="8"/>
       <c r="C262" s="5"/>
@@ -11879,7 +12026,7 @@
     </row>
     <row r="263" spans="1:8" ht="25" customHeight="1">
       <c r="A263" s="14" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="B263" s="8"/>
       <c r="C263" s="5"/>
@@ -11891,7 +12038,7 @@
     </row>
     <row r="264" spans="1:8" ht="39" customHeight="1">
       <c r="A264" s="13" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="B264" s="8"/>
       <c r="C264" s="5"/>
@@ -11903,7 +12050,7 @@
     </row>
     <row r="265" spans="1:8" ht="29" customHeight="1">
       <c r="A265" s="14" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="B265" s="8"/>
       <c r="C265" s="5"/>
@@ -11915,7 +12062,7 @@
     </row>
     <row r="266" spans="1:8" ht="23" customHeight="1">
       <c r="A266" s="14" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="B266" s="8"/>
       <c r="C266" s="5"/>
@@ -11927,7 +12074,7 @@
     </row>
     <row r="267" spans="1:8" ht="22" customHeight="1">
       <c r="A267" s="14" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="B267" s="8"/>
       <c r="C267" s="5"/>
@@ -11939,7 +12086,7 @@
     </row>
     <row r="268" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A268" s="14" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="B268" s="57"/>
       <c r="C268" s="49"/>
@@ -11951,7 +12098,7 @@
     </row>
     <row r="269" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A269" s="14" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="B269" s="57"/>
       <c r="C269" s="49"/>
@@ -11963,7 +12110,7 @@
     </row>
     <row r="270" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A270" s="14" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="B270" s="57"/>
       <c r="C270" s="49"/>
@@ -11975,10 +12122,10 @@
     </row>
     <row r="271" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A271" s="14" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="B271" s="57" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="C271" s="49"/>
       <c r="D271" s="49"/>
@@ -11989,7 +12136,7 @@
     </row>
     <row r="272" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A272" s="14" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="B272" s="57"/>
       <c r="C272" s="49"/>
@@ -12001,7 +12148,7 @@
     </row>
     <row r="273" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A273" s="14" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="B273" s="57"/>
       <c r="C273" s="49"/>
@@ -12013,7 +12160,7 @@
     </row>
     <row r="274" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A274" s="14" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="B274" s="57"/>
       <c r="C274" s="49"/>
@@ -12025,10 +12172,10 @@
     </row>
     <row r="275" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A275" s="14" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="B275" s="57" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="C275" s="49"/>
       <c r="D275" s="49"/>
@@ -12039,7 +12186,7 @@
     </row>
     <row r="276" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A276" s="14" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="B276" s="57"/>
       <c r="C276" s="49"/>
@@ -12051,7 +12198,7 @@
     </row>
     <row r="277" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A277" s="14" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="B277" s="57"/>
       <c r="C277" s="49"/>
@@ -12063,7 +12210,7 @@
     </row>
     <row r="278" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A278" s="14" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="B278" s="57"/>
       <c r="C278" s="49"/>
@@ -12075,7 +12222,7 @@
     </row>
     <row r="279" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A279" s="14" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B279" s="57"/>
       <c r="C279" s="49"/>
@@ -12087,7 +12234,7 @@
     </row>
     <row r="280" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A280" s="14" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="B280" s="57"/>
       <c r="C280" s="49"/>
@@ -12099,7 +12246,7 @@
     </row>
     <row r="281" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A281" s="14" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="B281" s="57"/>
       <c r="C281" s="49"/>
@@ -12111,7 +12258,7 @@
     </row>
     <row r="282" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A282" s="14" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="B282" s="57"/>
       <c r="C282" s="49"/>
@@ -12123,7 +12270,7 @@
     </row>
     <row r="283" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A283" s="14" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="B283" s="57"/>
       <c r="C283" s="49"/>
@@ -12149,7 +12296,7 @@
     </row>
     <row r="285" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A285" s="14" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="B285" s="57"/>
       <c r="C285" s="49"/>
@@ -12161,7 +12308,7 @@
     </row>
     <row r="286" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A286" s="14" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="B286" s="57"/>
       <c r="C286" s="49"/>
@@ -12173,7 +12320,7 @@
     </row>
     <row r="287" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A287" s="14" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="B287" s="57"/>
       <c r="C287" s="49"/>
@@ -12185,29 +12332,29 @@
     </row>
     <row r="288" spans="1:8" s="58" customFormat="1" ht="53" customHeight="1">
       <c r="A288" s="14" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="B288" s="63" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="C288" s="64"/>
       <c r="D288" s="49"/>
       <c r="E288" s="49"/>
       <c r="F288" s="49"/>
       <c r="G288" s="6" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="H288" s="49"/>
     </row>
     <row r="289" spans="1:8" s="58" customFormat="1" ht="71" customHeight="1">
       <c r="A289" s="14" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="B289" s="63" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="C289" s="65" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="D289" s="49"/>
       <c r="E289" s="49"/>
@@ -12217,43 +12364,43 @@
     </row>
     <row r="290" spans="1:8" s="58" customFormat="1" ht="74" customHeight="1">
       <c r="A290" s="14" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="B290" s="63" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="C290" s="67" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="D290" s="49"/>
       <c r="E290" s="49"/>
       <c r="F290" s="49"/>
       <c r="G290" s="49" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="H290" s="49"/>
     </row>
     <row r="291" spans="1:8" s="58" customFormat="1" ht="74" customHeight="1">
       <c r="A291" s="66" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B291" s="18" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C291" s="67" t="s">
         <v>1081</v>
-      </c>
-      <c r="B291" s="18" t="s">
-        <v>1083</v>
-      </c>
-      <c r="C291" s="67" t="s">
-        <v>1084</v>
       </c>
       <c r="D291" s="49"/>
       <c r="E291" s="49"/>
       <c r="F291" s="49"/>
       <c r="G291" s="55" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="H291" s="49"/>
     </row>
     <row r="292" spans="1:8" s="58" customFormat="1" ht="34" customHeight="1">
       <c r="A292" s="14" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="B292" s="63"/>
       <c r="C292" s="49"/>
@@ -12265,7 +12412,7 @@
     </row>
     <row r="293" spans="1:8" s="58" customFormat="1" ht="43" customHeight="1">
       <c r="A293" s="14" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="B293" s="63"/>
       <c r="C293" s="49"/>
@@ -12277,7 +12424,7 @@
     </row>
     <row r="294" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A294" s="14" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="B294" s="57"/>
       <c r="C294" s="49"/>
@@ -12289,7 +12436,7 @@
     </row>
     <row r="295" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A295" s="14" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="B295" s="57"/>
       <c r="C295" s="49"/>
@@ -12301,7 +12448,7 @@
     </row>
     <row r="296" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A296" s="14" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="B296" s="57"/>
       <c r="C296" s="49"/>
@@ -12313,7 +12460,7 @@
     </row>
     <row r="297" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A297" s="14" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="B297" s="57"/>
       <c r="C297" s="49"/>
@@ -12325,7 +12472,7 @@
     </row>
     <row r="298" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A298" s="14" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="B298" s="57"/>
       <c r="C298" s="49"/>
@@ -12337,7 +12484,7 @@
     </row>
     <row r="299" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A299" s="14" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="B299" s="57"/>
       <c r="C299" s="49"/>
@@ -12349,7 +12496,7 @@
     </row>
     <row r="300" spans="1:8" ht="28" customHeight="1">
       <c r="A300" s="42" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B300" s="41"/>
       <c r="C300" s="36"/>
@@ -12357,13 +12504,13 @@
       <c r="E300" s="36"/>
       <c r="F300" s="36"/>
       <c r="G300" s="36" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="H300" s="36"/>
     </row>
     <row r="301" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A301" s="14" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="B301" s="57"/>
       <c r="C301" s="49"/>
@@ -12375,7 +12522,7 @@
     </row>
     <row r="302" spans="1:8" s="58" customFormat="1" ht="47" customHeight="1">
       <c r="A302" s="13" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="B302" s="57"/>
       <c r="C302" s="49"/>
@@ -12387,7 +12534,7 @@
     </row>
     <row r="303" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A303" s="14" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="B303" s="57"/>
       <c r="C303" s="49"/>
@@ -12399,7 +12546,7 @@
     </row>
     <row r="304" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A304" s="14" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="B304" s="57"/>
       <c r="C304" s="49"/>
@@ -12411,7 +12558,7 @@
     </row>
     <row r="305" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A305" s="14" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="B305" s="57"/>
       <c r="C305" s="49"/>
@@ -12423,7 +12570,7 @@
     </row>
     <row r="306" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A306" s="14" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="B306" s="57"/>
       <c r="C306" s="49"/>
@@ -12435,7 +12582,7 @@
     </row>
     <row r="307" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A307" s="14" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="B307" s="57"/>
       <c r="C307" s="49"/>
@@ -12447,7 +12594,7 @@
     </row>
     <row r="308" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A308" s="14" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="B308" s="57"/>
       <c r="C308" s="49"/>
@@ -12459,7 +12606,7 @@
     </row>
     <row r="309" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A309" s="14" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="B309" s="57"/>
       <c r="C309" s="49"/>
@@ -12471,7 +12618,7 @@
     </row>
     <row r="310" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A310" s="14" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="B310" s="57"/>
       <c r="C310" s="49"/>
@@ -12483,7 +12630,7 @@
     </row>
     <row r="311" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A311" s="14" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="B311" s="57"/>
       <c r="C311" s="49"/>
@@ -12495,7 +12642,7 @@
     </row>
     <row r="312" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A312" s="14" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="B312" s="57"/>
       <c r="C312" s="49"/>
@@ -12507,7 +12654,7 @@
     </row>
     <row r="313" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A313" s="14" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="B313" s="57"/>
       <c r="C313" s="49"/>
@@ -12519,7 +12666,7 @@
     </row>
     <row r="314" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A314" s="14" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="B314" s="57"/>
       <c r="C314" s="49"/>
@@ -12531,7 +12678,7 @@
     </row>
     <row r="315" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A315" s="14" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="B315" s="57"/>
       <c r="C315" s="49"/>
@@ -12543,7 +12690,7 @@
     </row>
     <row r="316" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A316" s="14" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="B316" s="57"/>
       <c r="C316" s="49"/>
@@ -12555,7 +12702,7 @@
     </row>
     <row r="317" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A317" s="14" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B317" s="57"/>
       <c r="C317" s="49"/>
@@ -12567,7 +12714,7 @@
     </row>
     <row r="318" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A318" s="14" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="B318" s="57"/>
       <c r="C318" s="49"/>
@@ -12579,7 +12726,7 @@
     </row>
     <row r="319" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A319" s="14" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="B319" s="57"/>
       <c r="C319" s="49"/>
@@ -12591,7 +12738,7 @@
     </row>
     <row r="320" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A320" s="14" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B320" s="57"/>
       <c r="C320" s="49"/>
@@ -12603,7 +12750,7 @@
     </row>
     <row r="321" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A321" s="14" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="B321" s="57"/>
       <c r="C321" s="49"/>
@@ -12615,7 +12762,7 @@
     </row>
     <row r="322" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A322" s="14" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="B322" s="57"/>
       <c r="C322" s="49"/>
@@ -12627,7 +12774,7 @@
     </row>
     <row r="323" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A323" s="14" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="B323" s="57"/>
       <c r="C323" s="49"/>
@@ -12639,7 +12786,7 @@
     </row>
     <row r="324" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A324" s="14" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="B324" s="57"/>
       <c r="C324" s="49"/>
@@ -12651,7 +12798,7 @@
     </row>
     <row r="325" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A325" s="14" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="B325" s="57"/>
       <c r="C325" s="49"/>
@@ -12663,7 +12810,7 @@
     </row>
     <row r="326" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A326" s="14" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="B326" s="57"/>
       <c r="C326" s="49"/>
@@ -12675,7 +12822,7 @@
     </row>
     <row r="327" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A327" s="14" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="B327" s="57"/>
       <c r="C327" s="49"/>
@@ -12687,7 +12834,7 @@
     </row>
     <row r="328" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A328" s="14" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="B328" s="57"/>
       <c r="C328" s="49"/>
@@ -12699,7 +12846,7 @@
     </row>
     <row r="329" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A329" s="14" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="B329" s="57"/>
       <c r="C329" s="49"/>
@@ -12711,7 +12858,7 @@
     </row>
     <row r="330" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A330" s="14" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="B330" s="57"/>
       <c r="C330" s="49"/>
@@ -12723,7 +12870,7 @@
     </row>
     <row r="331" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A331" s="14" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="B331" s="57"/>
       <c r="C331" s="49"/>
@@ -12735,7 +12882,7 @@
     </row>
     <row r="332" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A332" s="14" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="B332" s="57"/>
       <c r="C332" s="49"/>
@@ -12747,7 +12894,7 @@
     </row>
     <row r="333" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A333" s="14" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="B333" s="57"/>
       <c r="C333" s="49"/>
@@ -12759,7 +12906,7 @@
     </row>
     <row r="334" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A334" s="14" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="B334" s="57"/>
       <c r="C334" s="49"/>
@@ -12771,7 +12918,7 @@
     </row>
     <row r="335" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A335" s="14" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="B335" s="57"/>
       <c r="C335" s="49"/>
@@ -12783,7 +12930,7 @@
     </row>
     <row r="336" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A336" s="14" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="B336" s="35"/>
       <c r="C336" s="37"/>
@@ -12795,7 +12942,7 @@
     </row>
     <row r="337" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A337" s="14" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="B337" s="35"/>
       <c r="C337" s="37"/>
@@ -12807,7 +12954,7 @@
     </row>
     <row r="338" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A338" s="14" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="B338" s="35"/>
       <c r="C338" s="37"/>
@@ -12819,7 +12966,7 @@
     </row>
     <row r="339" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A339" s="14" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="B339" s="35"/>
       <c r="C339" s="37"/>
@@ -12831,7 +12978,7 @@
     </row>
     <row r="340" spans="1:8">
       <c r="A340" s="56" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="B340" s="8"/>
       <c r="C340" s="5"/>
@@ -12843,7 +12990,7 @@
     </row>
     <row r="341" spans="1:8">
       <c r="A341" s="56" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="B341" s="8"/>
       <c r="C341" s="5"/>
@@ -12855,7 +13002,7 @@
     </row>
     <row r="342" spans="1:8">
       <c r="A342" s="56" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="B342" s="8"/>
       <c r="C342" s="5"/>
@@ -12867,7 +13014,7 @@
     </row>
     <row r="343" spans="1:8">
       <c r="A343" s="56" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="B343" s="8"/>
       <c r="C343" s="5"/>
@@ -12879,7 +13026,7 @@
     </row>
     <row r="344" spans="1:8">
       <c r="A344" s="56" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="B344" s="8"/>
       <c r="C344" s="5"/>
@@ -12891,7 +13038,7 @@
     </row>
     <row r="345" spans="1:8">
       <c r="A345" s="56" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="B345" s="8"/>
       <c r="C345" s="5"/>
@@ -12903,7 +13050,7 @@
     </row>
     <row r="346" spans="1:8">
       <c r="A346" s="56" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="B346" s="8"/>
       <c r="C346" s="5"/>
@@ -12915,7 +13062,7 @@
     </row>
     <row r="347" spans="1:8">
       <c r="A347" s="56" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="B347" s="8"/>
       <c r="C347" s="5"/>
@@ -13468,36 +13615,38 @@
     <hyperlink ref="G46" r:id="rId109" xr:uid="{52F32864-DDFD-044B-A6E1-085054B9B200}"/>
     <hyperlink ref="G208" r:id="rId110" xr:uid="{23D9C103-F2A2-474D-8B3B-C8B3ADAFAF09}"/>
     <hyperlink ref="G209" r:id="rId111" xr:uid="{2401B952-575E-1D45-AF80-42C35916F8A5}"/>
-    <hyperlink ref="G232" r:id="rId112" xr:uid="{7D0AAFC1-C690-2B49-9EB8-E3BA672C2424}"/>
-    <hyperlink ref="G212" r:id="rId113" xr:uid="{31219583-F195-ED42-A799-1B054B7D9E84}"/>
-    <hyperlink ref="G251" r:id="rId114" xr:uid="{E7446763-7D68-D94F-887C-EEC8548E4D16}"/>
-    <hyperlink ref="G252" r:id="rId115" xr:uid="{11A405A4-DF58-9545-BCDE-9414DE390A5E}"/>
-    <hyperlink ref="G142" r:id="rId116" xr:uid="{E5B20948-57A8-2E48-9191-175A672155C6}"/>
-    <hyperlink ref="G148" r:id="rId117" xr:uid="{08B7E248-E2F5-4A4A-BAC3-ABDA6CE1A484}"/>
-    <hyperlink ref="G161" r:id="rId118" xr:uid="{E597C9B9-B49B-E748-9679-4D7E6A09DF83}"/>
-    <hyperlink ref="G160" r:id="rId119" xr:uid="{E5F509BA-2BB8-D149-AA35-7BDB432E18AF}"/>
-    <hyperlink ref="G162" r:id="rId120" xr:uid="{4FC031CC-93DC-9244-9042-8DD1D67AC6F9}"/>
-    <hyperlink ref="G163" r:id="rId121" xr:uid="{C62E4B96-B936-B44E-8C2F-3864E9CFE4CC}"/>
-    <hyperlink ref="G164" r:id="rId122" xr:uid="{1BA81E42-D0F9-0044-8ED4-7FEE90A1B0AA}"/>
-    <hyperlink ref="G165" r:id="rId123" xr:uid="{A8CD9D15-E8C0-344E-A762-C25892E3B26A}"/>
-    <hyperlink ref="G166" r:id="rId124" xr:uid="{798B478D-29D7-E04E-8FB6-1E725649CEDE}"/>
-    <hyperlink ref="G181" r:id="rId125" xr:uid="{128F6ED5-8C9A-E146-83DF-187B87ED530F}"/>
-    <hyperlink ref="G189" r:id="rId126" xr:uid="{37331509-B7B8-7548-B5C6-857F36A7E109}"/>
-    <hyperlink ref="G190" r:id="rId127" xr:uid="{31FA25FC-46C7-D74A-99A5-1140E96809B5}"/>
-    <hyperlink ref="G198" r:id="rId128" xr:uid="{5CC18E71-C5D0-6A4D-AD79-B547613CD77D}"/>
-    <hyperlink ref="G291" r:id="rId129" xr:uid="{754094CD-003E-114E-B66D-2DEF0C37F04E}"/>
-    <hyperlink ref="G221" r:id="rId130" xr:uid="{88298BD6-A42F-864A-B628-C970B3D8AF36}"/>
-    <hyperlink ref="G220" r:id="rId131" xr:uid="{9D9B7F12-8E09-F14A-B4B2-B2CC263E87C2}"/>
-    <hyperlink ref="G222" r:id="rId132" xr:uid="{0CC180BE-FEEA-EA49-95EB-93F1AE813670}"/>
-    <hyperlink ref="G223" r:id="rId133" xr:uid="{ACF47BBB-0D42-1849-8E8C-F5374D58E72D}"/>
-    <hyperlink ref="G224" r:id="rId134" xr:uid="{F915674D-C6EE-8A49-BE56-B6E982947AE2}"/>
-    <hyperlink ref="G225" r:id="rId135" xr:uid="{59F0714C-9A83-7D45-94D6-EE6C98DDAA40}"/>
-    <hyperlink ref="G227" r:id="rId136" xr:uid="{0C8EEDA6-B628-FA4E-B83A-1C9AADAC775C}"/>
-    <hyperlink ref="G228" r:id="rId137" xr:uid="{5F7B4D87-E8BA-7148-A5D6-FB61786A1C54}"/>
-    <hyperlink ref="G230" r:id="rId138" xr:uid="{51F23D9B-48FC-4E4D-905C-C274C579A1CA}"/>
-    <hyperlink ref="G231" r:id="rId139" xr:uid="{D16C412B-860F-AC42-B67E-D71B6B8C1E14}"/>
+    <hyperlink ref="G212" r:id="rId112" xr:uid="{31219583-F195-ED42-A799-1B054B7D9E84}"/>
+    <hyperlink ref="G251" r:id="rId113" xr:uid="{E7446763-7D68-D94F-887C-EEC8548E4D16}"/>
+    <hyperlink ref="G252" r:id="rId114" xr:uid="{11A405A4-DF58-9545-BCDE-9414DE390A5E}"/>
+    <hyperlink ref="G142" r:id="rId115" xr:uid="{E5B20948-57A8-2E48-9191-175A672155C6}"/>
+    <hyperlink ref="G148" r:id="rId116" xr:uid="{08B7E248-E2F5-4A4A-BAC3-ABDA6CE1A484}"/>
+    <hyperlink ref="G161" r:id="rId117" xr:uid="{E597C9B9-B49B-E748-9679-4D7E6A09DF83}"/>
+    <hyperlink ref="G160" r:id="rId118" xr:uid="{E5F509BA-2BB8-D149-AA35-7BDB432E18AF}"/>
+    <hyperlink ref="G162" r:id="rId119" xr:uid="{4FC031CC-93DC-9244-9042-8DD1D67AC6F9}"/>
+    <hyperlink ref="G163" r:id="rId120" xr:uid="{C62E4B96-B936-B44E-8C2F-3864E9CFE4CC}"/>
+    <hyperlink ref="G164" r:id="rId121" xr:uid="{1BA81E42-D0F9-0044-8ED4-7FEE90A1B0AA}"/>
+    <hyperlink ref="G165" r:id="rId122" xr:uid="{A8CD9D15-E8C0-344E-A762-C25892E3B26A}"/>
+    <hyperlink ref="G166" r:id="rId123" xr:uid="{798B478D-29D7-E04E-8FB6-1E725649CEDE}"/>
+    <hyperlink ref="G181" r:id="rId124" xr:uid="{128F6ED5-8C9A-E146-83DF-187B87ED530F}"/>
+    <hyperlink ref="G189" r:id="rId125" xr:uid="{37331509-B7B8-7548-B5C6-857F36A7E109}"/>
+    <hyperlink ref="G190" r:id="rId126" xr:uid="{31FA25FC-46C7-D74A-99A5-1140E96809B5}"/>
+    <hyperlink ref="G198" r:id="rId127" xr:uid="{5CC18E71-C5D0-6A4D-AD79-B547613CD77D}"/>
+    <hyperlink ref="G291" r:id="rId128" xr:uid="{754094CD-003E-114E-B66D-2DEF0C37F04E}"/>
+    <hyperlink ref="G221" r:id="rId129" xr:uid="{88298BD6-A42F-864A-B628-C970B3D8AF36}"/>
+    <hyperlink ref="G220" r:id="rId130" xr:uid="{9D9B7F12-8E09-F14A-B4B2-B2CC263E87C2}"/>
+    <hyperlink ref="G222" r:id="rId131" xr:uid="{0CC180BE-FEEA-EA49-95EB-93F1AE813670}"/>
+    <hyperlink ref="G223" r:id="rId132" xr:uid="{ACF47BBB-0D42-1849-8E8C-F5374D58E72D}"/>
+    <hyperlink ref="G224" r:id="rId133" xr:uid="{F915674D-C6EE-8A49-BE56-B6E982947AE2}"/>
+    <hyperlink ref="G225" r:id="rId134" xr:uid="{59F0714C-9A83-7D45-94D6-EE6C98DDAA40}"/>
+    <hyperlink ref="G227" r:id="rId135" xr:uid="{0C8EEDA6-B628-FA4E-B83A-1C9AADAC775C}"/>
+    <hyperlink ref="G228" r:id="rId136" xr:uid="{5F7B4D87-E8BA-7148-A5D6-FB61786A1C54}"/>
+    <hyperlink ref="G230" r:id="rId137" xr:uid="{51F23D9B-48FC-4E4D-905C-C274C579A1CA}"/>
+    <hyperlink ref="G231" r:id="rId138" xr:uid="{D16C412B-860F-AC42-B67E-D71B6B8C1E14}"/>
+    <hyperlink ref="G233" r:id="rId139" xr:uid="{7D0AAFC1-C690-2B49-9EB8-E3BA672C2424}"/>
+    <hyperlink ref="G232" r:id="rId140" xr:uid="{A65E0F05-0669-C64B-A8E6-50DC31570000}"/>
+    <hyperlink ref="G234" r:id="rId141" xr:uid="{7D3C258D-3141-A34D-BFE7-93ABAF4EC570}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId140"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId142"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
alternate positive negative number
</commit_message>
<xml_diff>
--- a/Applications/QuestionListWithApproaches.xlsx
+++ b/Applications/QuestionListWithApproaches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksharkashyap/Documents/VisualStudio/Applications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0724F3E0-3EDE-EF47-B101-1F985AD0CDA0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FE0F1E-F039-244E-B50E-216CB8C7BF3E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="460" windowWidth="32600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="1152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="1156">
   <si>
     <t>Convert Binary Number in a Linked List to Integer</t>
   </si>
@@ -5201,9 +5201,6 @@
     </r>
   </si>
   <si>
-    <t>rearrange array in alternating positive &amp; negative items with O(1) extra space</t>
-  </si>
-  <si>
     <t>given an array of size n and a number k, find all elements that appear more than n/k times</t>
   </si>
   <si>
@@ -6440,6 +6437,41 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/find-common-elements-three-sorted-arrays/</t>
+  </si>
+  <si>
+    <t>A simple solution is to first find intersection of two arrays and store the intersection in a temporary array, then find the intersection of third array and temporary array</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/rearrange-array-alternating-positive-negative-items-o1-extra-space/</t>
+  </si>
+  <si>
+    <t>same as intersection of 2 arrays, extend it to three pointers.time O(x+y+z)
+1)loop till you advance the min(x,y,z) 
+2)if all are same add to answer and advance all 3
+3)keep the largest and advance the remaining (2 or 1(if there are 2 large))</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>rearrange array in alternating positive &amp; negative items with O(1) extra space</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> [note that order of appearance should be preserved and number of positive and negative numbers need not be equal, in this case just place them in the end]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Trivial solution :O(n) space </t>
   </si>
 </sst>
 </file>
@@ -6755,7 +6787,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
@@ -6938,6 +6970,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7225,8 +7260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" zoomScale="160" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A259" sqref="A259"/>
+    <sheetView tabSelected="1" topLeftCell="A257" zoomScale="200" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C260" sqref="C260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7548,7 +7583,7 @@
         <v>736</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>
@@ -7577,13 +7612,13 @@
     </row>
     <row r="19" spans="1:8" ht="46" customHeight="1">
       <c r="A19" s="13" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -7593,13 +7628,13 @@
     </row>
     <row r="20" spans="1:8" ht="43" customHeight="1">
       <c r="A20" s="14" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -7609,13 +7644,13 @@
     </row>
     <row r="21" spans="1:8" ht="63" customHeight="1">
       <c r="A21" s="14" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B21" s="61" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C21" s="62" t="s">
         <v>1067</v>
-      </c>
-      <c r="C21" s="62" t="s">
-        <v>1068</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -7625,7 +7660,7 @@
     </row>
     <row r="22" spans="1:8" ht="24" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="5"/>
@@ -7637,7 +7672,7 @@
     </row>
     <row r="23" spans="1:8" ht="32" customHeight="1">
       <c r="A23" s="14" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="5"/>
@@ -7649,7 +7684,7 @@
     </row>
     <row r="24" spans="1:8" ht="33" customHeight="1">
       <c r="A24" s="14" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="5"/>
@@ -7661,7 +7696,7 @@
     </row>
     <row r="25" spans="1:8" ht="33" customHeight="1">
       <c r="A25" s="14" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="5"/>
@@ -7673,7 +7708,7 @@
     </row>
     <row r="26" spans="1:8" ht="33" customHeight="1">
       <c r="A26" s="14" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="5"/>
@@ -7685,7 +7720,7 @@
     </row>
     <row r="27" spans="1:8" ht="29" customHeight="1">
       <c r="A27" s="14" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
@@ -11102,32 +11137,32 @@
     </row>
     <row r="211" spans="1:8" ht="61" customHeight="1">
       <c r="A211" s="13" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B211" s="18" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C211" s="19"/>
       <c r="D211" s="19"/>
       <c r="E211" s="19"/>
       <c r="F211" s="19"/>
       <c r="G211" s="20" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="H211" s="19"/>
     </row>
     <row r="212" spans="1:8" ht="78" customHeight="1">
       <c r="A212" s="13" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B212" s="35" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C212" s="19" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D212" s="19" t="s">
         <v>1087</v>
-      </c>
-      <c r="C212" s="19" t="s">
-        <v>1097</v>
-      </c>
-      <c r="D212" s="19" t="s">
-        <v>1088</v>
       </c>
       <c r="F212" s="36"/>
       <c r="G212" s="40" t="s">
@@ -11135,466 +11170,470 @@
       </c>
       <c r="H212" s="36"/>
     </row>
-    <row r="213" spans="1:8" ht="76" customHeight="1">
+    <row r="213" spans="1:8" ht="79" customHeight="1">
       <c r="A213" s="13" t="s">
+        <v>959</v>
+      </c>
+      <c r="B213" s="46" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C213" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D213" s="1"/>
+      <c r="E213" s="1"/>
+      <c r="F213" s="1"/>
+      <c r="G213" s="49" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H213" s="1"/>
+    </row>
+    <row r="214" spans="1:8" ht="76" customHeight="1">
+      <c r="A214" s="13" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B214" s="18" t="s">
         <v>1089</v>
       </c>
-      <c r="B213" s="18" t="s">
-        <v>1090</v>
-      </c>
-      <c r="C213" s="36"/>
-      <c r="D213" s="36"/>
-      <c r="E213" s="36"/>
-      <c r="F213" s="36"/>
-      <c r="G213" s="40" t="s">
-        <v>1093</v>
-      </c>
-      <c r="H213" s="36"/>
-    </row>
-    <row r="214" spans="1:8" ht="83" customHeight="1">
-      <c r="A214" s="13" t="s">
-        <v>1091</v>
-      </c>
-      <c r="B214" s="18" t="s">
-        <v>1095</v>
-      </c>
-      <c r="C214" s="39" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D214" s="19" t="s">
-        <v>1094</v>
-      </c>
+      <c r="C214" s="36"/>
+      <c r="D214" s="36"/>
+      <c r="E214" s="36"/>
       <c r="F214" s="36"/>
       <c r="G214" s="40" t="s">
         <v>1092</v>
       </c>
       <c r="H214" s="36"/>
     </row>
-    <row r="215" spans="1:8" ht="79" customHeight="1">
+    <row r="215" spans="1:8" ht="83" customHeight="1">
       <c r="A215" s="13" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B215" s="18" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C215" s="39" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D215" s="19" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F215" s="36"/>
+      <c r="G215" s="40" t="s">
+        <v>1091</v>
+      </c>
+      <c r="H215" s="36"/>
+    </row>
+    <row r="216" spans="1:8" ht="79" customHeight="1">
+      <c r="A216" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="B215" s="35" t="s">
+      <c r="B216" s="35" t="s">
         <v>695</v>
       </c>
-      <c r="C215" s="37" t="s">
+      <c r="C216" s="37" t="s">
         <v>697</v>
       </c>
-      <c r="D215" s="37" t="s">
+      <c r="D216" s="37" t="s">
         <v>696</v>
       </c>
-      <c r="E215" s="36"/>
-      <c r="F215" s="36"/>
-      <c r="G215" s="37" t="s">
-        <v>694</v>
-      </c>
-      <c r="H215" s="36"/>
-    </row>
-    <row r="216" spans="1:8" ht="43" customHeight="1">
-      <c r="A216" s="14" t="s">
-        <v>876</v>
-      </c>
-      <c r="B216" s="18" t="s">
-        <v>698</v>
-      </c>
-      <c r="C216" s="36"/>
-      <c r="D216" s="19"/>
       <c r="E216" s="36"/>
       <c r="F216" s="36"/>
       <c r="G216" s="37" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="H216" s="36"/>
     </row>
-    <row r="217" spans="1:8" ht="63" customHeight="1">
-      <c r="A217" s="33" t="s">
-        <v>1048</v>
+    <row r="217" spans="1:8" ht="43" customHeight="1">
+      <c r="A217" s="14" t="s">
+        <v>876</v>
       </c>
       <c r="B217" s="18" t="s">
-        <v>1049</v>
+        <v>698</v>
       </c>
       <c r="C217" s="36"/>
-      <c r="D217" s="36"/>
+      <c r="D217" s="19"/>
       <c r="E217" s="36"/>
       <c r="F217" s="36"/>
       <c r="G217" s="37" t="s">
+        <v>699</v>
+      </c>
+      <c r="H217" s="36"/>
+    </row>
+    <row r="218" spans="1:8" ht="63" customHeight="1">
+      <c r="A218" s="33" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B218" s="18" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C218" s="36"/>
+      <c r="D218" s="36"/>
+      <c r="E218" s="36"/>
+      <c r="F218" s="36"/>
+      <c r="G218" s="37" t="s">
         <v>721</v>
       </c>
-      <c r="H217" s="36"/>
-    </row>
-    <row r="218" spans="1:8" s="4" customFormat="1" ht="104" customHeight="1">
-      <c r="A218" s="32" t="s">
+      <c r="H218" s="36"/>
+    </row>
+    <row r="219" spans="1:8" s="4" customFormat="1" ht="104" customHeight="1">
+      <c r="A219" s="32" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B219" s="18" t="s">
+        <v>690</v>
+      </c>
+      <c r="C219" s="67" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D219" s="19" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E219" s="38" t="s">
         <v>1101</v>
       </c>
-      <c r="B218" s="18" t="s">
-        <v>690</v>
-      </c>
-      <c r="C218" s="67" t="s">
-        <v>1098</v>
-      </c>
-      <c r="D218" s="19" t="s">
+      <c r="F219" s="62" t="s">
+        <v>1102</v>
+      </c>
+      <c r="G219" s="19" t="s">
         <v>1099</v>
       </c>
-      <c r="E218" s="38" t="s">
-        <v>1102</v>
-      </c>
-      <c r="F218" s="62" t="s">
-        <v>1103</v>
-      </c>
-      <c r="G218" s="19" t="s">
-        <v>1100</v>
-      </c>
-      <c r="H218" s="19"/>
-    </row>
-    <row r="219" spans="1:8" ht="71" customHeight="1">
-      <c r="A219" s="13" t="s">
+      <c r="H219" s="19"/>
+    </row>
+    <row r="220" spans="1:8" ht="71" customHeight="1">
+      <c r="A220" s="13" t="s">
         <v>878</v>
       </c>
-      <c r="B219" s="18" t="s">
+      <c r="B220" s="18" t="s">
         <v>879</v>
       </c>
-      <c r="C219" s="19" t="s">
+      <c r="C220" s="19" t="s">
         <v>702</v>
       </c>
-      <c r="D219" s="36"/>
-      <c r="E219" s="36"/>
-      <c r="F219" s="36"/>
-      <c r="G219" s="19" t="s">
+      <c r="D220" s="36"/>
+      <c r="E220" s="36"/>
+      <c r="F220" s="36"/>
+      <c r="G220" s="19" t="s">
         <v>701</v>
       </c>
-      <c r="H219" s="37" t="s">
+      <c r="H220" s="37" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="220" spans="1:8" ht="96" customHeight="1">
-      <c r="A220" s="13" t="s">
+    <row r="221" spans="1:8" ht="96" customHeight="1">
+      <c r="A221" s="13" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B221" s="35" t="s">
         <v>1105</v>
       </c>
-      <c r="B220" s="35" t="s">
+      <c r="C221" s="19" t="s">
         <v>1106</v>
       </c>
-      <c r="C220" s="19" t="s">
+      <c r="D221" s="19" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E221" s="39" t="s">
         <v>1107</v>
       </c>
-      <c r="D220" s="19" t="s">
+      <c r="F221" s="19" t="s">
         <v>1109</v>
       </c>
-      <c r="E220" s="39" t="s">
-        <v>1108</v>
-      </c>
-      <c r="F220" s="19" t="s">
+      <c r="G221" s="68" t="s">
+        <v>706</v>
+      </c>
+      <c r="H221" s="36"/>
+    </row>
+    <row r="222" spans="1:8" ht="76" customHeight="1">
+      <c r="A222" s="13" t="s">
+        <v>880</v>
+      </c>
+      <c r="B222" s="18" t="s">
         <v>1110</v>
       </c>
-      <c r="G220" s="68" t="s">
-        <v>706</v>
-      </c>
-      <c r="H220" s="36"/>
-    </row>
-    <row r="221" spans="1:8" ht="76" customHeight="1">
-      <c r="A221" s="13" t="s">
-        <v>880</v>
-      </c>
-      <c r="B221" s="18" t="s">
+      <c r="C222" s="19" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D222" s="19" t="s">
         <v>1111</v>
       </c>
-      <c r="C221" s="19" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D221" s="19" t="s">
-        <v>1112</v>
-      </c>
-      <c r="E221" s="19"/>
-      <c r="F221" s="36"/>
-      <c r="G221" s="68" t="s">
-        <v>704</v>
-      </c>
-      <c r="H221" s="36"/>
-    </row>
-    <row r="222" spans="1:8" ht="79" customHeight="1">
-      <c r="A222" s="13" t="s">
-        <v>1115</v>
-      </c>
-      <c r="B222" s="18" t="s">
-        <v>1114</v>
-      </c>
-      <c r="C222" s="19" t="s">
-        <v>1116</v>
-      </c>
-      <c r="D222" s="69" t="s">
-        <v>1117</v>
-      </c>
-      <c r="E222" s="39"/>
+      <c r="E222" s="19"/>
       <c r="F222" s="36"/>
       <c r="G222" s="68" t="s">
-        <v>720</v>
+        <v>704</v>
       </c>
       <c r="H222" s="36"/>
     </row>
-    <row r="223" spans="1:8" ht="56" customHeight="1">
-      <c r="A223" s="33" t="s">
-        <v>888</v>
+    <row r="223" spans="1:8" ht="79" customHeight="1">
+      <c r="A223" s="13" t="s">
+        <v>1114</v>
       </c>
       <c r="B223" s="18" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C223" s="36"/>
-      <c r="D223" s="36"/>
-      <c r="E223" s="36"/>
+        <v>1113</v>
+      </c>
+      <c r="C223" s="19" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D223" s="69" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E223" s="39"/>
       <c r="F223" s="36"/>
       <c r="G223" s="68" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="H223" s="36"/>
     </row>
-    <row r="224" spans="1:8" ht="44" customHeight="1">
-      <c r="A224" s="13" t="s">
-        <v>887</v>
+    <row r="224" spans="1:8" ht="56" customHeight="1">
+      <c r="A224" s="33" t="s">
+        <v>888</v>
       </c>
       <c r="B224" s="18" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="C224" s="36"/>
       <c r="D224" s="36"/>
       <c r="E224" s="36"/>
       <c r="F224" s="36"/>
       <c r="G224" s="68" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="H224" s="36"/>
     </row>
-    <row r="225" spans="1:8" ht="70" customHeight="1">
+    <row r="225" spans="1:8" ht="44" customHeight="1">
       <c r="A225" s="13" t="s">
-        <v>874</v>
+        <v>887</v>
       </c>
       <c r="B225" s="18" t="s">
-        <v>1119</v>
-      </c>
-      <c r="C225" s="19" t="s">
-        <v>1120</v>
-      </c>
+        <v>1117</v>
+      </c>
+      <c r="C225" s="36"/>
       <c r="D225" s="36"/>
       <c r="E225" s="36"/>
       <c r="F225" s="36"/>
-      <c r="G225" s="55" t="s">
-        <v>693</v>
+      <c r="G225" s="68" t="s">
+        <v>719</v>
       </c>
       <c r="H225" s="36"/>
     </row>
-    <row r="226" spans="1:8" ht="69" customHeight="1">
+    <row r="226" spans="1:8" ht="70" customHeight="1">
       <c r="A226" s="13" t="s">
-        <v>892</v>
+        <v>874</v>
       </c>
       <c r="B226" s="18" t="s">
-        <v>730</v>
-      </c>
-      <c r="C226" s="36"/>
+        <v>1118</v>
+      </c>
+      <c r="C226" s="19" t="s">
+        <v>1119</v>
+      </c>
       <c r="D226" s="36"/>
       <c r="E226" s="36"/>
       <c r="F226" s="36"/>
-      <c r="G226" s="37" t="s">
-        <v>731</v>
+      <c r="G226" s="55" t="s">
+        <v>693</v>
       </c>
       <c r="H226" s="36"/>
     </row>
-    <row r="227" spans="1:8" ht="79" customHeight="1">
+    <row r="227" spans="1:8" ht="69" customHeight="1">
       <c r="A227" s="13" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B227" s="18" t="s">
-        <v>1122</v>
+        <v>730</v>
       </c>
       <c r="C227" s="36"/>
       <c r="D227" s="36"/>
       <c r="E227" s="36"/>
       <c r="F227" s="36"/>
-      <c r="G227" s="68" t="s">
-        <v>727</v>
+      <c r="G227" s="37" t="s">
+        <v>731</v>
       </c>
       <c r="H227" s="36"/>
     </row>
-    <row r="228" spans="1:8" ht="46" customHeight="1">
-      <c r="A228" s="14" t="s">
-        <v>728</v>
+    <row r="228" spans="1:8" ht="79" customHeight="1">
+      <c r="A228" s="13" t="s">
+        <v>891</v>
       </c>
       <c r="B228" s="18" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="C228" s="36"/>
       <c r="D228" s="36"/>
       <c r="E228" s="36"/>
       <c r="F228" s="36"/>
       <c r="G228" s="68" t="s">
+        <v>727</v>
+      </c>
+      <c r="H228" s="36"/>
+    </row>
+    <row r="229" spans="1:8" ht="46" customHeight="1">
+      <c r="A229" s="14" t="s">
+        <v>728</v>
+      </c>
+      <c r="B229" s="18" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C229" s="36"/>
+      <c r="D229" s="36"/>
+      <c r="E229" s="36"/>
+      <c r="F229" s="36"/>
+      <c r="G229" s="68" t="s">
         <v>729</v>
       </c>
-      <c r="H228" s="36"/>
-    </row>
-    <row r="229" spans="1:8" ht="66" customHeight="1">
-      <c r="A229" s="13" t="s">
-        <v>1129</v>
-      </c>
-      <c r="B229" s="18" t="s">
-        <v>1133</v>
-      </c>
-      <c r="C229" s="67" t="s">
-        <v>1126</v>
-      </c>
-      <c r="D229" s="19" t="s">
-        <v>1127</v>
-      </c>
-      <c r="E229" s="36"/>
-      <c r="F229" s="19" t="s">
-        <v>1134</v>
-      </c>
-      <c r="G229" s="52" t="s">
-        <v>1125</v>
-      </c>
-      <c r="H229" s="19"/>
-    </row>
-    <row r="230" spans="1:8" ht="75" customHeight="1">
+      <c r="H229" s="36"/>
+    </row>
+    <row r="230" spans="1:8" ht="66" customHeight="1">
       <c r="A230" s="13" t="s">
         <v>1128</v>
       </c>
       <c r="B230" s="18" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C230" s="67" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D230" s="19" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E230" s="36"/>
+      <c r="F230" s="19" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G230" s="52" t="s">
         <v>1124</v>
       </c>
-      <c r="C230" s="67" t="s">
+      <c r="H230" s="19"/>
+    </row>
+    <row r="231" spans="1:8" ht="75" customHeight="1">
+      <c r="A231" s="13" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B231" s="18" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C231" s="67" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D231" s="19" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E231" s="19" t="s">
         <v>1131</v>
       </c>
-      <c r="D230" s="19" t="s">
-        <v>1130</v>
-      </c>
-      <c r="E230" s="19" t="s">
-        <v>1132</v>
-      </c>
-      <c r="F230" s="19" t="s">
-        <v>1135</v>
-      </c>
-      <c r="G230" s="68" t="s">
+      <c r="F231" s="19" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G231" s="68" t="s">
         <v>732</v>
       </c>
-      <c r="H230" s="19"/>
-    </row>
-    <row r="231" spans="1:8" ht="68" customHeight="1">
-      <c r="A231" s="13" t="s">
+      <c r="H231" s="19"/>
+    </row>
+    <row r="232" spans="1:8" ht="68" customHeight="1">
+      <c r="A232" s="13" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B232" s="18" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C232" s="19" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D232" s="19" t="s">
         <v>1138</v>
       </c>
-      <c r="B231" s="18" t="s">
-        <v>1141</v>
-      </c>
-      <c r="C231" s="19" t="s">
-        <v>1142</v>
-      </c>
-      <c r="D231" s="19" t="s">
+      <c r="E232" s="19" t="s">
         <v>1139</v>
       </c>
-      <c r="E231" s="19" t="s">
-        <v>1140</v>
-      </c>
-      <c r="F231" s="36"/>
-      <c r="G231" s="55" t="s">
-        <v>733</v>
-      </c>
-      <c r="H231" s="36"/>
-    </row>
-    <row r="232" spans="1:8" ht="71" customHeight="1">
-      <c r="A232" s="13" t="s">
-        <v>881</v>
-      </c>
-      <c r="B232" s="18" t="s">
-        <v>1143</v>
-      </c>
-      <c r="C232" s="36"/>
-      <c r="D232" s="36"/>
-      <c r="E232" s="36"/>
       <c r="F232" s="36"/>
       <c r="G232" s="55" t="s">
-        <v>705</v>
+        <v>733</v>
       </c>
       <c r="H232" s="36"/>
     </row>
-    <row r="233" spans="1:8" ht="84" customHeight="1">
+    <row r="233" spans="1:8" ht="71" customHeight="1">
       <c r="A233" s="13" t="s">
-        <v>890</v>
+        <v>881</v>
       </c>
       <c r="B233" s="18" t="s">
-        <v>1145</v>
-      </c>
-      <c r="C233" s="19" t="s">
-        <v>1144</v>
-      </c>
+        <v>1142</v>
+      </c>
+      <c r="C233" s="36"/>
       <c r="D233" s="36"/>
       <c r="E233" s="36"/>
       <c r="F233" s="36"/>
       <c r="G233" s="55" t="s">
-        <v>726</v>
+        <v>705</v>
       </c>
       <c r="H233" s="36"/>
     </row>
-    <row r="234" spans="1:8" ht="74" customHeight="1">
+    <row r="234" spans="1:8" ht="84" customHeight="1">
       <c r="A234" s="13" t="s">
-        <v>1146</v>
+        <v>890</v>
       </c>
       <c r="B234" s="18" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="C234" s="19" t="s">
-        <v>1148</v>
-      </c>
-      <c r="D234" s="19" t="s">
-        <v>1150</v>
-      </c>
+        <v>1143</v>
+      </c>
+      <c r="D234" s="36"/>
       <c r="E234" s="36"/>
       <c r="F234" s="36"/>
-      <c r="G234" s="52" t="s">
+      <c r="G234" s="55" t="s">
+        <v>726</v>
+      </c>
+      <c r="H234" s="36"/>
+    </row>
+    <row r="235" spans="1:8" ht="74" customHeight="1">
+      <c r="A235" s="13" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B235" s="18" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C235" s="19" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D235" s="19" t="s">
         <v>1149</v>
       </c>
-      <c r="H234" s="36"/>
-    </row>
-    <row r="235" spans="1:8" ht="70" customHeight="1">
-      <c r="A235" s="13" t="s">
-        <v>877</v>
-      </c>
-      <c r="B235" s="41"/>
-      <c r="C235" s="36"/>
-      <c r="D235" s="36"/>
       <c r="E235" s="36"/>
       <c r="F235" s="36"/>
-      <c r="G235" s="37" t="s">
-        <v>700</v>
+      <c r="G235" s="52" t="s">
+        <v>1148</v>
       </c>
       <c r="H235" s="36"/>
     </row>
-    <row r="236" spans="1:8" ht="63" customHeight="1">
+    <row r="236" spans="1:8" ht="70" customHeight="1">
       <c r="A236" s="13" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="B236" s="41"/>
       <c r="C236" s="36"/>
       <c r="D236" s="36"/>
       <c r="E236" s="36"/>
       <c r="F236" s="36"/>
-      <c r="G236" s="20" t="s">
-        <v>691</v>
+      <c r="G236" s="37" t="s">
+        <v>700</v>
       </c>
       <c r="H236" s="36"/>
     </row>
-    <row r="237" spans="1:8" ht="70" customHeight="1">
+    <row r="237" spans="1:8" ht="63" customHeight="1">
       <c r="A237" s="13" t="s">
-        <v>882</v>
+        <v>872</v>
       </c>
       <c r="B237" s="41"/>
       <c r="C237" s="36"/>
       <c r="D237" s="36"/>
       <c r="E237" s="36"/>
       <c r="F237" s="36"/>
-      <c r="G237" s="37" t="s">
-        <v>707</v>
+      <c r="G237" s="20" t="s">
+        <v>691</v>
       </c>
       <c r="H237" s="36"/>
     </row>
-    <row r="238" spans="1:8" ht="60" customHeight="1">
+    <row r="238" spans="1:8" ht="70" customHeight="1">
       <c r="A238" s="13" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B238" s="41"/>
       <c r="C238" s="36"/>
@@ -11602,13 +11641,13 @@
       <c r="E238" s="36"/>
       <c r="F238" s="36"/>
       <c r="G238" s="37" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H238" s="36"/>
     </row>
-    <row r="239" spans="1:8" ht="66" customHeight="1">
+    <row r="239" spans="1:8" ht="60" customHeight="1">
       <c r="A239" s="13" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B239" s="41"/>
       <c r="C239" s="36"/>
@@ -11616,405 +11655,409 @@
       <c r="E239" s="36"/>
       <c r="F239" s="36"/>
       <c r="G239" s="37" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="H239" s="36"/>
     </row>
-    <row r="240" spans="1:8" ht="68" customHeight="1">
+    <row r="240" spans="1:8" ht="66" customHeight="1">
       <c r="A240" s="13" t="s">
-        <v>884</v>
-      </c>
-      <c r="B240" s="18" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C240" s="19" t="s">
-        <v>1137</v>
-      </c>
+        <v>885</v>
+      </c>
+      <c r="B240" s="41"/>
+      <c r="C240" s="36"/>
       <c r="D240" s="36"/>
       <c r="E240" s="36"/>
       <c r="F240" s="36"/>
-      <c r="G240" s="19" t="s">
-        <v>715</v>
+      <c r="G240" s="37" t="s">
+        <v>716</v>
       </c>
       <c r="H240" s="36"/>
     </row>
-    <row r="241" spans="1:8" ht="69" customHeight="1">
+    <row r="241" spans="1:8" ht="68" customHeight="1">
       <c r="A241" s="13" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B241" s="18" t="s">
-        <v>717</v>
-      </c>
-      <c r="C241" s="36"/>
+        <v>1135</v>
+      </c>
+      <c r="C241" s="19" t="s">
+        <v>1136</v>
+      </c>
       <c r="D241" s="36"/>
       <c r="E241" s="36"/>
       <c r="F241" s="36"/>
-      <c r="G241" s="37" t="s">
-        <v>718</v>
+      <c r="G241" s="19" t="s">
+        <v>715</v>
       </c>
       <c r="H241" s="36"/>
     </row>
-    <row r="242" spans="1:8" ht="65" customHeight="1">
+    <row r="242" spans="1:8" ht="69" customHeight="1">
       <c r="A242" s="13" t="s">
-        <v>889</v>
-      </c>
-      <c r="B242" s="35" t="s">
-        <v>724</v>
-      </c>
-      <c r="C242" s="37" t="s">
-        <v>725</v>
-      </c>
+        <v>886</v>
+      </c>
+      <c r="B242" s="18" t="s">
+        <v>717</v>
+      </c>
+      <c r="C242" s="36"/>
       <c r="D242" s="36"/>
       <c r="E242" s="36"/>
       <c r="F242" s="36"/>
       <c r="G242" s="37" t="s">
+        <v>718</v>
+      </c>
+      <c r="H242" s="36"/>
+    </row>
+    <row r="243" spans="1:8" ht="65" customHeight="1">
+      <c r="A243" s="13" t="s">
+        <v>889</v>
+      </c>
+      <c r="B243" s="35" t="s">
+        <v>724</v>
+      </c>
+      <c r="C243" s="37" t="s">
+        <v>725</v>
+      </c>
+      <c r="D243" s="36"/>
+      <c r="E243" s="36"/>
+      <c r="F243" s="36"/>
+      <c r="G243" s="37" t="s">
         <v>723</v>
       </c>
-      <c r="H242" s="36"/>
-    </row>
-    <row r="243" spans="1:8" ht="55" customHeight="1">
-      <c r="A243" s="13" t="s">
+      <c r="H243" s="36"/>
+    </row>
+    <row r="244" spans="1:8" ht="55" customHeight="1">
+      <c r="A244" s="13" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B244" s="18" t="s">
+        <v>741</v>
+      </c>
+      <c r="C244" s="19" t="s">
+        <v>739</v>
+      </c>
+      <c r="D244" s="43" t="s">
+        <v>740</v>
+      </c>
+      <c r="E244" s="44"/>
+      <c r="F244" s="44"/>
+      <c r="G244" s="37" t="s">
+        <v>738</v>
+      </c>
+      <c r="H244" s="44"/>
+    </row>
+    <row r="245" spans="1:8" ht="71" customHeight="1">
+      <c r="A245" s="13" t="s">
         <v>1040</v>
       </c>
-      <c r="B243" s="18" t="s">
-        <v>741</v>
-      </c>
-      <c r="C243" s="19" t="s">
-        <v>739</v>
-      </c>
-      <c r="D243" s="43" t="s">
-        <v>740</v>
-      </c>
-      <c r="E243" s="44"/>
-      <c r="F243" s="44"/>
-      <c r="G243" s="37" t="s">
-        <v>738</v>
-      </c>
-      <c r="H243" s="44"/>
-    </row>
-    <row r="244" spans="1:8" ht="71" customHeight="1">
-      <c r="A244" s="13" t="s">
+      <c r="B245" s="18" t="s">
+        <v>893</v>
+      </c>
+      <c r="C245" s="36"/>
+      <c r="D245" s="44"/>
+      <c r="E245" s="44"/>
+      <c r="F245" s="43" t="s">
+        <v>743</v>
+      </c>
+      <c r="G245" s="19" t="s">
+        <v>744</v>
+      </c>
+      <c r="H245" s="44"/>
+    </row>
+    <row r="246" spans="1:8" ht="43" customHeight="1">
+      <c r="A246" s="13" t="s">
         <v>1041</v>
       </c>
-      <c r="B244" s="18" t="s">
-        <v>893</v>
-      </c>
-      <c r="C244" s="36"/>
-      <c r="D244" s="44"/>
-      <c r="E244" s="44"/>
-      <c r="F244" s="43" t="s">
-        <v>743</v>
-      </c>
-      <c r="G244" s="19" t="s">
-        <v>744</v>
-      </c>
-      <c r="H244" s="44"/>
-    </row>
-    <row r="245" spans="1:8" ht="43" customHeight="1">
-      <c r="A245" s="13" t="s">
-        <v>1042</v>
-      </c>
-      <c r="B245" s="35" t="s">
+      <c r="B246" s="35" t="s">
         <v>749</v>
       </c>
-      <c r="C245" s="19" t="s">
+      <c r="C246" s="19" t="s">
         <v>746</v>
       </c>
-      <c r="D245" s="45" t="s">
+      <c r="D246" s="45" t="s">
         <v>747</v>
-      </c>
-      <c r="E245" s="44"/>
-      <c r="F245" s="44"/>
-      <c r="G245" s="37" t="s">
-        <v>748</v>
-      </c>
-      <c r="H245" s="44"/>
-    </row>
-    <row r="246" spans="1:8" ht="97" customHeight="1">
-      <c r="A246" s="13" t="s">
-        <v>751</v>
-      </c>
-      <c r="B246" s="35" t="s">
-        <v>752</v>
-      </c>
-      <c r="C246" s="19" t="s">
-        <v>753</v>
-      </c>
-      <c r="D246" s="45" t="s">
-        <v>755</v>
       </c>
       <c r="E246" s="44"/>
       <c r="F246" s="44"/>
       <c r="G246" s="37" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="H246" s="44"/>
     </row>
-    <row r="247" spans="1:8" ht="63" customHeight="1">
+    <row r="247" spans="1:8" ht="97" customHeight="1">
       <c r="A247" s="13" t="s">
-        <v>1043</v>
-      </c>
-      <c r="B247" s="18" t="s">
-        <v>757</v>
+        <v>751</v>
+      </c>
+      <c r="B247" s="35" t="s">
+        <v>752</v>
       </c>
       <c r="C247" s="19" t="s">
-        <v>894</v>
-      </c>
-      <c r="D247" s="44"/>
+        <v>753</v>
+      </c>
+      <c r="D247" s="45" t="s">
+        <v>755</v>
+      </c>
       <c r="E247" s="44"/>
       <c r="F247" s="44"/>
       <c r="G247" s="37" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="H247" s="44"/>
     </row>
-    <row r="248" spans="1:8" ht="57" customHeight="1">
+    <row r="248" spans="1:8" ht="63" customHeight="1">
       <c r="A248" s="13" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="B248" s="18" t="s">
-        <v>758</v>
-      </c>
-      <c r="C248" s="37" t="s">
-        <v>760</v>
+        <v>757</v>
+      </c>
+      <c r="C248" s="19" t="s">
+        <v>894</v>
       </c>
       <c r="D248" s="44"/>
       <c r="E248" s="44"/>
       <c r="F248" s="44"/>
       <c r="G248" s="37" t="s">
+        <v>756</v>
+      </c>
+      <c r="H248" s="44"/>
+    </row>
+    <row r="249" spans="1:8" ht="57" customHeight="1">
+      <c r="A249" s="13" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B249" s="18" t="s">
+        <v>758</v>
+      </c>
+      <c r="C249" s="37" t="s">
+        <v>760</v>
+      </c>
+      <c r="D249" s="44"/>
+      <c r="E249" s="44"/>
+      <c r="F249" s="44"/>
+      <c r="G249" s="37" t="s">
         <v>759</v>
       </c>
-      <c r="H248" s="44"/>
-    </row>
-    <row r="249" spans="1:8" ht="69" customHeight="1">
-      <c r="A249" s="13" t="s">
+      <c r="H249" s="44"/>
+    </row>
+    <row r="250" spans="1:8" ht="69" customHeight="1">
+      <c r="A250" s="13" t="s">
         <v>895</v>
       </c>
-      <c r="B249" s="18" t="s">
+      <c r="B250" s="18" t="s">
         <v>762</v>
       </c>
-      <c r="C249" s="19" t="s">
+      <c r="C250" s="19" t="s">
         <v>763</v>
       </c>
-      <c r="D249" s="19" t="s">
+      <c r="D250" s="19" t="s">
         <v>765</v>
       </c>
-      <c r="E249" s="19" t="s">
+      <c r="E250" s="19" t="s">
         <v>764</v>
       </c>
-      <c r="F249" s="19" t="s">
+      <c r="F250" s="19" t="s">
         <v>766</v>
       </c>
-      <c r="G249" s="19" t="s">
+      <c r="G250" s="19" t="s">
         <v>761</v>
       </c>
-      <c r="H249" s="44"/>
-    </row>
-    <row r="250" spans="1:8" ht="101" customHeight="1">
-      <c r="A250" s="13" t="s">
+      <c r="H250" s="44"/>
+    </row>
+    <row r="251" spans="1:8" ht="101" customHeight="1">
+      <c r="A251" s="13" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B251" s="35" t="s">
+        <v>768</v>
+      </c>
+      <c r="C251" s="19" t="s">
+        <v>769</v>
+      </c>
+      <c r="D251" s="19" t="s">
+        <v>770</v>
+      </c>
+      <c r="E251" s="44"/>
+      <c r="F251" s="44"/>
+      <c r="G251" s="37" t="s">
+        <v>767</v>
+      </c>
+      <c r="H251" s="44"/>
+    </row>
+    <row r="252" spans="1:8" s="4" customFormat="1" ht="72" customHeight="1">
+      <c r="A252" s="13" t="s">
         <v>1045</v>
       </c>
-      <c r="B250" s="35" t="s">
-        <v>768</v>
-      </c>
-      <c r="C250" s="19" t="s">
-        <v>769</v>
-      </c>
-      <c r="D250" s="19" t="s">
-        <v>770</v>
-      </c>
-      <c r="E250" s="44"/>
-      <c r="F250" s="44"/>
-      <c r="G250" s="37" t="s">
-        <v>767</v>
-      </c>
-      <c r="H250" s="44"/>
-    </row>
-    <row r="251" spans="1:8" s="4" customFormat="1" ht="72" customHeight="1">
-      <c r="A251" s="13" t="s">
+      <c r="B252" s="18" t="s">
+        <v>771</v>
+      </c>
+      <c r="C252" s="19" t="s">
+        <v>772</v>
+      </c>
+      <c r="D252" s="43" t="s">
+        <v>774</v>
+      </c>
+      <c r="E252" s="43"/>
+      <c r="F252" s="43" t="s">
+        <v>1103</v>
+      </c>
+      <c r="G252" s="20" t="s">
+        <v>773</v>
+      </c>
+      <c r="H252" s="43"/>
+    </row>
+    <row r="253" spans="1:8" s="4" customFormat="1" ht="54" customHeight="1">
+      <c r="A253" s="13" t="s">
         <v>1046</v>
       </c>
-      <c r="B251" s="18" t="s">
-        <v>771</v>
-      </c>
-      <c r="C251" s="19" t="s">
-        <v>772</v>
-      </c>
-      <c r="D251" s="43" t="s">
-        <v>774</v>
-      </c>
-      <c r="E251" s="43"/>
-      <c r="F251" s="43" t="s">
-        <v>1104</v>
-      </c>
-      <c r="G251" s="20" t="s">
-        <v>773</v>
-      </c>
-      <c r="H251" s="43"/>
-    </row>
-    <row r="252" spans="1:8" s="4" customFormat="1" ht="54" customHeight="1">
-      <c r="A252" s="13" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B252" s="18" t="s">
+      <c r="B253" s="18" t="s">
         <v>778</v>
       </c>
-      <c r="C252" s="19" t="s">
+      <c r="C253" s="19" t="s">
         <v>777</v>
       </c>
-      <c r="D252" s="43"/>
-      <c r="E252" s="43"/>
-      <c r="F252" s="43"/>
-      <c r="G252" s="20" t="s">
+      <c r="D253" s="43"/>
+      <c r="E253" s="43"/>
+      <c r="F253" s="43"/>
+      <c r="G253" s="20" t="s">
         <v>776</v>
       </c>
-      <c r="H252" s="43"/>
-    </row>
-    <row r="253" spans="1:8" ht="75" customHeight="1">
-      <c r="A253" s="13" t="s">
+      <c r="H253" s="43"/>
+    </row>
+    <row r="254" spans="1:8" ht="75" customHeight="1">
+      <c r="A254" s="13" t="s">
         <v>787</v>
       </c>
-      <c r="B253" s="18" t="s">
+      <c r="B254" s="18" t="s">
         <v>780</v>
       </c>
-      <c r="C253" s="36"/>
-      <c r="D253" s="44"/>
-      <c r="E253" s="44"/>
-      <c r="F253" s="44"/>
-      <c r="G253" s="37" t="s">
+      <c r="C254" s="36"/>
+      <c r="D254" s="44"/>
+      <c r="E254" s="44"/>
+      <c r="F254" s="44"/>
+      <c r="G254" s="37" t="s">
         <v>779</v>
       </c>
-      <c r="H253" s="44"/>
-    </row>
-    <row r="254" spans="1:8" s="4" customFormat="1" ht="66" customHeight="1">
-      <c r="A254" s="13" t="s">
+      <c r="H254" s="44"/>
+    </row>
+    <row r="255" spans="1:8" s="4" customFormat="1" ht="66" customHeight="1">
+      <c r="A255" s="13" t="s">
         <v>788</v>
       </c>
-      <c r="B254" s="18" t="s">
+      <c r="B255" s="18" t="s">
         <v>782</v>
       </c>
-      <c r="C254" s="19"/>
-      <c r="D254" s="43"/>
-      <c r="E254" s="43"/>
-      <c r="F254" s="43"/>
-      <c r="G254" s="19" t="s">
+      <c r="C255" s="19"/>
+      <c r="D255" s="43"/>
+      <c r="E255" s="43"/>
+      <c r="F255" s="43"/>
+      <c r="G255" s="19" t="s">
         <v>781</v>
       </c>
-      <c r="H254" s="43"/>
-    </row>
-    <row r="255" spans="1:8" s="3" customFormat="1" ht="42" customHeight="1">
-      <c r="A255" s="14" t="s">
+      <c r="H255" s="43"/>
+    </row>
+    <row r="256" spans="1:8" s="3" customFormat="1" ht="42" customHeight="1">
+      <c r="A256" s="14" t="s">
         <v>789</v>
       </c>
-      <c r="B255" s="18" t="s">
+      <c r="B256" s="18" t="s">
         <v>784</v>
       </c>
-      <c r="C255" s="37"/>
-      <c r="D255" s="45"/>
-      <c r="E255" s="45"/>
-      <c r="F255" s="45"/>
-      <c r="G255" s="37" t="s">
+      <c r="C256" s="37"/>
+      <c r="D256" s="45"/>
+      <c r="E256" s="45"/>
+      <c r="F256" s="45"/>
+      <c r="G256" s="37" t="s">
         <v>783</v>
       </c>
-      <c r="H255" s="45"/>
-    </row>
-    <row r="256" spans="1:8" ht="48" customHeight="1">
-      <c r="A256" s="13" t="s">
+      <c r="H256" s="45"/>
+    </row>
+    <row r="257" spans="1:8" ht="48" customHeight="1">
+      <c r="A257" s="13" t="s">
         <v>790</v>
       </c>
-      <c r="B256" s="18" t="s">
+      <c r="B257" s="18" t="s">
         <v>651</v>
       </c>
-      <c r="C256" s="19" t="s">
+      <c r="C257" s="19" t="s">
         <v>786</v>
       </c>
-      <c r="D256" s="36"/>
-      <c r="E256" s="36"/>
-      <c r="F256" s="36"/>
-      <c r="G256" s="19" t="s">
+      <c r="D257" s="36"/>
+      <c r="E257" s="36"/>
+      <c r="F257" s="36"/>
+      <c r="G257" s="19" t="s">
         <v>650</v>
       </c>
-      <c r="H256" s="36"/>
-    </row>
-    <row r="257" spans="1:8" s="4" customFormat="1" ht="89" customHeight="1">
-      <c r="A257" s="13" t="s">
+      <c r="H257" s="36"/>
+    </row>
+    <row r="258" spans="1:8" s="4" customFormat="1" ht="89" customHeight="1">
+      <c r="A258" s="13" t="s">
         <v>791</v>
       </c>
-      <c r="B257" s="18" t="s">
+      <c r="B258" s="18" t="s">
         <v>896</v>
       </c>
-      <c r="C257" s="19" t="s">
+      <c r="C258" s="19" t="s">
         <v>897</v>
       </c>
-      <c r="D257" s="43" t="s">
+      <c r="D258" s="43" t="s">
         <v>898</v>
       </c>
-      <c r="E257" s="43"/>
-      <c r="F257" s="43"/>
-      <c r="G257" s="19" t="s">
+      <c r="E258" s="43"/>
+      <c r="F258" s="43"/>
+      <c r="G258" s="19" t="s">
         <v>785</v>
       </c>
-      <c r="H257" s="43"/>
-    </row>
-    <row r="258" spans="1:8" s="3" customFormat="1" ht="64" customHeight="1">
-      <c r="A258" s="13" t="s">
-        <v>1050</v>
-      </c>
-      <c r="B258" s="11" t="s">
+      <c r="H258" s="43"/>
+    </row>
+    <row r="259" spans="1:8" s="3" customFormat="1" ht="64" customHeight="1">
+      <c r="A259" s="13" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B259" s="11" t="s">
         <v>909</v>
       </c>
-      <c r="C258" s="6" t="s">
+      <c r="C259" s="6" t="s">
         <v>910</v>
       </c>
-      <c r="D258" s="49"/>
-      <c r="E258" s="49"/>
-      <c r="F258" s="49"/>
-      <c r="G258" s="6" t="s">
+      <c r="D259" s="49"/>
+      <c r="E259" s="49"/>
+      <c r="F259" s="49"/>
+      <c r="G259" s="6" t="s">
         <v>911</v>
       </c>
-      <c r="H258" s="49"/>
-    </row>
-    <row r="259" spans="1:8" ht="43" customHeight="1">
-      <c r="A259" s="13" t="s">
-        <v>960</v>
-      </c>
-      <c r="B259" s="8"/>
-      <c r="C259" s="5"/>
-      <c r="D259" s="1"/>
-      <c r="E259" s="1"/>
-      <c r="F259" s="1"/>
-      <c r="G259" s="49" t="s">
-        <v>1151</v>
-      </c>
-      <c r="H259" s="1"/>
-    </row>
-    <row r="260" spans="1:8" ht="36" customHeight="1">
+      <c r="H259" s="49"/>
+    </row>
+    <row r="260" spans="1:8" ht="59" customHeight="1">
       <c r="A260" s="13" t="s">
-        <v>958</v>
-      </c>
-      <c r="B260" s="8"/>
+        <v>1154</v>
+      </c>
+      <c r="B260" s="70" t="s">
+        <v>1155</v>
+      </c>
       <c r="C260" s="5"/>
       <c r="D260" s="1"/>
       <c r="E260" s="1"/>
       <c r="F260" s="1"/>
-      <c r="G260" s="5"/>
+      <c r="G260" s="52" t="s">
+        <v>1152</v>
+      </c>
       <c r="H260" s="1"/>
     </row>
-    <row r="261" spans="1:8" ht="46" customHeight="1">
-      <c r="A261" s="13" t="s">
-        <v>959</v>
-      </c>
-      <c r="B261" s="8"/>
-      <c r="C261" s="5"/>
-      <c r="D261" s="1"/>
-      <c r="E261" s="1"/>
-      <c r="F261" s="1"/>
-      <c r="G261" s="5"/>
-      <c r="H261" s="1"/>
-    </row>
-    <row r="262" spans="1:8" ht="30" customHeight="1">
+    <row r="261" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
+      <c r="A261" s="14" t="s">
+        <v>968</v>
+      </c>
+      <c r="B261" s="57"/>
+      <c r="C261" s="49"/>
+      <c r="D261" s="49"/>
+      <c r="E261" s="49"/>
+      <c r="F261" s="49"/>
+      <c r="G261" s="49"/>
+      <c r="H261" s="49"/>
+    </row>
+    <row r="262" spans="1:8" ht="46" customHeight="1">
       <c r="A262" s="13" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="B262" s="8"/>
       <c r="C262" s="5"/>
@@ -12024,9 +12067,9 @@
       <c r="G262" s="5"/>
       <c r="H262" s="1"/>
     </row>
-    <row r="263" spans="1:8" ht="25" customHeight="1">
-      <c r="A263" s="14" t="s">
-        <v>962</v>
+    <row r="263" spans="1:8" ht="30" customHeight="1">
+      <c r="A263" s="13" t="s">
+        <v>960</v>
       </c>
       <c r="B263" s="8"/>
       <c r="C263" s="5"/>
@@ -12036,9 +12079,9 @@
       <c r="G263" s="5"/>
       <c r="H263" s="1"/>
     </row>
-    <row r="264" spans="1:8" ht="39" customHeight="1">
-      <c r="A264" s="13" t="s">
-        <v>963</v>
+    <row r="264" spans="1:8" ht="25" customHeight="1">
+      <c r="A264" s="14" t="s">
+        <v>961</v>
       </c>
       <c r="B264" s="8"/>
       <c r="C264" s="5"/>
@@ -12048,9 +12091,9 @@
       <c r="G264" s="5"/>
       <c r="H264" s="1"/>
     </row>
-    <row r="265" spans="1:8" ht="29" customHeight="1">
-      <c r="A265" s="14" t="s">
-        <v>964</v>
+    <row r="265" spans="1:8" ht="39" customHeight="1">
+      <c r="A265" s="13" t="s">
+        <v>962</v>
       </c>
       <c r="B265" s="8"/>
       <c r="C265" s="5"/>
@@ -12060,9 +12103,9 @@
       <c r="G265" s="5"/>
       <c r="H265" s="1"/>
     </row>
-    <row r="266" spans="1:8" ht="23" customHeight="1">
+    <row r="266" spans="1:8" ht="29" customHeight="1">
       <c r="A266" s="14" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="B266" s="8"/>
       <c r="C266" s="5"/>
@@ -12072,9 +12115,9 @@
       <c r="G266" s="5"/>
       <c r="H266" s="1"/>
     </row>
-    <row r="267" spans="1:8" ht="22" customHeight="1">
+    <row r="267" spans="1:8" ht="23" customHeight="1">
       <c r="A267" s="14" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="B267" s="8"/>
       <c r="C267" s="5"/>
@@ -12084,21 +12127,21 @@
       <c r="G267" s="5"/>
       <c r="H267" s="1"/>
     </row>
-    <row r="268" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
+    <row r="268" spans="1:8" ht="22" customHeight="1">
       <c r="A268" s="14" t="s">
-        <v>967</v>
-      </c>
-      <c r="B268" s="57"/>
-      <c r="C268" s="49"/>
-      <c r="D268" s="49"/>
-      <c r="E268" s="49"/>
-      <c r="F268" s="49"/>
-      <c r="G268" s="49"/>
-      <c r="H268" s="49"/>
+        <v>965</v>
+      </c>
+      <c r="B268" s="8"/>
+      <c r="C268" s="5"/>
+      <c r="D268" s="1"/>
+      <c r="E268" s="1"/>
+      <c r="F268" s="1"/>
+      <c r="G268" s="5"/>
+      <c r="H268" s="1"/>
     </row>
     <row r="269" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A269" s="14" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="B269" s="57"/>
       <c r="C269" s="49"/>
@@ -12110,7 +12153,7 @@
     </row>
     <row r="270" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A270" s="14" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="B270" s="57"/>
       <c r="C270" s="49"/>
@@ -12122,10 +12165,10 @@
     </row>
     <row r="271" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A271" s="14" t="s">
+        <v>969</v>
+      </c>
+      <c r="B271" s="57" t="s">
         <v>970</v>
-      </c>
-      <c r="B271" s="57" t="s">
-        <v>971</v>
       </c>
       <c r="C271" s="49"/>
       <c r="D271" s="49"/>
@@ -12136,7 +12179,7 @@
     </row>
     <row r="272" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A272" s="14" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B272" s="57"/>
       <c r="C272" s="49"/>
@@ -12148,7 +12191,7 @@
     </row>
     <row r="273" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A273" s="14" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B273" s="57"/>
       <c r="C273" s="49"/>
@@ -12160,7 +12203,7 @@
     </row>
     <row r="274" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A274" s="14" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B274" s="57"/>
       <c r="C274" s="49"/>
@@ -12172,10 +12215,10 @@
     </row>
     <row r="275" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A275" s="14" t="s">
+        <v>974</v>
+      </c>
+      <c r="B275" s="57" t="s">
         <v>975</v>
-      </c>
-      <c r="B275" s="57" t="s">
-        <v>976</v>
       </c>
       <c r="C275" s="49"/>
       <c r="D275" s="49"/>
@@ -12186,7 +12229,7 @@
     </row>
     <row r="276" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A276" s="14" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B276" s="57"/>
       <c r="C276" s="49"/>
@@ -12198,7 +12241,7 @@
     </row>
     <row r="277" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A277" s="14" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B277" s="57"/>
       <c r="C277" s="49"/>
@@ -12210,7 +12253,7 @@
     </row>
     <row r="278" spans="1:8" s="58" customFormat="1" ht="21" customHeight="1">
       <c r="A278" s="14" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B278" s="57"/>
       <c r="C278" s="49"/>
@@ -12222,7 +12265,7 @@
     </row>
     <row r="279" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A279" s="14" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B279" s="57"/>
       <c r="C279" s="49"/>
@@ -12234,7 +12277,7 @@
     </row>
     <row r="280" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A280" s="14" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B280" s="57"/>
       <c r="C280" s="49"/>
@@ -12246,7 +12289,7 @@
     </row>
     <row r="281" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A281" s="14" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B281" s="57"/>
       <c r="C281" s="49"/>
@@ -12258,7 +12301,7 @@
     </row>
     <row r="282" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A282" s="14" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B282" s="57"/>
       <c r="C282" s="49"/>
@@ -12270,7 +12313,7 @@
     </row>
     <row r="283" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A283" s="14" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B283" s="57"/>
       <c r="C283" s="49"/>
@@ -12296,7 +12339,7 @@
     </row>
     <row r="285" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A285" s="14" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B285" s="57"/>
       <c r="C285" s="49"/>
@@ -12308,7 +12351,7 @@
     </row>
     <row r="286" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A286" s="14" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B286" s="57"/>
       <c r="C286" s="49"/>
@@ -12320,7 +12363,7 @@
     </row>
     <row r="287" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A287" s="14" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B287" s="57"/>
       <c r="C287" s="49"/>
@@ -12332,29 +12375,29 @@
     </row>
     <row r="288" spans="1:8" s="58" customFormat="1" ht="53" customHeight="1">
       <c r="A288" s="14" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B288" s="63" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="C288" s="64"/>
       <c r="D288" s="49"/>
       <c r="E288" s="49"/>
       <c r="F288" s="49"/>
       <c r="G288" s="6" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="H288" s="49"/>
     </row>
     <row r="289" spans="1:8" s="58" customFormat="1" ht="71" customHeight="1">
       <c r="A289" s="14" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B289" s="63" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C289" s="65" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="D289" s="49"/>
       <c r="E289" s="49"/>
@@ -12364,43 +12407,43 @@
     </row>
     <row r="290" spans="1:8" s="58" customFormat="1" ht="74" customHeight="1">
       <c r="A290" s="14" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B290" s="63" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="C290" s="67" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D290" s="49"/>
       <c r="E290" s="49"/>
       <c r="F290" s="49"/>
       <c r="G290" s="49" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="H290" s="49"/>
     </row>
     <row r="291" spans="1:8" s="58" customFormat="1" ht="74" customHeight="1">
       <c r="A291" s="66" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B291" s="18" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C291" s="67" t="s">
         <v>1080</v>
-      </c>
-      <c r="C291" s="67" t="s">
-        <v>1081</v>
       </c>
       <c r="D291" s="49"/>
       <c r="E291" s="49"/>
       <c r="F291" s="49"/>
       <c r="G291" s="55" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="H291" s="49"/>
     </row>
     <row r="292" spans="1:8" s="58" customFormat="1" ht="34" customHeight="1">
       <c r="A292" s="14" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B292" s="63"/>
       <c r="C292" s="49"/>
@@ -12412,7 +12455,7 @@
     </row>
     <row r="293" spans="1:8" s="58" customFormat="1" ht="43" customHeight="1">
       <c r="A293" s="14" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B293" s="63"/>
       <c r="C293" s="49"/>
@@ -12424,7 +12467,7 @@
     </row>
     <row r="294" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A294" s="14" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B294" s="57"/>
       <c r="C294" s="49"/>
@@ -12436,7 +12479,7 @@
     </row>
     <row r="295" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A295" s="14" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B295" s="57"/>
       <c r="C295" s="49"/>
@@ -12448,7 +12491,7 @@
     </row>
     <row r="296" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A296" s="14" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B296" s="57"/>
       <c r="C296" s="49"/>
@@ -12460,7 +12503,7 @@
     </row>
     <row r="297" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A297" s="14" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B297" s="57"/>
       <c r="C297" s="49"/>
@@ -12472,7 +12515,7 @@
     </row>
     <row r="298" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A298" s="14" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B298" s="57"/>
       <c r="C298" s="49"/>
@@ -12484,7 +12527,7 @@
     </row>
     <row r="299" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A299" s="14" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B299" s="57"/>
       <c r="C299" s="49"/>
@@ -12510,7 +12553,7 @@
     </row>
     <row r="301" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A301" s="14" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B301" s="57"/>
       <c r="C301" s="49"/>
@@ -12522,7 +12565,7 @@
     </row>
     <row r="302" spans="1:8" s="58" customFormat="1" ht="47" customHeight="1">
       <c r="A302" s="13" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B302" s="57"/>
       <c r="C302" s="49"/>
@@ -12534,7 +12577,7 @@
     </row>
     <row r="303" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A303" s="14" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B303" s="57"/>
       <c r="C303" s="49"/>
@@ -12546,7 +12589,7 @@
     </row>
     <row r="304" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A304" s="14" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B304" s="57"/>
       <c r="C304" s="49"/>
@@ -12558,7 +12601,7 @@
     </row>
     <row r="305" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A305" s="14" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B305" s="57"/>
       <c r="C305" s="49"/>
@@ -12570,7 +12613,7 @@
     </row>
     <row r="306" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A306" s="14" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B306" s="57"/>
       <c r="C306" s="49"/>
@@ -12582,7 +12625,7 @@
     </row>
     <row r="307" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A307" s="14" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B307" s="57"/>
       <c r="C307" s="49"/>
@@ -12594,7 +12637,7 @@
     </row>
     <row r="308" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A308" s="14" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B308" s="57"/>
       <c r="C308" s="49"/>
@@ -12606,7 +12649,7 @@
     </row>
     <row r="309" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A309" s="14" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B309" s="57"/>
       <c r="C309" s="49"/>
@@ -12618,7 +12661,7 @@
     </row>
     <row r="310" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A310" s="14" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B310" s="57"/>
       <c r="C310" s="49"/>
@@ -12630,7 +12673,7 @@
     </row>
     <row r="311" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A311" s="14" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B311" s="57"/>
       <c r="C311" s="49"/>
@@ -12642,7 +12685,7 @@
     </row>
     <row r="312" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A312" s="14" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B312" s="57"/>
       <c r="C312" s="49"/>
@@ -12654,7 +12697,7 @@
     </row>
     <row r="313" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A313" s="14" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B313" s="57"/>
       <c r="C313" s="49"/>
@@ -12666,7 +12709,7 @@
     </row>
     <row r="314" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A314" s="14" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B314" s="57"/>
       <c r="C314" s="49"/>
@@ -12678,7 +12721,7 @@
     </row>
     <row r="315" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A315" s="14" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B315" s="57"/>
       <c r="C315" s="49"/>
@@ -12690,7 +12733,7 @@
     </row>
     <row r="316" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A316" s="14" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B316" s="57"/>
       <c r="C316" s="49"/>
@@ -12702,7 +12745,7 @@
     </row>
     <row r="317" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A317" s="14" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B317" s="57"/>
       <c r="C317" s="49"/>
@@ -12714,7 +12757,7 @@
     </row>
     <row r="318" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A318" s="14" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B318" s="57"/>
       <c r="C318" s="49"/>
@@ -12726,7 +12769,7 @@
     </row>
     <row r="319" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A319" s="14" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B319" s="57"/>
       <c r="C319" s="49"/>
@@ -12738,7 +12781,7 @@
     </row>
     <row r="320" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A320" s="14" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B320" s="57"/>
       <c r="C320" s="49"/>
@@ -12750,7 +12793,7 @@
     </row>
     <row r="321" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A321" s="14" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B321" s="57"/>
       <c r="C321" s="49"/>
@@ -12762,7 +12805,7 @@
     </row>
     <row r="322" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A322" s="14" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B322" s="57"/>
       <c r="C322" s="49"/>
@@ -12774,7 +12817,7 @@
     </row>
     <row r="323" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A323" s="14" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B323" s="57"/>
       <c r="C323" s="49"/>
@@ -12786,7 +12829,7 @@
     </row>
     <row r="324" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A324" s="14" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B324" s="57"/>
       <c r="C324" s="49"/>
@@ -12798,7 +12841,7 @@
     </row>
     <row r="325" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A325" s="14" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B325" s="57"/>
       <c r="C325" s="49"/>
@@ -12810,7 +12853,7 @@
     </row>
     <row r="326" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A326" s="14" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B326" s="57"/>
       <c r="C326" s="49"/>
@@ -12822,7 +12865,7 @@
     </row>
     <row r="327" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A327" s="14" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B327" s="57"/>
       <c r="C327" s="49"/>
@@ -12834,7 +12877,7 @@
     </row>
     <row r="328" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A328" s="14" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B328" s="57"/>
       <c r="C328" s="49"/>
@@ -12846,7 +12889,7 @@
     </row>
     <row r="329" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A329" s="14" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B329" s="57"/>
       <c r="C329" s="49"/>
@@ -12858,7 +12901,7 @@
     </row>
     <row r="330" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A330" s="14" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B330" s="57"/>
       <c r="C330" s="49"/>
@@ -12870,7 +12913,7 @@
     </row>
     <row r="331" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A331" s="14" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B331" s="57"/>
       <c r="C331" s="49"/>
@@ -12882,7 +12925,7 @@
     </row>
     <row r="332" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A332" s="14" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B332" s="57"/>
       <c r="C332" s="49"/>
@@ -12894,7 +12937,7 @@
     </row>
     <row r="333" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A333" s="14" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B333" s="57"/>
       <c r="C333" s="49"/>
@@ -12906,7 +12949,7 @@
     </row>
     <row r="334" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A334" s="14" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B334" s="57"/>
       <c r="C334" s="49"/>
@@ -12918,7 +12961,7 @@
     </row>
     <row r="335" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A335" s="14" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B335" s="57"/>
       <c r="C335" s="49"/>
@@ -12930,7 +12973,7 @@
     </row>
     <row r="336" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A336" s="14" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B336" s="35"/>
       <c r="C336" s="37"/>
@@ -12942,7 +12985,7 @@
     </row>
     <row r="337" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A337" s="14" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B337" s="35"/>
       <c r="C337" s="37"/>
@@ -12954,7 +12997,7 @@
     </row>
     <row r="338" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A338" s="14" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B338" s="35"/>
       <c r="C338" s="37"/>
@@ -12966,7 +13009,7 @@
     </row>
     <row r="339" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A339" s="14" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B339" s="35"/>
       <c r="C339" s="37"/>
@@ -12978,7 +13021,7 @@
     </row>
     <row r="340" spans="1:8">
       <c r="A340" s="56" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B340" s="8"/>
       <c r="C340" s="5"/>
@@ -12990,7 +13033,7 @@
     </row>
     <row r="341" spans="1:8">
       <c r="A341" s="56" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B341" s="8"/>
       <c r="C341" s="5"/>
@@ -13002,7 +13045,7 @@
     </row>
     <row r="342" spans="1:8">
       <c r="A342" s="56" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B342" s="8"/>
       <c r="C342" s="5"/>
@@ -13014,7 +13057,7 @@
     </row>
     <row r="343" spans="1:8">
       <c r="A343" s="56" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B343" s="8"/>
       <c r="C343" s="5"/>
@@ -13026,7 +13069,7 @@
     </row>
     <row r="344" spans="1:8">
       <c r="A344" s="56" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B344" s="8"/>
       <c r="C344" s="5"/>
@@ -13038,7 +13081,7 @@
     </row>
     <row r="345" spans="1:8">
       <c r="A345" s="56" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B345" s="8"/>
       <c r="C345" s="5"/>
@@ -13050,7 +13093,7 @@
     </row>
     <row r="346" spans="1:8">
       <c r="A346" s="56" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B346" s="8"/>
       <c r="C346" s="5"/>
@@ -13062,7 +13105,7 @@
     </row>
     <row r="347" spans="1:8">
       <c r="A347" s="56" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B347" s="8"/>
       <c r="C347" s="5"/>
@@ -13616,8 +13659,8 @@
     <hyperlink ref="G208" r:id="rId110" xr:uid="{23D9C103-F2A2-474D-8B3B-C8B3ADAFAF09}"/>
     <hyperlink ref="G209" r:id="rId111" xr:uid="{2401B952-575E-1D45-AF80-42C35916F8A5}"/>
     <hyperlink ref="G212" r:id="rId112" xr:uid="{31219583-F195-ED42-A799-1B054B7D9E84}"/>
-    <hyperlink ref="G251" r:id="rId113" xr:uid="{E7446763-7D68-D94F-887C-EEC8548E4D16}"/>
-    <hyperlink ref="G252" r:id="rId114" xr:uid="{11A405A4-DF58-9545-BCDE-9414DE390A5E}"/>
+    <hyperlink ref="G252" r:id="rId113" xr:uid="{E7446763-7D68-D94F-887C-EEC8548E4D16}"/>
+    <hyperlink ref="G253" r:id="rId114" xr:uid="{11A405A4-DF58-9545-BCDE-9414DE390A5E}"/>
     <hyperlink ref="G142" r:id="rId115" xr:uid="{E5B20948-57A8-2E48-9191-175A672155C6}"/>
     <hyperlink ref="G148" r:id="rId116" xr:uid="{08B7E248-E2F5-4A4A-BAC3-ABDA6CE1A484}"/>
     <hyperlink ref="G161" r:id="rId117" xr:uid="{E597C9B9-B49B-E748-9679-4D7E6A09DF83}"/>
@@ -13632,21 +13675,22 @@
     <hyperlink ref="G190" r:id="rId126" xr:uid="{31FA25FC-46C7-D74A-99A5-1140E96809B5}"/>
     <hyperlink ref="G198" r:id="rId127" xr:uid="{5CC18E71-C5D0-6A4D-AD79-B547613CD77D}"/>
     <hyperlink ref="G291" r:id="rId128" xr:uid="{754094CD-003E-114E-B66D-2DEF0C37F04E}"/>
-    <hyperlink ref="G221" r:id="rId129" xr:uid="{88298BD6-A42F-864A-B628-C970B3D8AF36}"/>
-    <hyperlink ref="G220" r:id="rId130" xr:uid="{9D9B7F12-8E09-F14A-B4B2-B2CC263E87C2}"/>
-    <hyperlink ref="G222" r:id="rId131" xr:uid="{0CC180BE-FEEA-EA49-95EB-93F1AE813670}"/>
-    <hyperlink ref="G223" r:id="rId132" xr:uid="{ACF47BBB-0D42-1849-8E8C-F5374D58E72D}"/>
-    <hyperlink ref="G224" r:id="rId133" xr:uid="{F915674D-C6EE-8A49-BE56-B6E982947AE2}"/>
-    <hyperlink ref="G225" r:id="rId134" xr:uid="{59F0714C-9A83-7D45-94D6-EE6C98DDAA40}"/>
-    <hyperlink ref="G227" r:id="rId135" xr:uid="{0C8EEDA6-B628-FA4E-B83A-1C9AADAC775C}"/>
-    <hyperlink ref="G228" r:id="rId136" xr:uid="{5F7B4D87-E8BA-7148-A5D6-FB61786A1C54}"/>
-    <hyperlink ref="G230" r:id="rId137" xr:uid="{51F23D9B-48FC-4E4D-905C-C274C579A1CA}"/>
-    <hyperlink ref="G231" r:id="rId138" xr:uid="{D16C412B-860F-AC42-B67E-D71B6B8C1E14}"/>
-    <hyperlink ref="G233" r:id="rId139" xr:uid="{7D0AAFC1-C690-2B49-9EB8-E3BA672C2424}"/>
-    <hyperlink ref="G232" r:id="rId140" xr:uid="{A65E0F05-0669-C64B-A8E6-50DC31570000}"/>
-    <hyperlink ref="G234" r:id="rId141" xr:uid="{7D3C258D-3141-A34D-BFE7-93ABAF4EC570}"/>
+    <hyperlink ref="G222" r:id="rId129" xr:uid="{88298BD6-A42F-864A-B628-C970B3D8AF36}"/>
+    <hyperlink ref="G221" r:id="rId130" xr:uid="{9D9B7F12-8E09-F14A-B4B2-B2CC263E87C2}"/>
+    <hyperlink ref="G223" r:id="rId131" xr:uid="{0CC180BE-FEEA-EA49-95EB-93F1AE813670}"/>
+    <hyperlink ref="G224" r:id="rId132" xr:uid="{ACF47BBB-0D42-1849-8E8C-F5374D58E72D}"/>
+    <hyperlink ref="G225" r:id="rId133" xr:uid="{F915674D-C6EE-8A49-BE56-B6E982947AE2}"/>
+    <hyperlink ref="G226" r:id="rId134" xr:uid="{59F0714C-9A83-7D45-94D6-EE6C98DDAA40}"/>
+    <hyperlink ref="G228" r:id="rId135" xr:uid="{0C8EEDA6-B628-FA4E-B83A-1C9AADAC775C}"/>
+    <hyperlink ref="G229" r:id="rId136" xr:uid="{5F7B4D87-E8BA-7148-A5D6-FB61786A1C54}"/>
+    <hyperlink ref="G231" r:id="rId137" xr:uid="{51F23D9B-48FC-4E4D-905C-C274C579A1CA}"/>
+    <hyperlink ref="G232" r:id="rId138" xr:uid="{D16C412B-860F-AC42-B67E-D71B6B8C1E14}"/>
+    <hyperlink ref="G234" r:id="rId139" xr:uid="{7D0AAFC1-C690-2B49-9EB8-E3BA672C2424}"/>
+    <hyperlink ref="G233" r:id="rId140" xr:uid="{A65E0F05-0669-C64B-A8E6-50DC31570000}"/>
+    <hyperlink ref="G235" r:id="rId141" xr:uid="{7D3C258D-3141-A34D-BFE7-93ABAF4EC570}"/>
+    <hyperlink ref="G260" r:id="rId142" xr:uid="{06803B17-EB1A-5741-9E70-F5A8FBBF83C1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId142"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId143"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reverse first k items from queue
</commit_message>
<xml_diff>
--- a/Applications/QuestionListWithApproaches.xlsx
+++ b/Applications/QuestionListWithApproaches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksharkashyap/Documents/VisualStudio/Applications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF6C18D-514B-494A-98B8-DD35E8041A6A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662E464E-72EB-FB45-8B84-BB2C19B91F96}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="460" windowWidth="32600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="1265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="1284">
   <si>
     <t>Convert Binary Number in a Linked List to Integer</t>
   </si>
@@ -5250,9 +5250,6 @@
     <t>Count pairs from 2 BST whose sum is equal to given value "X"</t>
   </si>
   <si>
-    <t>Find the median of BST in O(n) time and O(1) space</t>
-  </si>
-  <si>
     <t>Replace every element with the least greater element on its right</t>
   </si>
   <si>
@@ -5311,9 +5308,6 @@
   </si>
   <si>
     <t>reverse a queue using recursion</t>
-  </si>
-  <si>
-    <t>reverse first K elements of queue</t>
   </si>
   <si>
     <t>First negative integer in every window of size “k”</t>
@@ -5664,9 +5658,6 @@
     <t>n-ary tree postorder traversal (iterative)</t>
   </si>
   <si>
-    <t>morris inorder traversal</t>
-  </si>
-  <si>
     <t>https://www.geeksforgeeks.org/iterative-postorder-traversal-using-stack</t>
   </si>
   <si>
@@ -8033,7 +8024,273 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>] worst case when all the elements of arr2 are less than arr1 (see the last method in gfg link)</t>
+      <t>] worst case when all the elements of arr2 are less than arr1 (see gitlink)</t>
+    </r>
+  </si>
+  <si>
+    <t>https://github.com/aksharkashyap/DSALGO/blob/master/SORTING/MergeTwoSorted.java</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/kth-smallest-element-in-a-bst/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Do inorder traversal return the K'th element of sorted list </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Calibri Light (Headings)_x0000_"/>
+      </rPr>
+      <t>O(n) time and O(n)space</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Iterative inorder(stack) this way one could speed up the solution because there is no need to build the entire inorder traversal, and one could stop after the kth element. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>O(H+k) time and O(H) space</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">previous approach with the help of global Ans and count variable or class [return if Count &gt; k to improve time </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>O(H+k)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve"> [The code first traverses down to the rightmost node which takes O(h) time, then traverses k elements in O(k) time.]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>convert largest to smallest [ K = N - K + 1]</t>
+  </si>
+  <si>
+    <t>do reverse inorder traversal (recurse(right), root, recurse(left))</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/kth-largest-element-in-bst-when-modification-to-bst-is-not-allowed/</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/kth-largest-element-bst-using-constant-extra-space/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reverse Morris inorder traversal </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>O(n) time and O(1) space</t>
+    </r>
+  </si>
+  <si>
+    <t>morris inorder traversal O(1) space [ no recursion or stack used]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">morris inorder traversal </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>O(n) time and O(1) space</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve"> because it doesn’t uses stack or recursion</t>
+    </r>
+  </si>
+  <si>
+    <t>find median of BST in O(n) time and O(1) space</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/find-median-bst-time-o1-space/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">do inorder traversal and keep elements in a List and accordingly return the median </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Calibri Light (Headings)_x0000_"/>
+      </rPr>
+      <t>O(n) time and O(n) space</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">use global variables/class to hold Count and Median, calculate no. of nodes, if even: then median = ((n/2th node + (n+1)/2th node) /2 If odd : then median = (n+1)/2th node  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>O(2n) time and O(H) space</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>morris inorder traversal</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve"> O(n) time and O(1) space</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1)- Count the no. of nodes using morris (2) Perform Morris traversal again by counting nodes and by checking if count is equal to the median point.To consider even no. of nodes an extra pointer pointing to the previous node is used</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/reversing-first-k-elements-queue/</t>
+  </si>
+  <si>
+    <t>sort the queue</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>reverse first K elements of queue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> [ enqueue, dequeue,size and front operation is allowed]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">use 2 aux List, put first K items in list1 and remaining items in list2, now insert from list1 in reverse order and from list 2 as it is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Calibri Light (Headings)_x0000_"/>
+      </rPr>
+      <t>O(n) time and O(n) space</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">use 1 aux stack, push first K items into stack, now offer(back) them into Queue, now poll() remaining N-K items from front and offer() them into Queue </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>O(n) time O(K) space</t>
     </r>
   </si>
 </sst>
@@ -8041,7 +8298,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="53">
+  <fonts count="55">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8388,6 +8645,17 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -8451,7 +8719,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
@@ -8662,6 +8930,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8947,10 +9218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S416"/>
+  <dimension ref="A1:S417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="171" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D266" sqref="D266"/>
+    <sheetView tabSelected="1" topLeftCell="A350" zoomScale="171" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D359" sqref="D359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9272,7 +9543,7 @@
         <v>727</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>
@@ -9301,13 +9572,13 @@
     </row>
     <row r="19" spans="1:8" ht="46" customHeight="1">
       <c r="A19" s="13" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -9317,13 +9588,13 @@
     </row>
     <row r="20" spans="1:8" ht="43" customHeight="1">
       <c r="A20" s="14" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -9333,13 +9604,13 @@
     </row>
     <row r="21" spans="1:8" ht="63" customHeight="1">
       <c r="A21" s="14" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B21" s="61" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="C21" s="62" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -9349,7 +9620,7 @@
     </row>
     <row r="22" spans="1:8" ht="24" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="5"/>
@@ -9361,7 +9632,7 @@
     </row>
     <row r="23" spans="1:8" ht="32" customHeight="1">
       <c r="A23" s="14" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="5"/>
@@ -9373,7 +9644,7 @@
     </row>
     <row r="24" spans="1:8" ht="33" customHeight="1">
       <c r="A24" s="14" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="5"/>
@@ -9385,7 +9656,7 @@
     </row>
     <row r="25" spans="1:8" ht="33" customHeight="1">
       <c r="A25" s="14" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="5"/>
@@ -9397,7 +9668,7 @@
     </row>
     <row r="26" spans="1:8" ht="33" customHeight="1">
       <c r="A26" s="14" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="5"/>
@@ -9409,7 +9680,7 @@
     </row>
     <row r="27" spans="1:8" ht="29" customHeight="1">
       <c r="A27" s="14" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
@@ -10973,7 +11244,7 @@
     </row>
     <row r="112" spans="1:8" ht="28">
       <c r="A112" s="13" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="B112" s="18" t="s">
         <v>320</v>
@@ -10995,7 +11266,7 @@
     </row>
     <row r="113" spans="1:8" ht="50" customHeight="1">
       <c r="A113" s="23" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="B113" s="18" t="s">
         <v>123</v>
@@ -11004,7 +11275,7 @@
         <v>124</v>
       </c>
       <c r="D113" s="19" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="E113" s="19"/>
       <c r="F113" s="19"/>
@@ -11065,7 +11336,7 @@
     </row>
     <row r="117" spans="1:8" s="3" customFormat="1" ht="66" customHeight="1">
       <c r="A117" s="13" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="B117" s="18"/>
       <c r="C117" s="19"/>
@@ -11073,13 +11344,13 @@
       <c r="E117" s="19"/>
       <c r="F117" s="19"/>
       <c r="G117" s="52" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="H117" s="19"/>
     </row>
     <row r="118" spans="1:8" s="3" customFormat="1" ht="80" customHeight="1">
       <c r="A118" s="13" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="B118" s="18" t="s">
         <v>372</v>
@@ -11097,7 +11368,7 @@
     </row>
     <row r="119" spans="1:8" s="3" customFormat="1" ht="80" customHeight="1">
       <c r="A119" s="13" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="B119" s="18"/>
       <c r="C119" s="19"/>
@@ -11109,7 +11380,7 @@
     </row>
     <row r="120" spans="1:8" s="3" customFormat="1" ht="62" customHeight="1">
       <c r="A120" s="13" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="B120" s="18"/>
       <c r="C120" s="19"/>
@@ -11121,7 +11392,7 @@
     </row>
     <row r="121" spans="1:8" s="3" customFormat="1" ht="87" customHeight="1">
       <c r="A121" s="13" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="B121" s="18"/>
       <c r="C121" s="19"/>
@@ -11133,7 +11404,7 @@
     </row>
     <row r="122" spans="1:8" s="3" customFormat="1" ht="80" customHeight="1">
       <c r="A122" s="13" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="B122" s="18"/>
       <c r="C122" s="19"/>
@@ -11916,10 +12187,10 @@
     </row>
     <row r="164" spans="1:8" ht="52" customHeight="1">
       <c r="A164" s="13" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
       <c r="B164" s="70" t="s">
-        <v>1198</v>
+        <v>1195</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>152</v>
@@ -11927,10 +12198,10 @@
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
       <c r="F164" s="54" t="s">
-        <v>1200</v>
+        <v>1197</v>
       </c>
       <c r="G164" s="54" t="s">
-        <v>1199</v>
+        <v>1196</v>
       </c>
       <c r="H164" s="1"/>
     </row>
@@ -12302,17 +12573,17 @@
     </row>
     <row r="184" spans="1:8" ht="46" customHeight="1">
       <c r="A184" s="13" t="s">
-        <v>1203</v>
+        <v>1200</v>
       </c>
       <c r="B184" s="57" t="s">
-        <v>1202</v>
+        <v>1199</v>
       </c>
       <c r="C184" s="5"/>
       <c r="D184" s="1"/>
       <c r="E184" s="1"/>
       <c r="F184" s="1"/>
       <c r="G184" s="52" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="H184" s="1"/>
     </row>
@@ -12830,32 +13101,32 @@
     </row>
     <row r="213" spans="1:8" ht="61" customHeight="1">
       <c r="A213" s="13" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="B213" s="18" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="C213" s="19"/>
       <c r="D213" s="19"/>
       <c r="E213" s="19"/>
       <c r="F213" s="19"/>
       <c r="G213" s="20" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="H213" s="19"/>
     </row>
     <row r="214" spans="1:8" ht="78" customHeight="1">
       <c r="A214" s="13" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="B214" s="35" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="C214" s="19" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="D214" s="19" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="F214" s="36"/>
       <c r="G214" s="40" t="s">
@@ -12868,51 +13139,51 @@
         <v>946</v>
       </c>
       <c r="B215" s="46" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="C215" s="6" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="D215" s="1"/>
       <c r="E215" s="1"/>
       <c r="F215" s="1"/>
       <c r="G215" s="49" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="H215" s="1"/>
     </row>
     <row r="216" spans="1:8" ht="76" customHeight="1">
       <c r="A216" s="13" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="B216" s="18" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="C216" s="36"/>
       <c r="D216" s="36"/>
       <c r="E216" s="36"/>
       <c r="F216" s="36"/>
       <c r="G216" s="40" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="H216" s="36"/>
     </row>
     <row r="217" spans="1:8" ht="83" customHeight="1">
       <c r="A217" s="13" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B217" s="18" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C217" s="39" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D217" s="19" t="s">
         <v>1070</v>
-      </c>
-      <c r="B217" s="18" t="s">
-        <v>1074</v>
-      </c>
-      <c r="C217" s="39" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D217" s="19" t="s">
-        <v>1073</v>
       </c>
       <c r="F217" s="36"/>
       <c r="G217" s="40" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="H217" s="36"/>
     </row>
@@ -12954,10 +13225,10 @@
     </row>
     <row r="220" spans="1:8" ht="63" customHeight="1">
       <c r="A220" s="33" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="B220" s="18" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="C220" s="36"/>
       <c r="D220" s="36"/>
@@ -12970,25 +13241,25 @@
     </row>
     <row r="221" spans="1:8" s="4" customFormat="1" ht="104" customHeight="1">
       <c r="A221" s="32" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="B221" s="18" t="s">
         <v>681</v>
       </c>
       <c r="C221" s="67" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="D221" s="19" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E221" s="38" t="s">
         <v>1078</v>
       </c>
-      <c r="E221" s="38" t="s">
-        <v>1081</v>
-      </c>
       <c r="F221" s="62" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="G221" s="19" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="H221" s="19"/>
     </row>
@@ -13014,22 +13285,22 @@
     </row>
     <row r="223" spans="1:8" ht="96" customHeight="1">
       <c r="A223" s="13" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B223" s="35" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C223" s="19" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D223" s="19" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E223" s="39" t="s">
         <v>1084</v>
       </c>
-      <c r="B223" s="35" t="s">
-        <v>1085</v>
-      </c>
-      <c r="C223" s="19" t="s">
+      <c r="F223" s="19" t="s">
         <v>1086</v>
-      </c>
-      <c r="D223" s="19" t="s">
-        <v>1088</v>
-      </c>
-      <c r="E223" s="39" t="s">
-        <v>1087</v>
-      </c>
-      <c r="F223" s="19" t="s">
-        <v>1089</v>
       </c>
       <c r="G223" s="68" t="s">
         <v>697</v>
@@ -13041,13 +13312,13 @@
         <v>868</v>
       </c>
       <c r="B224" s="18" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="C224" s="19" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="D224" s="19" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="E224" s="19"/>
       <c r="F224" s="36"/>
@@ -13058,16 +13329,16 @@
     </row>
     <row r="225" spans="1:8" ht="79" customHeight="1">
       <c r="A225" s="13" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
       <c r="B225" s="18" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C225" s="19" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D225" s="69" t="s">
         <v>1093</v>
-      </c>
-      <c r="C225" s="19" t="s">
-        <v>1095</v>
-      </c>
-      <c r="D225" s="69" t="s">
-        <v>1096</v>
       </c>
       <c r="E225" s="39"/>
       <c r="F225" s="36"/>
@@ -13081,7 +13352,7 @@
         <v>876</v>
       </c>
       <c r="B226" s="18" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="C226" s="36"/>
       <c r="D226" s="36"/>
@@ -13097,7 +13368,7 @@
         <v>875</v>
       </c>
       <c r="B227" s="18" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="C227" s="36"/>
       <c r="D227" s="36"/>
@@ -13113,10 +13384,10 @@
         <v>862</v>
       </c>
       <c r="B228" s="18" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="C228" s="19" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="D228" s="36"/>
       <c r="E228" s="36"/>
@@ -13147,7 +13418,7 @@
         <v>879</v>
       </c>
       <c r="B230" s="18" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="C230" s="36"/>
       <c r="D230" s="36"/>
@@ -13163,7 +13434,7 @@
         <v>719</v>
       </c>
       <c r="B231" s="18" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="C231" s="36"/>
       <c r="D231" s="36"/>
@@ -13176,44 +13447,44 @@
     </row>
     <row r="232" spans="1:8" ht="66" customHeight="1">
       <c r="A232" s="13" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="B232" s="18" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="C232" s="67" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="D232" s="19" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
       <c r="E232" s="36"/>
       <c r="F232" s="19" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="G232" s="52" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="H232" s="19"/>
     </row>
     <row r="233" spans="1:8" ht="68" customHeight="1">
       <c r="A233" s="13" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B233" s="18" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C233" s="67" t="s">
         <v>1106</v>
       </c>
-      <c r="B233" s="18" t="s">
-        <v>1103</v>
-      </c>
-      <c r="C233" s="67" t="s">
-        <v>1109</v>
-      </c>
       <c r="D233" s="19" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="E233" s="19" t="s">
+        <v>1107</v>
+      </c>
+      <c r="F233" s="19" t="s">
         <v>1110</v>
-      </c>
-      <c r="F233" s="19" t="s">
-        <v>1113</v>
       </c>
       <c r="G233" s="68" t="s">
         <v>723</v>
@@ -13222,41 +13493,41 @@
     </row>
     <row r="234" spans="1:8" ht="83" customHeight="1">
       <c r="A234" s="13" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B234" s="18" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C234" s="67" t="s">
         <v>1192</v>
       </c>
-      <c r="B234" s="18" t="s">
-        <v>1196</v>
-      </c>
-      <c r="C234" s="67" t="s">
-        <v>1195</v>
-      </c>
       <c r="D234" s="19" t="s">
-        <v>1197</v>
+        <v>1194</v>
       </c>
       <c r="E234" s="19" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="F234" s="19"/>
       <c r="G234" s="52" t="s">
-        <v>1185</v>
+        <v>1182</v>
       </c>
       <c r="H234" s="19"/>
     </row>
     <row r="235" spans="1:8" ht="68" customHeight="1">
       <c r="A235" s="13" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B235" s="18" t="s">
         <v>1116</v>
       </c>
-      <c r="B235" s="18" t="s">
-        <v>1119</v>
-      </c>
       <c r="C235" s="19" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="D235" s="19" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="E235" s="19" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="F235" s="36"/>
       <c r="G235" s="55" t="s">
@@ -13269,7 +13540,7 @@
         <v>869</v>
       </c>
       <c r="B236" s="18" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="C236" s="36"/>
       <c r="D236" s="36"/>
@@ -13285,10 +13556,10 @@
         <v>878</v>
       </c>
       <c r="B237" s="18" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="C237" s="19" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="D237" s="36"/>
       <c r="E237" s="36"/>
@@ -13300,21 +13571,21 @@
     </row>
     <row r="238" spans="1:8" ht="74" customHeight="1">
       <c r="A238" s="13" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="B238" s="18" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C238" s="19" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D238" s="19" t="s">
         <v>1125</v>
-      </c>
-      <c r="C238" s="19" t="s">
-        <v>1126</v>
-      </c>
-      <c r="D238" s="19" t="s">
-        <v>1128</v>
       </c>
       <c r="E238" s="36"/>
       <c r="F238" s="36"/>
       <c r="G238" s="52" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="H238" s="36"/>
     </row>
@@ -13393,10 +13664,10 @@
         <v>872</v>
       </c>
       <c r="B244" s="18" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="C244" s="19" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="D244" s="36"/>
       <c r="E244" s="36"/>
@@ -13442,7 +13713,7 @@
     </row>
     <row r="247" spans="1:8" ht="55" customHeight="1">
       <c r="A247" s="13" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="B247" s="18" t="s">
         <v>732</v>
@@ -13462,7 +13733,7 @@
     </row>
     <row r="248" spans="1:8" ht="71" customHeight="1">
       <c r="A248" s="13" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="B248" s="18" t="s">
         <v>881</v>
@@ -13480,7 +13751,7 @@
     </row>
     <row r="249" spans="1:8" ht="43" customHeight="1">
       <c r="A249" s="13" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="B249" s="35" t="s">
         <v>740</v>
@@ -13520,7 +13791,7 @@
     </row>
     <row r="251" spans="1:8" ht="63" customHeight="1">
       <c r="A251" s="13" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="B251" s="18" t="s">
         <v>748</v>
@@ -13538,7 +13809,7 @@
     </row>
     <row r="252" spans="1:8" ht="57" customHeight="1">
       <c r="A252" s="13" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="B252" s="18" t="s">
         <v>749</v>
@@ -13580,7 +13851,7 @@
     </row>
     <row r="254" spans="1:8" ht="101" customHeight="1">
       <c r="A254" s="13" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="B254" s="35" t="s">
         <v>759</v>
@@ -13600,7 +13871,7 @@
     </row>
     <row r="255" spans="1:8" s="4" customFormat="1" ht="72" customHeight="1">
       <c r="A255" s="13" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="B255" s="18" t="s">
         <v>762</v>
@@ -13613,7 +13884,7 @@
       </c>
       <c r="E255" s="43"/>
       <c r="F255" s="43" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="G255" s="20" t="s">
         <v>764</v>
@@ -13622,7 +13893,7 @@
     </row>
     <row r="256" spans="1:8" s="4" customFormat="1" ht="54" customHeight="1">
       <c r="A256" s="13" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="B256" s="18" t="s">
         <v>769</v>
@@ -13726,7 +13997,7 @@
     </row>
     <row r="262" spans="1:8" s="3" customFormat="1" ht="64" customHeight="1">
       <c r="A262" s="13" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B262" s="11" t="s">
         <v>897</v>
@@ -13744,118 +14015,120 @@
     </row>
     <row r="263" spans="1:8" s="3" customFormat="1" ht="87" customHeight="1">
       <c r="A263" s="13" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
       <c r="B263" s="71" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="C263" s="6" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="D263" s="49"/>
       <c r="E263" s="49"/>
       <c r="F263" s="49"/>
       <c r="G263" s="52" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="H263" s="49"/>
     </row>
     <row r="264" spans="1:8" ht="76" customHeight="1">
       <c r="A264" s="13" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="B264" s="46" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="C264" s="6" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="D264" s="1"/>
       <c r="E264" s="1"/>
       <c r="F264" s="1"/>
       <c r="G264" s="52" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="H264" s="1"/>
     </row>
     <row r="265" spans="1:8" ht="80" customHeight="1">
       <c r="A265" s="13" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="B265" s="70" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C265" s="6" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D265" s="6" t="s">
         <v>1141</v>
-      </c>
-      <c r="C265" s="6" t="s">
-        <v>1143</v>
-      </c>
-      <c r="D265" s="6" t="s">
-        <v>1144</v>
       </c>
       <c r="E265" s="1"/>
       <c r="F265" s="72" t="s">
-        <v>1142</v>
+        <v>1139</v>
       </c>
       <c r="G265" s="52" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="H265" s="1"/>
     </row>
-    <row r="266" spans="1:8" ht="55" customHeight="1">
+    <row r="266" spans="1:8" ht="47" customHeight="1">
       <c r="A266" s="13" t="s">
         <v>912</v>
       </c>
       <c r="B266" s="18" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C266" s="19" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D266" s="19" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E266" s="52" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F266" s="52" t="s">
+        <v>1258</v>
+      </c>
+      <c r="G266" s="52" t="s">
         <v>1260</v>
-      </c>
-      <c r="C266" s="19" t="s">
-        <v>1264</v>
-      </c>
-      <c r="D266" s="19" t="s">
-        <v>1262</v>
-      </c>
-      <c r="E266" s="19"/>
-      <c r="F266" s="52" t="s">
-        <v>1261</v>
-      </c>
-      <c r="G266" s="52" t="s">
-        <v>1263</v>
       </c>
       <c r="H266" s="19"/>
     </row>
     <row r="267" spans="1:8" s="58" customFormat="1" ht="62" customHeight="1">
       <c r="A267" s="13" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="B267" s="18" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="C267" s="6" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="D267" s="6" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="E267" s="73" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="F267" s="6"/>
       <c r="G267" s="68" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
       <c r="H267" s="54" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="268" spans="1:8" s="58" customFormat="1" ht="62" customHeight="1">
       <c r="A268" s="13" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="B268" s="18" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="C268" s="6"/>
       <c r="D268" s="6" t="s">
-        <v>1175</v>
+        <v>1172</v>
       </c>
       <c r="E268" s="49"/>
       <c r="F268" s="49"/>
@@ -13864,19 +14137,19 @@
     </row>
     <row r="269" spans="1:8" s="58" customFormat="1" ht="62" customHeight="1">
       <c r="A269" s="13" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B269" s="18" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C269" s="6" t="s">
         <v>1150</v>
-      </c>
-      <c r="B269" s="18" t="s">
-        <v>1152</v>
-      </c>
-      <c r="C269" s="6" t="s">
-        <v>1153</v>
       </c>
       <c r="D269" s="49"/>
       <c r="E269" s="49"/>
       <c r="F269" s="49"/>
       <c r="G269" s="68" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="H269" s="49"/>
     </row>
@@ -13885,45 +14158,45 @@
         <v>950</v>
       </c>
       <c r="B270" s="70" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="C270" s="6" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="D270" s="6" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="E270" s="1"/>
       <c r="F270" s="1"/>
       <c r="G270" s="68" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="H270" s="1"/>
     </row>
     <row r="271" spans="1:8" ht="55" customHeight="1">
       <c r="A271" s="14" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B271" s="70" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C271" s="6" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D271" s="6" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E271" s="52" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F271" s="6" t="s">
         <v>1170</v>
       </c>
-      <c r="B271" s="70" t="s">
-        <v>1169</v>
-      </c>
-      <c r="C271" s="6" t="s">
-        <v>1171</v>
-      </c>
-      <c r="D271" s="6" t="s">
-        <v>1178</v>
-      </c>
-      <c r="E271" s="52" t="s">
-        <v>1172</v>
-      </c>
-      <c r="F271" s="6" t="s">
-        <v>1173</v>
-      </c>
       <c r="G271" s="68" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="H271" s="52" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="272" spans="1:8" ht="35" customHeight="1">
@@ -13946,52 +14219,52 @@
     </row>
     <row r="273" spans="1:8" ht="80" customHeight="1">
       <c r="A273" s="14" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B273" s="70" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C273" s="6" t="s">
         <v>1187</v>
       </c>
-      <c r="B273" s="70" t="s">
+      <c r="D273" s="6" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E273" s="6" t="s">
         <v>1186</v>
-      </c>
-      <c r="C273" s="6" t="s">
-        <v>1190</v>
-      </c>
-      <c r="D273" s="6" t="s">
-        <v>1191</v>
-      </c>
-      <c r="E273" s="6" t="s">
-        <v>1189</v>
       </c>
       <c r="F273" s="1"/>
       <c r="G273" s="55" t="s">
-        <v>1188</v>
+        <v>1185</v>
       </c>
       <c r="H273" s="1"/>
     </row>
     <row r="274" spans="1:8" ht="51" customHeight="1">
       <c r="A274" s="14" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="B274" s="70" t="s">
-        <v>1180</v>
+        <v>1177</v>
       </c>
       <c r="C274" s="6" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
       <c r="D274" s="6" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="E274" s="1"/>
       <c r="F274" s="1"/>
       <c r="G274" s="49" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="H274" s="1"/>
     </row>
     <row r="275" spans="1:8" ht="87" customHeight="1">
       <c r="A275" s="32" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="B275" s="18" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="C275" s="19" t="s">
         <v>909</v>
@@ -14010,7 +14283,7 @@
     </row>
     <row r="276" spans="1:8" ht="37" customHeight="1">
       <c r="A276" s="13" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="B276" s="18"/>
       <c r="C276" s="19"/>
@@ -14042,7 +14315,7 @@
     </row>
     <row r="278" spans="1:8" s="58" customFormat="1" ht="25" customHeight="1">
       <c r="A278" s="13" t="s">
-        <v>1184</v>
+        <v>1181</v>
       </c>
       <c r="B278" s="18"/>
       <c r="C278" s="6"/>
@@ -14050,13 +14323,13 @@
       <c r="E278" s="49"/>
       <c r="F278" s="49"/>
       <c r="G278" s="68" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="H278" s="49"/>
     </row>
     <row r="279" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A279" s="13" t="s">
-        <v>1182</v>
+        <v>1179</v>
       </c>
       <c r="B279" s="18"/>
       <c r="C279" s="6"/>
@@ -14064,7 +14337,7 @@
       <c r="E279" s="49"/>
       <c r="F279" s="49"/>
       <c r="G279" s="68" t="s">
-        <v>1183</v>
+        <v>1180</v>
       </c>
       <c r="H279" s="49"/>
     </row>
@@ -14087,14 +14360,14 @@
         <v>948</v>
       </c>
       <c r="B281" s="70" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
       <c r="C281" s="5"/>
       <c r="D281" s="1"/>
       <c r="E281" s="1"/>
       <c r="F281" s="1"/>
       <c r="G281" s="6" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="H281" s="1"/>
     </row>
@@ -14163,18 +14436,18 @@
         <v>956</v>
       </c>
       <c r="B287" s="77" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="C287" s="6" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="D287" s="6" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="E287" s="49"/>
       <c r="F287" s="49"/>
       <c r="G287" s="68" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="H287" s="49"/>
     </row>
@@ -14238,7 +14511,7 @@
       <c r="E292" s="49"/>
       <c r="F292" s="49"/>
       <c r="G292" s="52" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="H292" s="49"/>
     </row>
@@ -14354,23 +14627,23 @@
     </row>
     <row r="302" spans="1:8" s="58" customFormat="1" ht="66" customHeight="1">
       <c r="A302" s="13" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B302" s="70" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C302" s="6" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D302" s="6" t="s">
         <v>1222</v>
-      </c>
-      <c r="B302" s="70" t="s">
-        <v>1224</v>
-      </c>
-      <c r="C302" s="6" t="s">
-        <v>1223</v>
-      </c>
-      <c r="D302" s="6" t="s">
-        <v>1225</v>
       </c>
       <c r="E302" s="49"/>
       <c r="F302" s="78" t="s">
-        <v>1221</v>
+        <v>1218</v>
       </c>
       <c r="G302" s="52" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
       <c r="H302" s="49"/>
     </row>
@@ -14379,14 +14652,14 @@
         <v>972</v>
       </c>
       <c r="B303" s="63" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="C303" s="64"/>
       <c r="D303" s="49"/>
       <c r="E303" s="49"/>
       <c r="F303" s="49"/>
       <c r="G303" s="6" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="H303" s="49"/>
     </row>
@@ -14395,10 +14668,10 @@
         <v>973</v>
       </c>
       <c r="B304" s="63" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="C304" s="65" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="D304" s="49"/>
       <c r="E304" s="49"/>
@@ -14411,52 +14684,52 @@
         <v>971</v>
       </c>
       <c r="B305" s="63" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="C305" s="67" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="D305" s="49"/>
       <c r="E305" s="49"/>
       <c r="F305" s="49"/>
       <c r="G305" s="49" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="H305" s="49"/>
     </row>
     <row r="306" spans="1:8" s="58" customFormat="1" ht="74" customHeight="1">
       <c r="A306" s="66" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B306" s="18" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C306" s="67" t="s">
         <v>1057</v>
-      </c>
-      <c r="B306" s="18" t="s">
-        <v>1059</v>
-      </c>
-      <c r="C306" s="67" t="s">
-        <v>1060</v>
       </c>
       <c r="D306" s="49"/>
       <c r="E306" s="49"/>
       <c r="F306" s="49"/>
       <c r="G306" s="55" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="H306" s="49"/>
     </row>
-    <row r="307" spans="1:8" s="58" customFormat="1" ht="36" customHeight="1">
+    <row r="307" spans="1:8" s="58" customFormat="1" ht="34" customHeight="1">
       <c r="A307" s="14" t="s">
-        <v>1211</v>
-      </c>
-      <c r="B307" s="18"/>
-      <c r="C307" s="67"/>
+        <v>1272</v>
+      </c>
+      <c r="B307" s="63"/>
+      <c r="C307" s="49"/>
       <c r="D307" s="49"/>
       <c r="E307" s="49"/>
       <c r="F307" s="49"/>
-      <c r="G307" s="55"/>
+      <c r="G307" s="49"/>
       <c r="H307" s="49"/>
     </row>
-    <row r="308" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
+    <row r="308" spans="1:8" s="58" customFormat="1" ht="36" customHeight="1">
       <c r="A308" s="14" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="B308" s="18"/>
       <c r="C308" s="67"/>
@@ -14468,7 +14741,7 @@
     </row>
     <row r="309" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
       <c r="A309" s="14" t="s">
-        <v>1228</v>
+        <v>1209</v>
       </c>
       <c r="B309" s="18"/>
       <c r="C309" s="67"/>
@@ -14480,7 +14753,7 @@
     </row>
     <row r="310" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
       <c r="A310" s="14" t="s">
-        <v>1213</v>
+        <v>1225</v>
       </c>
       <c r="B310" s="18"/>
       <c r="C310" s="67"/>
@@ -14492,7 +14765,7 @@
     </row>
     <row r="311" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
       <c r="A311" s="14" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="B311" s="18"/>
       <c r="C311" s="67"/>
@@ -14504,7 +14777,7 @@
     </row>
     <row r="312" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
       <c r="A312" s="14" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="B312" s="18"/>
       <c r="C312" s="67"/>
@@ -14516,7 +14789,7 @@
     </row>
     <row r="313" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
       <c r="A313" s="14" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="B313" s="18"/>
       <c r="C313" s="67"/>
@@ -14528,7 +14801,7 @@
     </row>
     <row r="314" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
       <c r="A314" s="14" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
       <c r="B314" s="18"/>
       <c r="C314" s="67"/>
@@ -14539,8 +14812,8 @@
       <c r="H314" s="49"/>
     </row>
     <row r="315" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
-      <c r="A315" s="42" t="s">
-        <v>1218</v>
+      <c r="A315" s="14" t="s">
+        <v>1214</v>
       </c>
       <c r="B315" s="18"/>
       <c r="C315" s="67"/>
@@ -14551,8 +14824,8 @@
       <c r="H315" s="49"/>
     </row>
     <row r="316" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
-      <c r="A316" s="14" t="s">
-        <v>1219</v>
+      <c r="A316" s="42" t="s">
+        <v>1215</v>
       </c>
       <c r="B316" s="18"/>
       <c r="C316" s="67"/>
@@ -14562,21 +14835,21 @@
       <c r="G316" s="55"/>
       <c r="H316" s="49"/>
     </row>
-    <row r="317" spans="1:8" s="58" customFormat="1" ht="34" customHeight="1">
+    <row r="317" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
       <c r="A317" s="14" t="s">
-        <v>1055</v>
-      </c>
-      <c r="B317" s="63"/>
-      <c r="C317" s="49"/>
+        <v>1216</v>
+      </c>
+      <c r="B317" s="18"/>
+      <c r="C317" s="67"/>
       <c r="D317" s="49"/>
       <c r="E317" s="49"/>
       <c r="F317" s="49"/>
-      <c r="G317" s="49"/>
+      <c r="G317" s="55"/>
       <c r="H317" s="49"/>
     </row>
     <row r="318" spans="1:8" s="58" customFormat="1" ht="43" customHeight="1">
       <c r="A318" s="14" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="B318" s="63"/>
       <c r="C318" s="49"/>
@@ -14686,7 +14959,7 @@
     </row>
     <row r="327" spans="1:8" s="58" customFormat="1" ht="47" customHeight="1">
       <c r="A327" s="13" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="B327" s="57"/>
       <c r="C327" s="49"/>
@@ -14722,49 +14995,49 @@
     </row>
     <row r="330" spans="1:8" s="58" customFormat="1" ht="81" customHeight="1">
       <c r="A330" s="79" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="B330" s="70" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
       <c r="C330" s="6" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="D330" s="6" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="E330" s="49"/>
       <c r="F330" s="49"/>
       <c r="G330" s="68" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="H330" s="49"/>
     </row>
     <row r="331" spans="1:8" s="58" customFormat="1" ht="68" customHeight="1">
       <c r="A331" s="13" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B331" s="70" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C331" s="78" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D331" s="6" t="s">
         <v>1248</v>
       </c>
-      <c r="B331" s="70" t="s">
+      <c r="E331" s="6" t="s">
         <v>1249</v>
-      </c>
-      <c r="C331" s="78" t="s">
-        <v>1250</v>
-      </c>
-      <c r="D331" s="6" t="s">
-        <v>1251</v>
-      </c>
-      <c r="E331" s="6" t="s">
-        <v>1252</v>
       </c>
       <c r="F331" s="49"/>
       <c r="G331" s="52" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="H331" s="49"/>
     </row>
     <row r="332" spans="1:8" s="58" customFormat="1" ht="68" customHeight="1">
       <c r="A332" s="13" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
       <c r="B332" s="70"/>
       <c r="C332" s="78"/>
@@ -14776,70 +15049,98 @@
     </row>
     <row r="333" spans="1:8" s="58" customFormat="1" ht="69" customHeight="1">
       <c r="A333" s="79" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="B333" s="70" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="C333" s="6" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="D333" s="6" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="E333" s="6" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="F333" s="52" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="G333" s="52" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="H333" s="49"/>
     </row>
-    <row r="334" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
-      <c r="A334" s="74" t="s">
+    <row r="334" spans="1:8" s="58" customFormat="1" ht="78" customHeight="1">
+      <c r="A334" s="14" t="s">
+        <v>984</v>
+      </c>
+      <c r="B334" s="70" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C334" s="6" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D334" s="6" t="s">
+        <v>1265</v>
+      </c>
+      <c r="E334" s="80" t="s">
+        <v>1273</v>
+      </c>
+      <c r="F334" s="49"/>
+      <c r="G334" s="68" t="s">
+        <v>1263</v>
+      </c>
+      <c r="H334" s="49"/>
+    </row>
+    <row r="335" spans="1:8" s="58" customFormat="1" ht="42" customHeight="1">
+      <c r="A335" s="14" t="s">
         <v>983</v>
       </c>
-      <c r="B334" s="57"/>
-      <c r="C334" s="49"/>
-      <c r="D334" s="49"/>
-      <c r="E334" s="49"/>
-      <c r="F334" s="49"/>
-      <c r="G334" s="49"/>
-      <c r="H334" s="49"/>
-    </row>
-    <row r="335" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
-      <c r="A335" s="14" t="s">
-        <v>984</v>
-      </c>
-      <c r="B335" s="57"/>
-      <c r="C335" s="49"/>
-      <c r="D335" s="49"/>
+      <c r="B335" s="57" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C335" s="49" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D335" s="6" t="s">
+        <v>1271</v>
+      </c>
       <c r="E335" s="49"/>
-      <c r="F335" s="49"/>
-      <c r="G335" s="49"/>
+      <c r="F335" s="52" t="s">
+        <v>1270</v>
+      </c>
+      <c r="G335" s="52" t="s">
+        <v>1269</v>
+      </c>
       <c r="H335" s="49"/>
     </row>
-    <row r="336" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
+    <row r="336" spans="1:8" s="58" customFormat="1" ht="80" customHeight="1">
       <c r="A336" s="14" t="s">
-        <v>985</v>
-      </c>
-      <c r="B336" s="57"/>
-      <c r="C336" s="49"/>
-      <c r="D336" s="49"/>
+        <v>1274</v>
+      </c>
+      <c r="B336" s="70" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C336" s="6" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D336" s="6" t="s">
+        <v>1278</v>
+      </c>
       <c r="E336" s="49"/>
       <c r="F336" s="49"/>
-      <c r="G336" s="49"/>
+      <c r="G336" s="49" t="s">
+        <v>1275</v>
+      </c>
       <c r="H336" s="49"/>
     </row>
     <row r="337" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
-      <c r="A337" s="74" t="s">
-        <v>986</v>
+      <c r="A337" s="14" t="s">
+        <v>985</v>
       </c>
       <c r="B337" s="57"/>
-      <c r="C337" s="49"/>
+      <c r="C337" s="6"/>
       <c r="D337" s="49"/>
       <c r="E337" s="49"/>
       <c r="F337" s="49"/>
@@ -14848,7 +15149,7 @@
     </row>
     <row r="338" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A338" s="14" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B338" s="57"/>
       <c r="C338" s="49"/>
@@ -14860,7 +15161,7 @@
     </row>
     <row r="339" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A339" s="14" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B339" s="57"/>
       <c r="C339" s="49"/>
@@ -14872,7 +15173,7 @@
     </row>
     <row r="340" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A340" s="14" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B340" s="57"/>
       <c r="C340" s="49"/>
@@ -14884,7 +15185,7 @@
     </row>
     <row r="341" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A341" s="14" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="B341" s="57"/>
       <c r="C341" s="49"/>
@@ -14896,7 +15197,7 @@
     </row>
     <row r="342" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A342" s="14" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B342" s="57"/>
       <c r="C342" s="49"/>
@@ -14908,7 +15209,7 @@
     </row>
     <row r="343" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A343" s="14" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B343" s="57"/>
       <c r="C343" s="49"/>
@@ -14920,7 +15221,7 @@
     </row>
     <row r="344" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A344" s="14" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B344" s="57"/>
       <c r="C344" s="49"/>
@@ -14932,7 +15233,7 @@
     </row>
     <row r="345" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A345" s="14" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B345" s="57"/>
       <c r="C345" s="49"/>
@@ -14944,7 +15245,7 @@
     </row>
     <row r="346" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A346" s="14" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B346" s="57"/>
       <c r="C346" s="49"/>
@@ -14956,7 +15257,7 @@
     </row>
     <row r="347" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A347" s="14" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B347" s="57"/>
       <c r="C347" s="49"/>
@@ -14968,7 +15269,7 @@
     </row>
     <row r="348" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A348" s="14" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B348" s="57"/>
       <c r="C348" s="49"/>
@@ -14980,7 +15281,7 @@
     </row>
     <row r="349" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A349" s="14" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B349" s="57"/>
       <c r="C349" s="49"/>
@@ -14992,7 +15293,7 @@
     </row>
     <row r="350" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A350" s="14" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B350" s="57"/>
       <c r="C350" s="49"/>
@@ -15004,7 +15305,7 @@
     </row>
     <row r="351" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A351" s="14" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B351" s="57"/>
       <c r="C351" s="49"/>
@@ -15016,7 +15317,7 @@
     </row>
     <row r="352" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A352" s="14" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B352" s="57"/>
       <c r="C352" s="49"/>
@@ -15028,7 +15329,7 @@
     </row>
     <row r="353" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A353" s="14" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B353" s="57"/>
       <c r="C353" s="49"/>
@@ -15040,7 +15341,7 @@
     </row>
     <row r="354" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A354" s="14" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B354" s="57"/>
       <c r="C354" s="49"/>
@@ -15052,7 +15353,7 @@
     </row>
     <row r="355" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A355" s="74" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B355" s="57"/>
       <c r="C355" s="49"/>
@@ -15064,7 +15365,7 @@
     </row>
     <row r="356" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A356" s="14" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B356" s="57"/>
       <c r="C356" s="49"/>
@@ -15076,7 +15377,7 @@
     </row>
     <row r="357" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A357" s="14" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B357" s="57"/>
       <c r="C357" s="49"/>
@@ -15088,7 +15389,7 @@
     </row>
     <row r="358" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A358" s="14" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B358" s="57"/>
       <c r="C358" s="49"/>
@@ -15098,33 +15399,39 @@
       <c r="G358" s="49"/>
       <c r="H358" s="49"/>
     </row>
-    <row r="359" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
-      <c r="A359" s="74" t="s">
-        <v>1007</v>
-      </c>
-      <c r="B359" s="57"/>
-      <c r="C359" s="49"/>
+    <row r="359" spans="1:8" s="58" customFormat="1" ht="53" customHeight="1">
+      <c r="A359" s="13" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B359" s="70" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C359" s="6" t="s">
+        <v>1283</v>
+      </c>
       <c r="D359" s="49"/>
       <c r="E359" s="49"/>
       <c r="F359" s="49"/>
-      <c r="G359" s="49"/>
+      <c r="G359" s="52" t="s">
+        <v>1279</v>
+      </c>
       <c r="H359" s="49"/>
     </row>
     <row r="360" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A360" s="14" t="s">
-        <v>1008</v>
+        <v>1280</v>
       </c>
       <c r="B360" s="57"/>
       <c r="C360" s="49"/>
       <c r="D360" s="49"/>
       <c r="E360" s="49"/>
       <c r="F360" s="49"/>
-      <c r="G360" s="49"/>
+      <c r="G360" s="52"/>
       <c r="H360" s="49"/>
     </row>
     <row r="361" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A361" s="14" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="B361" s="57"/>
       <c r="C361" s="49"/>
@@ -15136,7 +15443,7 @@
     </row>
     <row r="362" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A362" s="14" t="s">
-        <v>1015</v>
+        <v>1007</v>
       </c>
       <c r="B362" s="57"/>
       <c r="C362" s="49"/>
@@ -15148,7 +15455,7 @@
     </row>
     <row r="363" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A363" s="14" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B363" s="57"/>
       <c r="C363" s="49"/>
@@ -15158,21 +15465,21 @@
       <c r="G363" s="49"/>
       <c r="H363" s="49"/>
     </row>
-    <row r="364" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
+    <row r="364" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A364" s="14" t="s">
-        <v>1016</v>
-      </c>
-      <c r="B364" s="35"/>
-      <c r="C364" s="37"/>
-      <c r="D364" s="37"/>
-      <c r="E364" s="37"/>
-      <c r="F364" s="37"/>
-      <c r="G364" s="37"/>
-      <c r="H364" s="37"/>
+        <v>1012</v>
+      </c>
+      <c r="B364" s="57"/>
+      <c r="C364" s="49"/>
+      <c r="D364" s="49"/>
+      <c r="E364" s="49"/>
+      <c r="F364" s="49"/>
+      <c r="G364" s="49"/>
+      <c r="H364" s="49"/>
     </row>
     <row r="365" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A365" s="14" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="B365" s="35"/>
       <c r="C365" s="37"/>
@@ -15184,7 +15491,7 @@
     </row>
     <row r="366" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A366" s="14" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="B366" s="35"/>
       <c r="C366" s="37"/>
@@ -15196,7 +15503,7 @@
     </row>
     <row r="367" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A367" s="14" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B367" s="35"/>
       <c r="C367" s="37"/>
@@ -15206,21 +15513,21 @@
       <c r="G367" s="37"/>
       <c r="H367" s="37"/>
     </row>
-    <row r="368" spans="1:8">
-      <c r="A368" s="56" t="s">
-        <v>1031</v>
-      </c>
-      <c r="B368" s="8"/>
-      <c r="C368" s="5"/>
-      <c r="D368" s="1"/>
-      <c r="E368" s="1"/>
-      <c r="F368" s="1"/>
-      <c r="G368" s="5"/>
-      <c r="H368" s="1"/>
+    <row r="368" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
+      <c r="A368" s="14" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B368" s="35"/>
+      <c r="C368" s="37"/>
+      <c r="D368" s="37"/>
+      <c r="E368" s="37"/>
+      <c r="F368" s="37"/>
+      <c r="G368" s="37"/>
+      <c r="H368" s="37"/>
     </row>
     <row r="369" spans="1:8">
       <c r="A369" s="56" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="B369" s="8"/>
       <c r="C369" s="5"/>
@@ -15232,7 +15539,7 @@
     </row>
     <row r="370" spans="1:8">
       <c r="A370" s="56" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="B370" s="8"/>
       <c r="C370" s="5"/>
@@ -15243,8 +15550,8 @@
       <c r="H370" s="1"/>
     </row>
     <row r="371" spans="1:8">
-      <c r="A371" s="75" t="s">
-        <v>1034</v>
+      <c r="A371" s="56" t="s">
+        <v>1031</v>
       </c>
       <c r="B371" s="8"/>
       <c r="C371" s="5"/>
@@ -15255,8 +15562,8 @@
       <c r="H371" s="1"/>
     </row>
     <row r="372" spans="1:8">
-      <c r="A372" s="56" t="s">
-        <v>1035</v>
+      <c r="A372" s="75" t="s">
+        <v>1032</v>
       </c>
       <c r="B372" s="8"/>
       <c r="C372" s="5"/>
@@ -15268,7 +15575,7 @@
     </row>
     <row r="373" spans="1:8">
       <c r="A373" s="56" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="B373" s="8"/>
       <c r="C373" s="5"/>
@@ -15280,7 +15587,7 @@
     </row>
     <row r="374" spans="1:8">
       <c r="A374" s="56" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="B374" s="8"/>
       <c r="C374" s="5"/>
@@ -15292,7 +15599,7 @@
     </row>
     <row r="375" spans="1:8">
       <c r="A375" s="56" t="s">
-        <v>1181</v>
+        <v>1035</v>
       </c>
       <c r="B375" s="8"/>
       <c r="C375" s="5"/>
@@ -15304,7 +15611,7 @@
     </row>
     <row r="376" spans="1:8">
       <c r="A376" s="56" t="s">
-        <v>1229</v>
+        <v>1178</v>
       </c>
       <c r="B376" s="8"/>
       <c r="C376" s="5"/>
@@ -15315,7 +15622,9 @@
       <c r="H376" s="1"/>
     </row>
     <row r="377" spans="1:8">
-      <c r="A377" s="56"/>
+      <c r="A377" s="56" t="s">
+        <v>1226</v>
+      </c>
       <c r="B377" s="8"/>
       <c r="C377" s="5"/>
       <c r="D377" s="1"/>
@@ -15713,6 +16022,16 @@
       <c r="F416" s="1"/>
       <c r="G416" s="5"/>
       <c r="H416" s="1"/>
+    </row>
+    <row r="417" spans="1:8">
+      <c r="A417" s="56"/>
+      <c r="B417" s="8"/>
+      <c r="C417" s="5"/>
+      <c r="D417" s="1"/>
+      <c r="E417" s="1"/>
+      <c r="F417" s="1"/>
+      <c r="G417" s="5"/>
+      <c r="H417" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -15882,8 +16201,13 @@
     <hyperlink ref="G117" r:id="rId164" xr:uid="{2433591E-E411-6746-B249-C92375CC3D18}"/>
     <hyperlink ref="F266" r:id="rId165" xr:uid="{67739776-BDA5-8645-92A8-9C973B7B7ABA}"/>
     <hyperlink ref="G266" r:id="rId166" xr:uid="{01C42E52-E49F-194B-A10B-2B76D38D3393}"/>
+    <hyperlink ref="E266" r:id="rId167" xr:uid="{B23044BB-3690-284E-BC6E-BB70AB972573}"/>
+    <hyperlink ref="G334" r:id="rId168" xr:uid="{80654B4F-CF02-F64F-B30F-FFCF3142746A}"/>
+    <hyperlink ref="G335" r:id="rId169" xr:uid="{8F913997-4003-3944-B0F9-A2B8764AF8D8}"/>
+    <hyperlink ref="F335" r:id="rId170" xr:uid="{0530DF63-A52D-004E-82AF-ED33E28EAF80}"/>
+    <hyperlink ref="G359" r:id="rId171" xr:uid="{C10B92B6-2829-1842-8167-60AE046440E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId167"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId172"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bfs technique for lexographically smallest path
</commit_message>
<xml_diff>
--- a/Applications/QuestionListWithApproaches.xlsx
+++ b/Applications/QuestionListWithApproaches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksharkashyap/Documents/VisualStudio/Applications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1AC8D0-0E40-D148-B4F6-18DE82DF3A68}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB55CA1F-5F6F-184E-BAA2-7E53653B5851}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="460" windowWidth="32600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="1303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="1311">
   <si>
     <t>Convert Binary Number in a Linked List to Integer</t>
   </si>
@@ -8780,6 +8780,27 @@
     <t>sort the arr, loop through elements, if(SET has arr[i]) count++ SET.add(arr[i]+k)</t>
   </si>
   <si>
+    <t>count all distinct pairs with difference equal to k</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-bottom-left-tree-value/</t>
+  </si>
+  <si>
+    <t>find bottom left tree value[Given the root of a binary tree, return the leftmost value in the last row of the tree.]</t>
+  </si>
+  <si>
+    <t>bfs traversal from right to left, the last node visited will be the leftmost node of the last row)</t>
+  </si>
+  <si>
+    <t>calculate hight + dfs to get the items of the last row  + return first item of the list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">range update query </t>
+  </si>
+  <si>
+    <t>practice problem : https://www.hackerrank.com/challenges/crush/problem</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">put all elements to hashmap_arr -&gt; set to true, now find arr[i]+k increase count and find arr[i]-k increase count, now remove arr[i] -&gt; set to false </t>
     </r>
@@ -8787,7 +8808,7 @@
       <rPr>
         <b/>
         <u/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
@@ -8795,14 +8816,42 @@
     </r>
   </si>
   <si>
-    <t>count all distinct pairs with difference equal to k</t>
+    <t>point update (segment tree) O(NlogN) (for n given elements we need to run logn update queries)
+lazy propogation (segment tree) [O(logn) time]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Range update query in O(1) with condition that all the update quries are performed first before any other query [basically we want something out of after all the update queries are done]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>lecture</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : https://www.youtube.com/watch?v=i7xZ4Yd_jN8
+</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="59">
+  <fonts count="58">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9178,13 +9227,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)_x0000_"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -9248,7 +9290,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
@@ -9463,6 +9505,9 @@
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -9749,8 +9794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A366" zoomScale="171" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A380" sqref="A380"/>
+    <sheetView tabSelected="1" topLeftCell="A374" zoomScale="171" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B382" sqref="B382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -16208,7 +16253,7 @@
     </row>
     <row r="380" spans="1:8" ht="75" customHeight="1">
       <c r="A380" s="13" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="B380" s="57" t="s">
         <v>1297</v>
@@ -16222,31 +16267,47 @@
       <c r="E380" s="6" t="s">
         <v>1300</v>
       </c>
-      <c r="F380" s="72" t="s">
-        <v>1301</v>
+      <c r="F380" s="6" t="s">
+        <v>1308</v>
       </c>
       <c r="G380" s="49" t="s">
         <v>1296</v>
       </c>
       <c r="H380" s="1"/>
     </row>
-    <row r="381" spans="1:8">
-      <c r="A381" s="56"/>
-      <c r="B381" s="8"/>
-      <c r="C381" s="5"/>
+    <row r="381" spans="1:8" ht="48" customHeight="1">
+      <c r="A381" s="13" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B381" s="70" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C381" s="6" t="s">
+        <v>1304</v>
+      </c>
       <c r="D381" s="1"/>
       <c r="E381" s="1"/>
       <c r="F381" s="1"/>
-      <c r="G381" s="5"/>
+      <c r="G381" s="6" t="s">
+        <v>1302</v>
+      </c>
       <c r="H381" s="1"/>
     </row>
-    <row r="382" spans="1:8">
-      <c r="A382" s="56"/>
-      <c r="B382" s="8"/>
-      <c r="C382" s="5"/>
-      <c r="D382" s="1"/>
-      <c r="E382" s="1"/>
-      <c r="F382" s="1"/>
+    <row r="382" spans="1:8" ht="77" customHeight="1">
+      <c r="A382" s="81" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B382" s="70" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C382" s="6" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D382" s="6" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E382" s="5"/>
+      <c r="F382" s="5"/>
       <c r="G382" s="5"/>
       <c r="H382" s="1"/>
     </row>

</xml_diff>

<commit_message>
java nextLine issue notes
</commit_message>
<xml_diff>
--- a/Applications/QuestionListWithApproaches.xlsx
+++ b/Applications/QuestionListWithApproaches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksharkashyap/Documents/VisualStudio/Applications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EECBE8-2879-074B-9271-3D8F9A47F28A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2019288D-5636-9849-80EA-B625D6208C33}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="460" windowWidth="32600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="1351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="1363">
   <si>
     <t>Convert Binary Number in a Linked List to Integer</t>
   </si>
@@ -5220,9 +5220,6 @@
     <t>Print all "K" Sum paths in a Binary tree</t>
   </si>
   <si>
-    <t>find distance betweeen two nodes in binary tree</t>
-  </si>
-  <si>
     <t>Find inorder successor and inorder predecessor in a BST</t>
   </si>
   <si>
@@ -9117,12 +9114,211 @@
   <si>
     <t>we want a node which is in the top-most(visited first HD-wise) in every horizontal distances [if we do vertical order traversall]</t>
   </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/bottom-view-binary-tree/</t>
+  </si>
+  <si>
+    <r>
+      <t>do PreOrder(root,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>left</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>,right)  and maintain HashSet to store depths when you encounter it first time for every level, it will avoid visiting another nodes in the same level</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> O(n) time and  O(height) space </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>do PreOrder(root,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>right</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">,left)  and maintain HashSet to store depths when you encounter it first time for every level, it will avoid visiting another nodes in the same level </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">O(n) time and O(height) space </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">avoid hashset by maintaining two variables </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>[curr_depth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">,  GLOBAL </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>max_depth_visited</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>] if(curr_depth &gt; max_depth_visited){update maxdepthvisited and add this node to answer}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">avoid hashset by maintaining two variables </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>[curr_depth,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>GLOBAL</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> max_depth_visited]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> if(curr_depth &gt; max_depth_visited){update maxdepthvisited and add this node to answer}</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/print-left-view-binary-tree/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">using BFS print the rightmost(when iterator is at the SIZE-1) node only in every level </t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/print-right-view-binary-tree-2</t>
+  </si>
+  <si>
+    <t>using BFS print the leftmost node only in every level</t>
+  </si>
+  <si>
+    <t>merge two sorted linkedlist</t>
+  </si>
+  <si>
+    <t>recursive (use extra dummy result pointer)</t>
+  </si>
+  <si>
+    <t>iterative two pointer approach (use dummy result pointer)</t>
+  </si>
+  <si>
+    <t>https://www.hackerrank.com/challenges/merge-two-sorted-linked-lists/problem</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="60">
+  <fonts count="61">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9507,6 +9703,13 @@
     <font>
       <b/>
       <u/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -10077,10 +10280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S421"/>
+  <dimension ref="A1:S420"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A308" zoomScale="171" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B314" sqref="B314"/>
+    <sheetView tabSelected="1" topLeftCell="A385" zoomScale="171" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A396" sqref="A396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10402,7 +10605,7 @@
         <v>723</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>
@@ -10431,13 +10634,13 @@
     </row>
     <row r="19" spans="1:8" ht="46" customHeight="1">
       <c r="A19" s="13" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -10447,13 +10650,13 @@
     </row>
     <row r="20" spans="1:8" ht="43" customHeight="1">
       <c r="A20" s="14" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -10463,13 +10666,13 @@
     </row>
     <row r="21" spans="1:8" ht="63" customHeight="1">
       <c r="A21" s="14" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B21" s="61" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C21" s="62" t="s">
         <v>1039</v>
-      </c>
-      <c r="C21" s="62" t="s">
-        <v>1040</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -10479,7 +10682,7 @@
     </row>
     <row r="22" spans="1:8" ht="24" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="5"/>
@@ -10491,7 +10694,7 @@
     </row>
     <row r="23" spans="1:8" ht="32" customHeight="1">
       <c r="A23" s="14" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="5"/>
@@ -10503,7 +10706,7 @@
     </row>
     <row r="24" spans="1:8" ht="33" customHeight="1">
       <c r="A24" s="14" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="5"/>
@@ -10515,7 +10718,7 @@
     </row>
     <row r="25" spans="1:8" ht="33" customHeight="1">
       <c r="A25" s="14" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="5"/>
@@ -10527,7 +10730,7 @@
     </row>
     <row r="26" spans="1:8" ht="33" customHeight="1">
       <c r="A26" s="14" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="5"/>
@@ -10539,7 +10742,7 @@
     </row>
     <row r="27" spans="1:8" ht="29" customHeight="1">
       <c r="A27" s="14" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
@@ -10859,13 +11062,13 @@
     </row>
     <row r="46" spans="1:8" ht="71" customHeight="1">
       <c r="A46" s="13" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C46" s="19" t="s">
         <v>1332</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>1331</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>1333</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="19"/>
@@ -11460,7 +11663,7 @@
         <v>224</v>
       </c>
       <c r="D77" s="19" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="E77" s="19" t="s">
         <v>225</v>
@@ -12105,7 +12308,7 @@
     </row>
     <row r="112" spans="1:8" ht="28">
       <c r="A112" s="13" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B112" s="18" t="s">
         <v>319</v>
@@ -12127,7 +12330,7 @@
     </row>
     <row r="113" spans="1:8" ht="50" customHeight="1">
       <c r="A113" s="23" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B113" s="18" t="s">
         <v>123</v>
@@ -12136,7 +12339,7 @@
         <v>124</v>
       </c>
       <c r="D113" s="19" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="E113" s="19"/>
       <c r="F113" s="19"/>
@@ -12197,7 +12400,7 @@
     </row>
     <row r="117" spans="1:8" s="3" customFormat="1" ht="66" customHeight="1">
       <c r="A117" s="13" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B117" s="18"/>
       <c r="C117" s="19"/>
@@ -12205,13 +12408,13 @@
       <c r="E117" s="19"/>
       <c r="F117" s="19"/>
       <c r="G117" s="52" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="H117" s="19"/>
     </row>
     <row r="118" spans="1:8" s="3" customFormat="1" ht="80" customHeight="1">
       <c r="A118" s="13" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B118" s="18" t="s">
         <v>371</v>
@@ -12229,7 +12432,7 @@
     </row>
     <row r="119" spans="1:8" s="3" customFormat="1" ht="80" customHeight="1">
       <c r="A119" s="13" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B119" s="18"/>
       <c r="C119" s="19"/>
@@ -12241,7 +12444,7 @@
     </row>
     <row r="120" spans="1:8" s="3" customFormat="1" ht="62" customHeight="1">
       <c r="A120" s="13" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B120" s="18"/>
       <c r="C120" s="19"/>
@@ -12253,7 +12456,7 @@
     </row>
     <row r="121" spans="1:8" s="3" customFormat="1" ht="87" customHeight="1">
       <c r="A121" s="13" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B121" s="18"/>
       <c r="C121" s="19"/>
@@ -12265,7 +12468,7 @@
     </row>
     <row r="122" spans="1:8" s="3" customFormat="1" ht="80" customHeight="1">
       <c r="A122" s="13" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B122" s="18"/>
       <c r="C122" s="19"/>
@@ -13021,7 +13224,7 @@
         <v>505</v>
       </c>
       <c r="F162" s="19" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="G162" s="52" t="s">
         <v>501</v>
@@ -13048,10 +13251,10 @@
     </row>
     <row r="164" spans="1:8" ht="52" customHeight="1">
       <c r="A164" s="13" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B164" s="70" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>152</v>
@@ -13059,10 +13262,10 @@
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
       <c r="F164" s="54" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="G164" s="54" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="H164" s="1"/>
     </row>
@@ -13434,17 +13637,17 @@
     </row>
     <row r="184" spans="1:8" ht="46" customHeight="1">
       <c r="A184" s="13" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B184" s="57" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="C184" s="5"/>
       <c r="D184" s="1"/>
       <c r="E184" s="1"/>
       <c r="F184" s="1"/>
       <c r="G184" s="52" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="H184" s="1"/>
     </row>
@@ -13962,32 +14165,32 @@
     </row>
     <row r="213" spans="1:8" ht="61" customHeight="1">
       <c r="A213" s="13" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B213" s="18" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C213" s="19"/>
       <c r="D213" s="19"/>
       <c r="E213" s="19"/>
       <c r="F213" s="19"/>
       <c r="G213" s="20" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="H213" s="19"/>
     </row>
     <row r="214" spans="1:8" ht="78" customHeight="1">
       <c r="A214" s="13" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B214" s="35" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C214" s="19" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D214" s="19" t="s">
         <v>1058</v>
-      </c>
-      <c r="C214" s="19" t="s">
-        <v>1068</v>
-      </c>
-      <c r="D214" s="19" t="s">
-        <v>1059</v>
       </c>
       <c r="F214" s="36"/>
       <c r="G214" s="40" t="s">
@@ -14000,51 +14203,51 @@
         <v>942</v>
       </c>
       <c r="B215" s="46" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C215" s="6" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="D215" s="1"/>
       <c r="E215" s="1"/>
       <c r="F215" s="1"/>
       <c r="G215" s="49" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="H215" s="1"/>
     </row>
     <row r="216" spans="1:8" ht="76" customHeight="1">
       <c r="A216" s="13" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B216" s="18" t="s">
         <v>1060</v>
-      </c>
-      <c r="B216" s="18" t="s">
-        <v>1061</v>
       </c>
       <c r="C216" s="36"/>
       <c r="D216" s="36"/>
       <c r="E216" s="36"/>
       <c r="F216" s="36"/>
       <c r="G216" s="40" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="H216" s="36"/>
     </row>
     <row r="217" spans="1:8" ht="83" customHeight="1">
       <c r="A217" s="13" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B217" s="18" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C217" s="39" t="s">
         <v>1066</v>
       </c>
-      <c r="C217" s="39" t="s">
-        <v>1067</v>
-      </c>
       <c r="D217" s="19" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="F217" s="36"/>
       <c r="G217" s="40" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="H217" s="36"/>
     </row>
@@ -14086,10 +14289,10 @@
     </row>
     <row r="220" spans="1:8" ht="63" customHeight="1">
       <c r="A220" s="33" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B220" s="18" t="s">
         <v>1021</v>
-      </c>
-      <c r="B220" s="18" t="s">
-        <v>1022</v>
       </c>
       <c r="C220" s="36"/>
       <c r="D220" s="36"/>
@@ -14102,25 +14305,25 @@
     </row>
     <row r="221" spans="1:8" s="4" customFormat="1" ht="104" customHeight="1">
       <c r="A221" s="32" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B221" s="18" t="s">
         <v>677</v>
       </c>
       <c r="C221" s="67" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D221" s="19" t="s">
         <v>1069</v>
       </c>
-      <c r="D221" s="19" t="s">
+      <c r="E221" s="38" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F221" s="62" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G221" s="19" t="s">
         <v>1070</v>
-      </c>
-      <c r="E221" s="38" t="s">
-        <v>1073</v>
-      </c>
-      <c r="F221" s="62" t="s">
-        <v>1074</v>
-      </c>
-      <c r="G221" s="19" t="s">
-        <v>1071</v>
       </c>
       <c r="H221" s="19"/>
     </row>
@@ -14146,22 +14349,22 @@
     </row>
     <row r="223" spans="1:8" ht="96" customHeight="1">
       <c r="A223" s="13" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B223" s="35" t="s">
         <v>1076</v>
       </c>
-      <c r="B223" s="35" t="s">
+      <c r="C223" s="19" t="s">
         <v>1077</v>
       </c>
-      <c r="C223" s="19" t="s">
+      <c r="D223" s="19" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E223" s="39" t="s">
         <v>1078</v>
       </c>
-      <c r="D223" s="19" t="s">
+      <c r="F223" s="19" t="s">
         <v>1080</v>
-      </c>
-      <c r="E223" s="39" t="s">
-        <v>1079</v>
-      </c>
-      <c r="F223" s="19" t="s">
-        <v>1081</v>
       </c>
       <c r="G223" s="68" t="s">
         <v>693</v>
@@ -14173,13 +14376,13 @@
         <v>864</v>
       </c>
       <c r="B224" s="18" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C224" s="19" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D224" s="19" t="s">
         <v>1082</v>
-      </c>
-      <c r="C224" s="19" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D224" s="19" t="s">
-        <v>1083</v>
       </c>
       <c r="E224" s="19"/>
       <c r="F224" s="36"/>
@@ -14190,16 +14393,16 @@
     </row>
     <row r="225" spans="1:8" ht="79" customHeight="1">
       <c r="A225" s="13" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B225" s="18" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C225" s="19" t="s">
         <v>1086</v>
       </c>
-      <c r="B225" s="18" t="s">
-        <v>1085</v>
-      </c>
-      <c r="C225" s="19" t="s">
+      <c r="D225" s="69" t="s">
         <v>1087</v>
-      </c>
-      <c r="D225" s="69" t="s">
-        <v>1088</v>
       </c>
       <c r="E225" s="39"/>
       <c r="F225" s="36"/>
@@ -14213,7 +14416,7 @@
         <v>872</v>
       </c>
       <c r="B226" s="18" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C226" s="36"/>
       <c r="D226" s="36"/>
@@ -14229,7 +14432,7 @@
         <v>871</v>
       </c>
       <c r="B227" s="18" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C227" s="36"/>
       <c r="D227" s="36"/>
@@ -14245,10 +14448,10 @@
         <v>858</v>
       </c>
       <c r="B228" s="18" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C228" s="19" t="s">
         <v>1090</v>
-      </c>
-      <c r="C228" s="19" t="s">
-        <v>1091</v>
       </c>
       <c r="D228" s="36"/>
       <c r="E228" s="36"/>
@@ -14279,7 +14482,7 @@
         <v>875</v>
       </c>
       <c r="B230" s="18" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C230" s="36"/>
       <c r="D230" s="36"/>
@@ -14295,7 +14498,7 @@
         <v>715</v>
       </c>
       <c r="B231" s="18" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C231" s="36"/>
       <c r="D231" s="36"/>
@@ -14308,44 +14511,44 @@
     </row>
     <row r="232" spans="1:8" ht="66" customHeight="1">
       <c r="A232" s="13" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B232" s="18" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C232" s="67" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D232" s="19" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="E232" s="36"/>
       <c r="F232" s="19" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="G232" s="52" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="H232" s="19"/>
     </row>
     <row r="233" spans="1:8" ht="68" customHeight="1">
       <c r="A233" s="13" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B233" s="18" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C233" s="67" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D233" s="19" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E233" s="19" t="s">
         <v>1101</v>
       </c>
-      <c r="D233" s="19" t="s">
-        <v>1100</v>
-      </c>
-      <c r="E233" s="19" t="s">
-        <v>1102</v>
-      </c>
       <c r="F233" s="19" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="G233" s="68" t="s">
         <v>719</v>
@@ -14354,41 +14557,41 @@
     </row>
     <row r="234" spans="1:8" ht="83" customHeight="1">
       <c r="A234" s="13" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="B234" s="18" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C234" s="67" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D234" s="19" t="s">
         <v>1188</v>
       </c>
-      <c r="C234" s="67" t="s">
-        <v>1187</v>
-      </c>
-      <c r="D234" s="19" t="s">
-        <v>1189</v>
-      </c>
       <c r="E234" s="19" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="F234" s="19"/>
       <c r="G234" s="52" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="H234" s="19"/>
     </row>
     <row r="235" spans="1:8" ht="68" customHeight="1">
       <c r="A235" s="13" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B235" s="18" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C235" s="19" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D235" s="19" t="s">
         <v>1108</v>
       </c>
-      <c r="B235" s="18" t="s">
-        <v>1111</v>
-      </c>
-      <c r="C235" s="19" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D235" s="19" t="s">
+      <c r="E235" s="19" t="s">
         <v>1109</v>
-      </c>
-      <c r="E235" s="19" t="s">
-        <v>1110</v>
       </c>
       <c r="F235" s="36"/>
       <c r="G235" s="55" t="s">
@@ -14401,7 +14604,7 @@
         <v>865</v>
       </c>
       <c r="B236" s="18" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C236" s="36"/>
       <c r="D236" s="36"/>
@@ -14417,10 +14620,10 @@
         <v>874</v>
       </c>
       <c r="B237" s="18" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C237" s="19" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="D237" s="36"/>
       <c r="E237" s="36"/>
@@ -14432,21 +14635,21 @@
     </row>
     <row r="238" spans="1:8" ht="74" customHeight="1">
       <c r="A238" s="13" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B238" s="18" t="s">
         <v>1116</v>
       </c>
-      <c r="B238" s="18" t="s">
+      <c r="C238" s="19" t="s">
         <v>1117</v>
       </c>
-      <c r="C238" s="19" t="s">
-        <v>1118</v>
-      </c>
       <c r="D238" s="19" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="E238" s="36"/>
       <c r="F238" s="36"/>
       <c r="G238" s="52" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="H238" s="36"/>
     </row>
@@ -14525,10 +14728,10 @@
         <v>868</v>
       </c>
       <c r="B244" s="18" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C244" s="19" t="s">
         <v>1106</v>
-      </c>
-      <c r="C244" s="19" t="s">
-        <v>1107</v>
       </c>
       <c r="D244" s="36"/>
       <c r="E244" s="36"/>
@@ -14574,7 +14777,7 @@
     </row>
     <row r="247" spans="1:8" ht="55" customHeight="1">
       <c r="A247" s="13" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B247" s="18" t="s">
         <v>728</v>
@@ -14594,7 +14797,7 @@
     </row>
     <row r="248" spans="1:8" ht="71" customHeight="1">
       <c r="A248" s="13" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B248" s="18" t="s">
         <v>877</v>
@@ -14612,7 +14815,7 @@
     </row>
     <row r="249" spans="1:8" ht="43" customHeight="1">
       <c r="A249" s="13" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B249" s="35" t="s">
         <v>736</v>
@@ -14652,7 +14855,7 @@
     </row>
     <row r="251" spans="1:8" ht="63" customHeight="1">
       <c r="A251" s="13" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B251" s="18" t="s">
         <v>744</v>
@@ -14670,7 +14873,7 @@
     </row>
     <row r="252" spans="1:8" ht="57" customHeight="1">
       <c r="A252" s="13" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B252" s="18" t="s">
         <v>745</v>
@@ -14712,7 +14915,7 @@
     </row>
     <row r="254" spans="1:8" ht="101" customHeight="1">
       <c r="A254" s="13" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B254" s="35" t="s">
         <v>755</v>
@@ -14732,7 +14935,7 @@
     </row>
     <row r="255" spans="1:8" s="4" customFormat="1" ht="72" customHeight="1">
       <c r="A255" s="13" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B255" s="18" t="s">
         <v>758</v>
@@ -14745,7 +14948,7 @@
       </c>
       <c r="E255" s="43"/>
       <c r="F255" s="43" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G255" s="20" t="s">
         <v>760</v>
@@ -14754,7 +14957,7 @@
     </row>
     <row r="256" spans="1:8" s="4" customFormat="1" ht="54" customHeight="1">
       <c r="A256" s="13" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B256" s="18" t="s">
         <v>765</v>
@@ -14858,7 +15061,7 @@
     </row>
     <row r="262" spans="1:8" s="3" customFormat="1" ht="64" customHeight="1">
       <c r="A262" s="13" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B262" s="11" t="s">
         <v>893</v>
@@ -14876,59 +15079,59 @@
     </row>
     <row r="263" spans="1:8" s="3" customFormat="1" ht="87" customHeight="1">
       <c r="A263" s="13" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B263" s="71" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C263" s="6" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="D263" s="49"/>
       <c r="E263" s="49"/>
       <c r="F263" s="49"/>
       <c r="G263" s="52" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="H263" s="49"/>
     </row>
     <row r="264" spans="1:8" ht="76" customHeight="1">
       <c r="A264" s="13" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B264" s="46" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C264" s="6" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="D264" s="1"/>
       <c r="E264" s="1"/>
       <c r="F264" s="1"/>
       <c r="G264" s="52" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="H264" s="1"/>
     </row>
     <row r="265" spans="1:8" ht="80" customHeight="1">
       <c r="A265" s="13" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B265" s="70" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C265" s="6" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D265" s="6" t="s">
         <v>1135</v>
-      </c>
-      <c r="D265" s="6" t="s">
-        <v>1136</v>
       </c>
       <c r="E265" s="1"/>
       <c r="F265" s="72" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="G265" s="52" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="H265" s="1"/>
     </row>
@@ -14937,59 +15140,59 @@
         <v>908</v>
       </c>
       <c r="B266" s="18" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C266" s="19" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D266" s="19" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E266" s="52" t="s">
+        <v>1256</v>
+      </c>
+      <c r="F266" s="52" t="s">
         <v>1252</v>
       </c>
-      <c r="C266" s="19" t="s">
-        <v>1256</v>
-      </c>
-      <c r="D266" s="19" t="s">
+      <c r="G266" s="52" t="s">
         <v>1254</v>
-      </c>
-      <c r="E266" s="52" t="s">
-        <v>1257</v>
-      </c>
-      <c r="F266" s="52" t="s">
-        <v>1253</v>
-      </c>
-      <c r="G266" s="52" t="s">
-        <v>1255</v>
       </c>
       <c r="H266" s="19"/>
     </row>
     <row r="267" spans="1:8" s="58" customFormat="1" ht="62" customHeight="1">
       <c r="A267" s="13" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B267" s="18" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="C267" s="6" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="D267" s="6" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E267" s="73" t="s">
         <v>1146</v>
-      </c>
-      <c r="E267" s="73" t="s">
-        <v>1147</v>
       </c>
       <c r="F267" s="6"/>
       <c r="G267" s="68" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="H267" s="54" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="268" spans="1:8" s="58" customFormat="1" ht="62" customHeight="1">
       <c r="A268" s="13" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B268" s="18" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="C268" s="6"/>
       <c r="D268" s="6" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="E268" s="49"/>
       <c r="F268" s="49"/>
@@ -14998,19 +15201,19 @@
     </row>
     <row r="269" spans="1:8" s="58" customFormat="1" ht="62" customHeight="1">
       <c r="A269" s="13" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B269" s="18" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C269" s="6" t="s">
         <v>1144</v>
-      </c>
-      <c r="C269" s="6" t="s">
-        <v>1145</v>
       </c>
       <c r="D269" s="49"/>
       <c r="E269" s="49"/>
       <c r="F269" s="49"/>
       <c r="G269" s="68" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="H269" s="49"/>
     </row>
@@ -15019,45 +15222,45 @@
         <v>946</v>
       </c>
       <c r="B270" s="70" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C270" s="6" t="s">
         <v>1152</v>
       </c>
-      <c r="C270" s="6" t="s">
-        <v>1153</v>
-      </c>
       <c r="D270" s="6" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="E270" s="1"/>
       <c r="F270" s="1"/>
       <c r="G270" s="68" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="H270" s="1"/>
     </row>
     <row r="271" spans="1:8" ht="55" customHeight="1">
       <c r="A271" s="14" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B271" s="70" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C271" s="6" t="s">
         <v>1162</v>
       </c>
-      <c r="B271" s="70" t="s">
-        <v>1161</v>
-      </c>
-      <c r="C271" s="6" t="s">
+      <c r="D271" s="6" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E271" s="52" t="s">
         <v>1163</v>
       </c>
-      <c r="D271" s="6" t="s">
-        <v>1170</v>
-      </c>
-      <c r="E271" s="52" t="s">
+      <c r="F271" s="6" t="s">
         <v>1164</v>
       </c>
-      <c r="F271" s="6" t="s">
-        <v>1165</v>
-      </c>
       <c r="G271" s="68" t="s">
+        <v>1158</v>
+      </c>
+      <c r="H271" s="52" t="s">
         <v>1159</v>
-      </c>
-      <c r="H271" s="52" t="s">
-        <v>1160</v>
       </c>
     </row>
     <row r="272" spans="1:8" ht="35" customHeight="1">
@@ -15080,52 +15283,52 @@
     </row>
     <row r="273" spans="1:8" ht="80" customHeight="1">
       <c r="A273" s="14" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B273" s="70" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C273" s="6" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D273" s="6" t="s">
         <v>1182</v>
       </c>
-      <c r="D273" s="6" t="s">
-        <v>1183</v>
-      </c>
       <c r="E273" s="6" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="F273" s="1"/>
       <c r="G273" s="55" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="H273" s="1"/>
     </row>
     <row r="274" spans="1:8" ht="51" customHeight="1">
       <c r="A274" s="14" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B274" s="70" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C274" s="6" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="D274" s="6" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="E274" s="1"/>
       <c r="F274" s="1"/>
       <c r="G274" s="49" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="H274" s="1"/>
     </row>
     <row r="275" spans="1:8" ht="87" customHeight="1">
       <c r="A275" s="32" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B275" s="18" t="s">
         <v>1155</v>
-      </c>
-      <c r="B275" s="18" t="s">
-        <v>1156</v>
       </c>
       <c r="C275" s="19" t="s">
         <v>905</v>
@@ -15144,7 +15347,7 @@
     </row>
     <row r="276" spans="1:8" ht="37" customHeight="1">
       <c r="A276" s="13" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B276" s="18"/>
       <c r="C276" s="19"/>
@@ -15176,7 +15379,7 @@
     </row>
     <row r="278" spans="1:8" s="58" customFormat="1" ht="25" customHeight="1">
       <c r="A278" s="13" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B278" s="18"/>
       <c r="C278" s="6"/>
@@ -15184,13 +15387,13 @@
       <c r="E278" s="49"/>
       <c r="F278" s="49"/>
       <c r="G278" s="68" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="H278" s="49"/>
     </row>
     <row r="279" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A279" s="13" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B279" s="18"/>
       <c r="C279" s="6"/>
@@ -15198,7 +15401,7 @@
       <c r="E279" s="49"/>
       <c r="F279" s="49"/>
       <c r="G279" s="68" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="H279" s="49"/>
     </row>
@@ -15221,14 +15424,14 @@
         <v>944</v>
       </c>
       <c r="B281" s="70" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="C281" s="5"/>
       <c r="D281" s="1"/>
       <c r="E281" s="1"/>
       <c r="F281" s="1"/>
       <c r="G281" s="6" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="H281" s="1"/>
     </row>
@@ -15297,18 +15500,18 @@
         <v>952</v>
       </c>
       <c r="B287" s="77" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C287" s="6" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="D287" s="6" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="E287" s="49"/>
       <c r="F287" s="49"/>
       <c r="G287" s="68" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="H287" s="49"/>
     </row>
@@ -15372,7 +15575,7 @@
       <c r="E292" s="49"/>
       <c r="F292" s="49"/>
       <c r="G292" s="52" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="H292" s="49"/>
     </row>
@@ -15453,7 +15656,7 @@
         <v>668</v>
       </c>
       <c r="B299" s="18" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="C299" s="19"/>
       <c r="D299" s="19"/>
@@ -15490,23 +15693,23 @@
     </row>
     <row r="302" spans="1:8" s="58" customFormat="1" ht="66" customHeight="1">
       <c r="A302" s="13" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B302" s="70" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C302" s="6" t="s">
         <v>1214</v>
       </c>
-      <c r="B302" s="70" t="s">
+      <c r="D302" s="6" t="s">
         <v>1216</v>
-      </c>
-      <c r="C302" s="6" t="s">
-        <v>1215</v>
-      </c>
-      <c r="D302" s="6" t="s">
-        <v>1217</v>
       </c>
       <c r="E302" s="49"/>
       <c r="F302" s="78" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="G302" s="52" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="H302" s="49"/>
     </row>
@@ -15515,14 +15718,14 @@
         <v>968</v>
       </c>
       <c r="B303" s="63" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="C303" s="64"/>
       <c r="D303" s="49"/>
       <c r="E303" s="49"/>
       <c r="F303" s="49"/>
       <c r="G303" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="H303" s="49"/>
     </row>
@@ -15531,10 +15734,10 @@
         <v>969</v>
       </c>
       <c r="B304" s="63" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="C304" s="65" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D304" s="49"/>
       <c r="E304" s="49"/>
@@ -15547,40 +15750,40 @@
         <v>967</v>
       </c>
       <c r="B305" s="63" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C305" s="67" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="D305" s="49"/>
       <c r="E305" s="49"/>
       <c r="F305" s="49"/>
       <c r="G305" s="49" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="H305" s="49"/>
     </row>
     <row r="306" spans="1:8" s="58" customFormat="1" ht="74" customHeight="1">
       <c r="A306" s="66" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B306" s="18" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C306" s="67" t="s">
         <v>1051</v>
-      </c>
-      <c r="C306" s="67" t="s">
-        <v>1052</v>
       </c>
       <c r="D306" s="49"/>
       <c r="E306" s="49"/>
       <c r="F306" s="49"/>
       <c r="G306" s="55" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="H306" s="49"/>
     </row>
     <row r="307" spans="1:8" s="58" customFormat="1" ht="34" customHeight="1">
       <c r="A307" s="14" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B307" s="63"/>
       <c r="C307" s="49"/>
@@ -15592,43 +15795,43 @@
     </row>
     <row r="308" spans="1:8" s="58" customFormat="1" ht="93" customHeight="1">
       <c r="A308" s="14" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="B308" s="18" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="C308" s="67" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="D308" s="49"/>
       <c r="E308" s="49"/>
       <c r="F308" s="49"/>
       <c r="G308" s="52" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="H308" s="49"/>
     </row>
     <row r="309" spans="1:8" s="58" customFormat="1" ht="57" customHeight="1">
       <c r="A309" s="14" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B309" s="18" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="C309" s="67" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="D309" s="49"/>
       <c r="E309" s="49"/>
       <c r="F309" s="49"/>
       <c r="G309" s="52" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="H309" s="49"/>
     </row>
     <row r="310" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
       <c r="A310" s="14" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B310" s="18"/>
       <c r="C310" s="67"/>
@@ -15640,7 +15843,7 @@
     </row>
     <row r="311" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
       <c r="A311" s="14" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B311" s="18"/>
       <c r="C311" s="67"/>
@@ -15652,30 +15855,30 @@
     </row>
     <row r="312" spans="1:8" s="58" customFormat="1" ht="37" customHeight="1">
       <c r="A312" s="66" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B312" s="18" t="s">
         <v>1342</v>
       </c>
-      <c r="B312" s="18" t="s">
+      <c r="C312" s="67" t="s">
         <v>1343</v>
       </c>
-      <c r="C312" s="67" t="s">
-        <v>1344</v>
-      </c>
       <c r="D312" s="49" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="E312" s="49"/>
       <c r="F312" s="49"/>
       <c r="G312" s="68" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="H312" s="49"/>
     </row>
     <row r="313" spans="1:8" s="58" customFormat="1" ht="39" customHeight="1">
       <c r="A313" s="42" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B313" s="18" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="C313" s="67"/>
       <c r="D313" s="49"/>
@@ -15686,71 +15889,89 @@
     </row>
     <row r="314" spans="1:8" s="58" customFormat="1" ht="58" customHeight="1">
       <c r="A314" s="14" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B314" s="18" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="C314" s="67" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D314" s="6" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="E314" s="6" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="F314" s="49"/>
       <c r="G314" s="68" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="H314" s="49"/>
     </row>
     <row r="315" spans="1:8" s="58" customFormat="1" ht="68" customHeight="1">
       <c r="A315" s="14" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B315" s="18" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="C315" s="67" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="D315" s="6" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="E315" s="49"/>
       <c r="F315" s="49"/>
-      <c r="G315" s="55"/>
+      <c r="G315" s="68" t="s">
+        <v>1350</v>
+      </c>
       <c r="H315" s="49"/>
     </row>
-    <row r="316" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
+    <row r="316" spans="1:8" s="58" customFormat="1" ht="49" customHeight="1">
       <c r="A316" s="14" t="s">
-        <v>1207</v>
-      </c>
-      <c r="B316" s="18"/>
-      <c r="C316" s="67"/>
-      <c r="D316" s="49"/>
+        <v>1206</v>
+      </c>
+      <c r="B316" s="18" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C316" s="67" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D316" s="49" t="s">
+        <v>1358</v>
+      </c>
       <c r="E316" s="49"/>
       <c r="F316" s="49"/>
-      <c r="G316" s="55"/>
+      <c r="G316" s="68" t="s">
+        <v>1355</v>
+      </c>
       <c r="H316" s="49"/>
     </row>
-    <row r="317" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
+    <row r="317" spans="1:8" s="58" customFormat="1" ht="54" customHeight="1">
       <c r="A317" s="14" t="s">
-        <v>1208</v>
-      </c>
-      <c r="B317" s="18"/>
-      <c r="C317" s="67"/>
-      <c r="D317" s="49"/>
+        <v>1207</v>
+      </c>
+      <c r="B317" s="18" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C317" s="67" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D317" s="6" t="s">
+        <v>1356</v>
+      </c>
       <c r="E317" s="49"/>
       <c r="F317" s="49"/>
-      <c r="G317" s="55"/>
+      <c r="G317" s="68" t="s">
+        <v>1357</v>
+      </c>
       <c r="H317" s="49"/>
     </row>
     <row r="318" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
       <c r="A318" s="14" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B318" s="18"/>
       <c r="C318" s="67"/>
@@ -15762,7 +15983,7 @@
     </row>
     <row r="319" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
       <c r="A319" s="14" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B319" s="18"/>
       <c r="C319" s="67"/>
@@ -15774,39 +15995,43 @@
     </row>
     <row r="320" spans="1:8" s="58" customFormat="1" ht="28" customHeight="1">
       <c r="A320" s="14" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B320" s="18" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C320" s="67" t="s">
         <v>1338</v>
-      </c>
-      <c r="B320" s="18" t="s">
-        <v>1340</v>
-      </c>
-      <c r="C320" s="67" t="s">
-        <v>1339</v>
       </c>
       <c r="D320" s="49"/>
       <c r="E320" s="49"/>
       <c r="F320" s="49"/>
       <c r="G320" s="68" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="H320" s="49"/>
     </row>
-    <row r="321" spans="1:8" s="58" customFormat="1" ht="43" customHeight="1">
+    <row r="321" spans="1:8" ht="56" customHeight="1">
       <c r="A321" s="14" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B321" s="63"/>
-      <c r="C321" s="49"/>
-      <c r="D321" s="49"/>
-      <c r="E321" s="49"/>
-      <c r="F321" s="49"/>
-      <c r="G321" s="49"/>
-      <c r="H321" s="49"/>
-    </row>
-    <row r="322" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
+        <v>1311</v>
+      </c>
+      <c r="B321" s="70" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C321" s="5"/>
+      <c r="D321" s="1"/>
+      <c r="E321" s="1"/>
+      <c r="F321" s="1"/>
+      <c r="G321" s="6" t="s">
+        <v>1313</v>
+      </c>
+      <c r="H321" s="1"/>
+    </row>
+    <row r="322" spans="1:8" s="58" customFormat="1" ht="43" customHeight="1">
       <c r="A322" s="14" t="s">
-        <v>970</v>
-      </c>
-      <c r="B322" s="57"/>
+        <v>1046</v>
+      </c>
+      <c r="B322" s="63"/>
       <c r="C322" s="49"/>
       <c r="D322" s="49"/>
       <c r="E322" s="49"/>
@@ -15816,7 +16041,7 @@
     </row>
     <row r="323" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A323" s="14" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B323" s="57"/>
       <c r="C323" s="49"/>
@@ -15828,7 +16053,7 @@
     </row>
     <row r="324" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A324" s="14" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B324" s="57"/>
       <c r="C324" s="49"/>
@@ -15840,7 +16065,7 @@
     </row>
     <row r="325" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A325" s="14" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B325" s="57"/>
       <c r="C325" s="49"/>
@@ -15852,7 +16077,7 @@
     </row>
     <row r="326" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A326" s="14" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B326" s="57"/>
       <c r="C326" s="49"/>
@@ -15864,7 +16089,7 @@
     </row>
     <row r="327" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A327" s="14" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B327" s="57"/>
       <c r="C327" s="49"/>
@@ -15874,35 +16099,35 @@
       <c r="G327" s="49"/>
       <c r="H327" s="49"/>
     </row>
-    <row r="328" spans="1:8" ht="28" customHeight="1">
-      <c r="A328" s="42" t="s">
+    <row r="328" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
+      <c r="A328" s="14" t="s">
+        <v>975</v>
+      </c>
+      <c r="B328" s="57"/>
+      <c r="C328" s="49"/>
+      <c r="D328" s="49"/>
+      <c r="E328" s="49"/>
+      <c r="F328" s="49"/>
+      <c r="G328" s="49"/>
+      <c r="H328" s="49"/>
+    </row>
+    <row r="329" spans="1:8" ht="28" customHeight="1">
+      <c r="A329" s="42" t="s">
         <v>721</v>
       </c>
-      <c r="B328" s="41"/>
-      <c r="C328" s="36"/>
-      <c r="D328" s="36"/>
-      <c r="E328" s="36"/>
-      <c r="F328" s="36"/>
-      <c r="G328" s="36" t="s">
+      <c r="B329" s="41"/>
+      <c r="C329" s="36"/>
+      <c r="D329" s="36"/>
+      <c r="E329" s="36"/>
+      <c r="F329" s="36"/>
+      <c r="G329" s="36" t="s">
         <v>722</v>
       </c>
-      <c r="H328" s="36"/>
-    </row>
-    <row r="329" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
-      <c r="A329" s="14" t="s">
-        <v>976</v>
-      </c>
-      <c r="B329" s="57"/>
-      <c r="C329" s="49"/>
-      <c r="D329" s="49"/>
-      <c r="E329" s="49"/>
-      <c r="F329" s="49"/>
-      <c r="G329" s="49"/>
-      <c r="H329" s="49"/>
+      <c r="H329" s="36"/>
     </row>
     <row r="330" spans="1:8" s="58" customFormat="1" ht="47" customHeight="1">
       <c r="A330" s="13" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B330" s="57"/>
       <c r="C330" s="49"/>
@@ -15914,7 +16139,7 @@
     </row>
     <row r="331" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A331" s="14" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B331" s="57"/>
       <c r="C331" s="49"/>
@@ -15926,7 +16151,7 @@
     </row>
     <row r="332" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A332" s="14" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B332" s="57"/>
       <c r="C332" s="49"/>
@@ -15938,49 +16163,49 @@
     </row>
     <row r="333" spans="1:8" s="58" customFormat="1" ht="81" customHeight="1">
       <c r="A333" s="79" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B333" s="70" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="C333" s="6" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D333" s="6" t="s">
         <v>1223</v>
-      </c>
-      <c r="D333" s="6" t="s">
-        <v>1224</v>
       </c>
       <c r="E333" s="49"/>
       <c r="F333" s="49"/>
       <c r="G333" s="68" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="H333" s="49"/>
     </row>
     <row r="334" spans="1:8" s="58" customFormat="1" ht="68" customHeight="1">
       <c r="A334" s="13" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B334" s="70" t="s">
         <v>1240</v>
       </c>
-      <c r="B334" s="70" t="s">
+      <c r="C334" s="78" t="s">
         <v>1241</v>
       </c>
-      <c r="C334" s="78" t="s">
+      <c r="D334" s="6" t="s">
         <v>1242</v>
       </c>
-      <c r="D334" s="6" t="s">
+      <c r="E334" s="6" t="s">
         <v>1243</v>
-      </c>
-      <c r="E334" s="6" t="s">
-        <v>1244</v>
       </c>
       <c r="F334" s="49"/>
       <c r="G334" s="52" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="H334" s="49"/>
     </row>
     <row r="335" spans="1:8" s="58" customFormat="1" ht="68" customHeight="1">
       <c r="A335" s="13" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B335" s="70"/>
       <c r="C335" s="78"/>
@@ -15992,95 +16217,95 @@
     </row>
     <row r="336" spans="1:8" s="58" customFormat="1" ht="69" customHeight="1">
       <c r="A336" s="79" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B336" s="70" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C336" s="6" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D336" s="6" t="s">
         <v>1249</v>
       </c>
-      <c r="C336" s="6" t="s">
-        <v>1248</v>
-      </c>
-      <c r="D336" s="6" t="s">
-        <v>1250</v>
-      </c>
       <c r="E336" s="6" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="F336" s="52" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="G336" s="52" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="H336" s="49"/>
     </row>
     <row r="337" spans="1:8" s="58" customFormat="1" ht="78" customHeight="1">
       <c r="A337" s="14" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B337" s="70" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C337" s="6" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D337" s="6" t="s">
         <v>1259</v>
       </c>
-      <c r="C337" s="6" t="s">
-        <v>1261</v>
-      </c>
-      <c r="D337" s="6" t="s">
-        <v>1260</v>
-      </c>
       <c r="E337" s="80" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="F337" s="49"/>
       <c r="G337" s="68" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="H337" s="49"/>
     </row>
     <row r="338" spans="1:8" s="58" customFormat="1" ht="42" customHeight="1">
       <c r="A338" s="14" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B338" s="57" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C338" s="49" t="s">
         <v>1262</v>
       </c>
-      <c r="C338" s="49" t="s">
-        <v>1263</v>
-      </c>
       <c r="D338" s="6" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="E338" s="49"/>
       <c r="F338" s="52" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="G338" s="52" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="H338" s="49"/>
     </row>
     <row r="339" spans="1:8" s="58" customFormat="1" ht="80" customHeight="1">
       <c r="A339" s="14" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B339" s="70" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C339" s="6" t="s">
         <v>1271</v>
       </c>
-      <c r="C339" s="6" t="s">
+      <c r="D339" s="6" t="s">
         <v>1272</v>
-      </c>
-      <c r="D339" s="6" t="s">
-        <v>1273</v>
       </c>
       <c r="E339" s="49"/>
       <c r="F339" s="49"/>
       <c r="G339" s="49" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="H339" s="49"/>
     </row>
     <row r="340" spans="1:8" s="58" customFormat="1" ht="23" customHeight="1">
       <c r="A340" s="14" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B340" s="57"/>
       <c r="C340" s="6"/>
@@ -16092,7 +16317,7 @@
     </row>
     <row r="341" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A341" s="14" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B341" s="57"/>
       <c r="C341" s="49"/>
@@ -16104,7 +16329,7 @@
     </row>
     <row r="342" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A342" s="14" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B342" s="57"/>
       <c r="C342" s="49"/>
@@ -16116,7 +16341,7 @@
     </row>
     <row r="343" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A343" s="14" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B343" s="57"/>
       <c r="C343" s="49"/>
@@ -16128,7 +16353,7 @@
     </row>
     <row r="344" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A344" s="14" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B344" s="57"/>
       <c r="C344" s="49"/>
@@ -16140,7 +16365,7 @@
     </row>
     <row r="345" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A345" s="14" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B345" s="57"/>
       <c r="C345" s="49"/>
@@ -16152,7 +16377,7 @@
     </row>
     <row r="346" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A346" s="14" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B346" s="57"/>
       <c r="C346" s="49"/>
@@ -16164,7 +16389,7 @@
     </row>
     <row r="347" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A347" s="14" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B347" s="57"/>
       <c r="C347" s="49"/>
@@ -16176,7 +16401,7 @@
     </row>
     <row r="348" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A348" s="14" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B348" s="57"/>
       <c r="C348" s="49"/>
@@ -16188,7 +16413,7 @@
     </row>
     <row r="349" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A349" s="14" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B349" s="57"/>
       <c r="C349" s="49"/>
@@ -16200,7 +16425,7 @@
     </row>
     <row r="350" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A350" s="14" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B350" s="57"/>
       <c r="C350" s="49"/>
@@ -16212,7 +16437,7 @@
     </row>
     <row r="351" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A351" s="14" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B351" s="57"/>
       <c r="C351" s="49"/>
@@ -16224,7 +16449,7 @@
     </row>
     <row r="352" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A352" s="14" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="B352" s="57"/>
       <c r="C352" s="49"/>
@@ -16236,7 +16461,7 @@
     </row>
     <row r="353" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A353" s="14" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B353" s="57"/>
       <c r="C353" s="49"/>
@@ -16248,7 +16473,7 @@
     </row>
     <row r="354" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A354" s="14" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B354" s="57"/>
       <c r="C354" s="49"/>
@@ -16260,7 +16485,7 @@
     </row>
     <row r="355" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A355" s="14" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B355" s="57"/>
       <c r="C355" s="49"/>
@@ -16272,7 +16497,7 @@
     </row>
     <row r="356" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A356" s="14" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B356" s="57"/>
       <c r="C356" s="49"/>
@@ -16284,27 +16509,27 @@
     </row>
     <row r="357" spans="1:8" s="58" customFormat="1" ht="91" customHeight="1">
       <c r="A357" s="13" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B357" s="70" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C357" s="6" t="s">
         <v>1283</v>
       </c>
-      <c r="C357" s="6" t="s">
+      <c r="D357" s="6" t="s">
         <v>1284</v>
-      </c>
-      <c r="D357" s="6" t="s">
-        <v>1285</v>
       </c>
       <c r="E357" s="49"/>
       <c r="F357" s="49"/>
       <c r="G357" s="49" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="H357" s="49"/>
     </row>
     <row r="358" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A358" s="74" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B358" s="57"/>
       <c r="C358" s="49"/>
@@ -16316,7 +16541,7 @@
     </row>
     <row r="359" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A359" s="74" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B359" s="57"/>
       <c r="C359" s="49"/>
@@ -16328,7 +16553,7 @@
     </row>
     <row r="360" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A360" s="14" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B360" s="57"/>
       <c r="C360" s="49"/>
@@ -16340,7 +16565,7 @@
     </row>
     <row r="361" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A361" s="14" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B361" s="57"/>
       <c r="C361" s="49"/>
@@ -16352,41 +16577,41 @@
     </row>
     <row r="362" spans="1:8" s="58" customFormat="1" ht="50" customHeight="1">
       <c r="A362" s="14" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B362" s="70" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="C362" s="49"/>
       <c r="D362" s="49"/>
       <c r="E362" s="49"/>
       <c r="F362" s="49"/>
       <c r="G362" s="68" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="H362" s="49"/>
     </row>
     <row r="363" spans="1:8" s="58" customFormat="1" ht="53" customHeight="1">
       <c r="A363" s="13" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B363" s="70" t="s">
         <v>1276</v>
       </c>
-      <c r="B363" s="70" t="s">
+      <c r="C363" s="6" t="s">
         <v>1277</v>
-      </c>
-      <c r="C363" s="6" t="s">
-        <v>1278</v>
       </c>
       <c r="D363" s="49"/>
       <c r="E363" s="49"/>
       <c r="F363" s="49"/>
       <c r="G363" s="52" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="H363" s="49"/>
     </row>
     <row r="364" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A364" s="14" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B364" s="57"/>
       <c r="C364" s="49"/>
@@ -16398,7 +16623,7 @@
     </row>
     <row r="365" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A365" s="14" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B365" s="57"/>
       <c r="C365" s="49"/>
@@ -16410,7 +16635,7 @@
     </row>
     <row r="366" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A366" s="14" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B366" s="57"/>
       <c r="C366" s="49"/>
@@ -16422,7 +16647,7 @@
     </row>
     <row r="367" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A367" s="14" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B367" s="57"/>
       <c r="C367" s="49"/>
@@ -16434,7 +16659,7 @@
     </row>
     <row r="368" spans="1:8" s="58" customFormat="1" ht="22" customHeight="1">
       <c r="A368" s="14" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B368" s="57"/>
       <c r="C368" s="49"/>
@@ -16446,7 +16671,7 @@
     </row>
     <row r="369" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A369" s="14" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B369" s="35"/>
       <c r="C369" s="37"/>
@@ -16458,7 +16683,7 @@
     </row>
     <row r="370" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A370" s="14" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B370" s="35"/>
       <c r="C370" s="37"/>
@@ -16470,7 +16695,7 @@
     </row>
     <row r="371" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A371" s="14" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B371" s="35"/>
       <c r="C371" s="37"/>
@@ -16482,7 +16707,7 @@
     </row>
     <row r="372" spans="1:8" s="59" customFormat="1" ht="22" customHeight="1">
       <c r="A372" s="14" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B372" s="35"/>
       <c r="C372" s="37"/>
@@ -16494,7 +16719,7 @@
     </row>
     <row r="373" spans="1:8">
       <c r="A373" s="56" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B373" s="8"/>
       <c r="C373" s="5"/>
@@ -16506,7 +16731,7 @@
     </row>
     <row r="374" spans="1:8">
       <c r="A374" s="56" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B374" s="8"/>
       <c r="C374" s="5"/>
@@ -16518,7 +16743,7 @@
     </row>
     <row r="375" spans="1:8">
       <c r="A375" s="56" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B375" s="8"/>
       <c r="C375" s="5"/>
@@ -16530,7 +16755,7 @@
     </row>
     <row r="376" spans="1:8">
       <c r="A376" s="75" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B376" s="8"/>
       <c r="C376" s="5"/>
@@ -16542,7 +16767,7 @@
     </row>
     <row r="377" spans="1:8">
       <c r="A377" s="56" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B377" s="8"/>
       <c r="C377" s="5"/>
@@ -16554,7 +16779,7 @@
     </row>
     <row r="378" spans="1:8">
       <c r="A378" s="56" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B378" s="8"/>
       <c r="C378" s="5"/>
@@ -16566,7 +16791,7 @@
     </row>
     <row r="379" spans="1:8">
       <c r="A379" s="56" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B379" s="8"/>
       <c r="C379" s="5"/>
@@ -16578,7 +16803,7 @@
     </row>
     <row r="380" spans="1:8">
       <c r="A380" s="56" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B380" s="8"/>
       <c r="C380" s="5"/>
@@ -16590,7 +16815,7 @@
     </row>
     <row r="381" spans="1:8">
       <c r="A381" s="56" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B381" s="8"/>
       <c r="C381" s="5"/>
@@ -16602,78 +16827,78 @@
     </row>
     <row r="382" spans="1:8" ht="51" customHeight="1">
       <c r="A382" s="13" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B382" s="70" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="C382" s="5"/>
       <c r="D382" s="1"/>
       <c r="E382" s="1"/>
       <c r="F382" s="52" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="G382" s="52" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="H382" s="6" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="383" spans="1:8" ht="75" customHeight="1">
       <c r="A383" s="13" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="B383" s="57" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C383" s="6" t="s">
         <v>1295</v>
       </c>
-      <c r="C383" s="6" t="s">
+      <c r="D383" s="80" t="s">
         <v>1296</v>
       </c>
-      <c r="D383" s="80" t="s">
+      <c r="E383" s="6" t="s">
         <v>1297</v>
       </c>
-      <c r="E383" s="6" t="s">
-        <v>1298</v>
-      </c>
       <c r="F383" s="6" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="G383" s="49" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="H383" s="1"/>
     </row>
     <row r="384" spans="1:8" ht="48" customHeight="1">
       <c r="A384" s="13" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B384" s="70" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C384" s="6" t="s">
         <v>1301</v>
-      </c>
-      <c r="B384" s="70" t="s">
-        <v>1303</v>
-      </c>
-      <c r="C384" s="6" t="s">
-        <v>1302</v>
       </c>
       <c r="D384" s="1"/>
       <c r="E384" s="1"/>
       <c r="F384" s="1"/>
       <c r="G384" s="6" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="H384" s="1"/>
     </row>
     <row r="385" spans="1:8" ht="77" customHeight="1">
       <c r="A385" s="81" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B385" s="70" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C385" s="6" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D385" s="6" t="s">
         <v>1304</v>
-      </c>
-      <c r="B385" s="70" t="s">
-        <v>1307</v>
-      </c>
-      <c r="C385" s="6" t="s">
-        <v>1308</v>
-      </c>
-      <c r="D385" s="6" t="s">
-        <v>1305</v>
       </c>
       <c r="E385" s="5"/>
       <c r="F385" s="5"/>
@@ -16682,71 +16907,73 @@
     </row>
     <row r="386" spans="1:8" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A386" s="13" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B386" s="70" t="s">
         <v>78</v>
       </c>
       <c r="C386" s="6" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="D386" s="72"/>
       <c r="E386" s="72"/>
       <c r="F386" s="72"/>
       <c r="G386" s="6" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="H386" s="72"/>
     </row>
     <row r="387" spans="1:8" ht="56" customHeight="1">
-      <c r="A387" s="14" t="s">
-        <v>1312</v>
+      <c r="A387" s="13" t="s">
+        <v>1316</v>
       </c>
       <c r="B387" s="70" t="s">
-        <v>1313</v>
-      </c>
-      <c r="C387" s="5"/>
+        <v>1317</v>
+      </c>
+      <c r="C387" s="52" t="s">
+        <v>1314</v>
+      </c>
       <c r="D387" s="1"/>
       <c r="E387" s="1"/>
       <c r="F387" s="1"/>
-      <c r="G387" s="6" t="s">
-        <v>1314</v>
+      <c r="G387" s="49" t="s">
+        <v>1315</v>
       </c>
       <c r="H387" s="1"/>
     </row>
-    <row r="388" spans="1:8" ht="56" customHeight="1">
+    <row r="388" spans="1:8" ht="89" customHeight="1">
       <c r="A388" s="13" t="s">
-        <v>1317</v>
+        <v>1325</v>
       </c>
       <c r="B388" s="70" t="s">
-        <v>1318</v>
-      </c>
-      <c r="C388" s="52" t="s">
-        <v>1315</v>
+        <v>1327</v>
+      </c>
+      <c r="C388" s="6" t="s">
+        <v>1328</v>
       </c>
       <c r="D388" s="1"/>
       <c r="E388" s="1"/>
       <c r="F388" s="1"/>
       <c r="G388" s="49" t="s">
-        <v>1316</v>
+        <v>1326</v>
       </c>
       <c r="H388" s="1"/>
     </row>
-    <row r="389" spans="1:8" ht="89" customHeight="1">
+    <row r="389" spans="1:8" ht="35" customHeight="1">
       <c r="A389" s="13" t="s">
-        <v>1326</v>
+        <v>1359</v>
       </c>
       <c r="B389" s="70" t="s">
-        <v>1328</v>
+        <v>1360</v>
       </c>
       <c r="C389" s="6" t="s">
-        <v>1329</v>
+        <v>1361</v>
       </c>
       <c r="D389" s="1"/>
       <c r="E389" s="1"/>
       <c r="F389" s="1"/>
       <c r="G389" s="49" t="s">
-        <v>1327</v>
+        <v>1362</v>
       </c>
       <c r="H389" s="1"/>
     </row>
@@ -17059,16 +17286,6 @@
       <c r="F420" s="1"/>
       <c r="G420" s="5"/>
       <c r="H420" s="1"/>
-    </row>
-    <row r="421" spans="1:8">
-      <c r="A421" s="56"/>
-      <c r="B421" s="8"/>
-      <c r="C421" s="5"/>
-      <c r="D421" s="1"/>
-      <c r="E421" s="1"/>
-      <c r="F421" s="1"/>
-      <c r="G421" s="5"/>
-      <c r="H421" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -17245,7 +17462,7 @@
     <hyperlink ref="G363" r:id="rId171" xr:uid="{C10B92B6-2829-1842-8167-60AE046440E2}"/>
     <hyperlink ref="G362" r:id="rId172" xr:uid="{96F5038D-CC80-EC41-BDFF-0324640F4236}"/>
     <hyperlink ref="G382" r:id="rId173" xr:uid="{06D587F7-8278-B347-9E59-5FE6B08A6D67}"/>
-    <hyperlink ref="C388" r:id="rId174" xr:uid="{A8124453-5202-9542-8010-B6B373121DD2}"/>
+    <hyperlink ref="C387" r:id="rId174" xr:uid="{A8124453-5202-9542-8010-B6B373121DD2}"/>
     <hyperlink ref="G309" r:id="rId175" xr:uid="{0E8AC46B-4D36-FD4F-9477-FE182A63B756}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>